<commit_message>
Anpassung eines Erros in der Vorhersage
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,75 +491,85 @@
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>A_Frühbucher_Nachfrage</t>
+          <t>A_Frühbucher_Nachfrage_Geschätzt</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>A_LastMinute_Nachfrage</t>
+          <t>A_LastMinute_Nachfrage_Geschätzt</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>A_Frühbucher_Nachfrage_Tatsächlich</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>A_LastMinute_Nachfrage_Tatsächlich</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>B_Frühbucher_Nachfrage</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>B_LastMinute_Nachfrage</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="R1" s="1" t="inlineStr">
         <is>
           <t>Verkaufte_Menge_B</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="S1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_A</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_B</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>Var_Kosten_A/Einheit</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>Fix_Kosten_A/Einheit</t>
-        </is>
-      </c>
       <c r="U1" s="1" t="inlineStr">
         <is>
-          <t>Var_Kosten_B/Einheit</t>
+          <t>Var_Kosten_A_Einheit</t>
         </is>
       </c>
       <c r="V1" s="1" t="inlineStr">
         <is>
-          <t>Fix_Kosten_B/Einheit</t>
+          <t>Fix_Kosten_A_Einheit</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Var_Kosten_B_Einheit</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Fix_Kosten_B_Einheit</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>25772.12109008056</v>
+        <v>23471.26401655808</v>
       </c>
       <c r="C2" t="n">
-        <v>38000</v>
+        <v>35406.15686931537</v>
       </c>
       <c r="D2" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E2" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F2" t="n">
         <v>105</v>
@@ -568,43 +578,43 @@
         <v>105</v>
       </c>
       <c r="H2" t="n">
-        <v>476.24803</v>
+        <v>540.68737</v>
       </c>
       <c r="I2" t="n">
         <v>201</v>
       </c>
       <c r="J2" t="n">
-        <v>550</v>
+        <v>512.9450981330766</v>
       </c>
       <c r="K2" t="n">
         <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>195.1134071920112</v>
+        <v>276.3164434010242</v>
       </c>
       <c r="M2" t="n">
-        <v>80.13462566599497</v>
+        <v>63.37092974021979</v>
       </c>
       <c r="N2" t="n">
-        <v>596.8950648177041</v>
+        <v>271.0098883321972</v>
       </c>
       <c r="O2" t="n">
-        <v>125.9463503452637</v>
+        <v>71.73646543176002</v>
       </c>
       <c r="P2" t="n">
-        <v>550</v>
+        <v>404.2992447175371</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.275774915167946</v>
+        <v>108.6458534155395</v>
       </c>
       <c r="R2" t="n">
-        <v>0.7242250848320539</v>
+        <v>512.9450981330766</v>
       </c>
       <c r="S2" t="n">
-        <v>35</v>
+        <v>0.4005489981278909</v>
       </c>
       <c r="T2" t="n">
-        <v>0.9090909090909091</v>
+        <v>0.5994510018721091</v>
       </c>
       <c r="U2" t="n">
         <v>35</v>
@@ -612,34 +622,40 @@
       <c r="V2" t="n">
         <v>0.9090909090909091</v>
       </c>
+      <c r="W2" t="n">
+        <v>35</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.9090909090909091</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>47177.8039314285</v>
+        <v>41257.47841285834</v>
       </c>
       <c r="C3" t="n">
-        <v>39339.41703797915</v>
+        <v>35040.7315396596</v>
       </c>
       <c r="D3" t="n">
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E3" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F3" t="n">
-        <v>110.25</v>
+        <v>99.75</v>
       </c>
       <c r="G3" t="n">
-        <v>110.25</v>
+        <v>99.75</v>
       </c>
       <c r="H3" t="n">
-        <v>385.8157</v>
+        <v>514.54252</v>
       </c>
       <c r="I3" t="n">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J3" t="n">
         <v>550</v>
@@ -648,48 +664,54 @@
         <v>0</v>
       </c>
       <c r="L3" t="n">
-        <v>261.0543398165291</v>
+        <v>392.4545575610027</v>
       </c>
       <c r="M3" t="n">
-        <v>123.7613631927229</v>
+        <v>125.0879660788822</v>
       </c>
       <c r="N3" t="n">
-        <v>657.5667803266747</v>
+        <v>419.2106912013869</v>
       </c>
       <c r="O3" t="n">
-        <v>188.3500564020373</v>
+        <v>94.28463709200997</v>
       </c>
       <c r="P3" t="n">
+        <v>422.3705558783609</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>149.9385981432077</v>
+      </c>
+      <c r="R3" t="n">
         <v>550</v>
       </c>
-      <c r="Q3" t="n">
-        <v>0.3126720799071286</v>
-      </c>
-      <c r="R3" t="n">
-        <v>0.6873279200928712</v>
-      </c>
       <c r="S3" t="n">
-        <v>34.25878283706489</v>
+        <v>0.472916935467618</v>
       </c>
       <c r="T3" t="n">
-        <v>0.9099999999999999</v>
+        <v>0.5270830645323821</v>
       </c>
       <c r="U3" t="n">
-        <v>37.81378720367428</v>
+        <v>33.24419508782885</v>
       </c>
       <c r="V3" t="n">
         <v>0.9099999999999999</v>
       </c>
+      <c r="W3" t="n">
+        <v>35.12957901880074</v>
+      </c>
+      <c r="X3" t="n">
+        <v>0.9099999999999999</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>48762.61644827357</v>
+        <v>36016.13368424537</v>
       </c>
       <c r="C4" t="n">
-        <v>26476.85825671007</v>
+        <v>38449.99869790149</v>
       </c>
       <c r="D4" t="n">
         <v>120</v>
@@ -698,84 +720,90 @@
         <v>160</v>
       </c>
       <c r="F4" t="n">
-        <v>115.7625</v>
+        <v>104.7375</v>
       </c>
       <c r="G4" t="n">
-        <v>115.7625</v>
+        <v>104.7375</v>
       </c>
       <c r="H4" t="n">
-        <v>520.35887</v>
+        <v>390.30485</v>
       </c>
       <c r="I4" t="n">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="J4" t="n">
-        <v>350.6332404820494</v>
+        <v>547.9905723108342</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
       </c>
       <c r="L4" t="n">
-        <v>409.8499248302218</v>
+        <v>309.3134917627625</v>
       </c>
       <c r="M4" t="n">
-        <v>114.5089435909447</v>
+        <v>76.99135331187259</v>
       </c>
       <c r="N4" t="n">
-        <v>275.2115625487534</v>
+        <v>329.5692621236929</v>
       </c>
       <c r="O4" t="n">
-        <v>75.42167793329607</v>
+        <v>34.67514564357283</v>
       </c>
       <c r="P4" t="n">
-        <v>350.6332404820494</v>
+        <v>495.3486824185978</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.5992726826741779</v>
+        <v>52.64188989223639</v>
       </c>
       <c r="R4" t="n">
-        <v>0.4007273173258222</v>
+        <v>547.9905723108342</v>
       </c>
       <c r="S4" t="n">
-        <v>34.29134398324795</v>
+        <v>0.3992879200226255</v>
       </c>
       <c r="T4" t="n">
-        <v>0.9109099999999998</v>
+        <v>0.6007120799773745</v>
       </c>
       <c r="U4" t="n">
-        <v>38.82210861092064</v>
+        <v>32.06493938567698</v>
       </c>
       <c r="V4" t="n">
         <v>0.9109099999999998</v>
       </c>
+      <c r="W4" t="n">
+        <v>33.65781146877562</v>
+      </c>
+      <c r="X4" t="n">
+        <v>0.9109099999999998</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>55649.91750573777</v>
+        <v>43101.15689658331</v>
       </c>
       <c r="C5" t="n">
-        <v>44163.56980690929</v>
+        <v>41840.32016475205</v>
       </c>
       <c r="D5" t="n">
         <v>140</v>
       </c>
       <c r="E5" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F5" t="n">
-        <v>121.550625</v>
+        <v>109.974375</v>
       </c>
       <c r="G5" t="n">
-        <v>121.550625</v>
+        <v>109.974375</v>
       </c>
       <c r="H5" t="n">
-        <v>501.61415</v>
+        <v>357.51269</v>
       </c>
       <c r="I5" t="n">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="J5" t="n">
         <v>550</v>
@@ -784,54 +812,60 @@
         <v>0</v>
       </c>
       <c r="L5" t="n">
-        <v>385.5675794279104</v>
+        <v>270.6952865229658</v>
       </c>
       <c r="M5" t="n">
-        <v>118.0465741785051</v>
+        <v>90.81740427164588</v>
       </c>
       <c r="N5" t="n">
-        <v>437.7698284449452</v>
+        <v>292.7177300325081</v>
       </c>
       <c r="O5" t="n">
-        <v>116.9769275002386</v>
+        <v>82.48798358795894</v>
       </c>
       <c r="P5" t="n">
+        <v>601.783434087286</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>147.4532428108741</v>
+      </c>
+      <c r="R5" t="n">
         <v>550</v>
       </c>
-      <c r="Q5" t="n">
-        <v>0.4758434944652142</v>
-      </c>
-      <c r="R5" t="n">
-        <v>0.5241565055347858</v>
-      </c>
       <c r="S5" t="n">
-        <v>32.54193284266505</v>
+        <v>0.3336815801184895</v>
       </c>
       <c r="T5" t="n">
-        <v>0.9118209099999997</v>
+        <v>0.6663184198815105</v>
       </c>
       <c r="U5" t="n">
-        <v>40.34140444107403</v>
+        <v>33.73911726171475</v>
       </c>
       <c r="V5" t="n">
         <v>0.9118209099999997</v>
       </c>
+      <c r="W5" t="n">
+        <v>32.98924469954176</v>
+      </c>
+      <c r="X5" t="n">
+        <v>0.9118209099999997</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>52865.81978503198</v>
+        <v>46617.93930746317</v>
       </c>
       <c r="C6" t="n">
-        <v>40584.82401653207</v>
+        <v>44391.10454247082</v>
       </c>
       <c r="D6" t="n">
+        <v>140</v>
+      </c>
+      <c r="E6" t="n">
         <v>120</v>
-      </c>
-      <c r="E6" t="n">
-        <v>200</v>
       </c>
       <c r="F6" t="n">
         <v>115.47309375</v>
@@ -840,10 +874,10 @@
         <v>115.47309375</v>
       </c>
       <c r="H6" t="n">
-        <v>524.76616</v>
+        <v>461.66965</v>
       </c>
       <c r="I6" t="n">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J6" t="n">
         <v>550</v>
@@ -852,54 +886,60 @@
         <v>0</v>
       </c>
       <c r="L6" t="n">
-        <v>425.9413387881494</v>
+        <v>352.2975066197536</v>
       </c>
       <c r="M6" t="n">
-        <v>99.82481717863361</v>
+        <v>110.3721402511483</v>
       </c>
       <c r="N6" t="n">
-        <v>585.9540414117304</v>
+        <v>281.9616781226598</v>
       </c>
       <c r="O6" t="n">
-        <v>71.80720839224188</v>
+        <v>157.9488936708956</v>
       </c>
       <c r="P6" t="n">
+        <v>501.6015827935475</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>164.1402063779627</v>
+      </c>
+      <c r="R6" t="n">
         <v>550</v>
       </c>
-      <c r="Q6" t="n">
-        <v>0.4442365706135764</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.5557634293864236</v>
-      </c>
       <c r="S6" t="n">
-        <v>33.0053700552493</v>
+        <v>0.3978742209798933</v>
       </c>
       <c r="T6" t="n">
-        <v>0.9127327309099995</v>
+        <v>0.6021257790201066</v>
       </c>
       <c r="U6" t="n">
-        <v>40.7697718981226</v>
+        <v>32.60419099986242</v>
       </c>
       <c r="V6" t="n">
         <v>0.9127327309099995</v>
       </c>
+      <c r="W6" t="n">
+        <v>33.84926185096127</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.9127327309099995</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>53679.63174011969</v>
+        <v>49356.75472915149</v>
       </c>
       <c r="C7" t="n">
-        <v>44735.40329398898</v>
+        <v>38509.4801339573</v>
       </c>
       <c r="D7" t="n">
         <v>140</v>
       </c>
       <c r="E7" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F7" t="n">
         <v>121.2467484375</v>
@@ -908,267 +948,291 @@
         <v>121.2467484375</v>
       </c>
       <c r="H7" t="n">
-        <v>491.30206</v>
+        <v>426.18336</v>
       </c>
       <c r="I7" t="n">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J7" t="n">
-        <v>550</v>
+        <v>444.4009129142731</v>
       </c>
       <c r="K7" t="n">
         <v>0</v>
       </c>
       <c r="L7" t="n">
-        <v>345.3722602743696</v>
+        <v>347.9936538005721</v>
       </c>
       <c r="M7" t="n">
-        <v>141.9297959838644</v>
+        <v>78.1897100241527</v>
       </c>
       <c r="N7" t="n">
-        <v>445.4435608769603</v>
+        <v>239.531322688979</v>
       </c>
       <c r="O7" t="n">
-        <v>180.1169915945932</v>
+        <v>46.49736086065403</v>
       </c>
       <c r="P7" t="n">
-        <v>550</v>
+        <v>368.4799274421143</v>
       </c>
       <c r="Q7" t="n">
-        <v>0.4378815969155767</v>
+        <v>75.92098547215878</v>
       </c>
       <c r="R7" t="n">
-        <v>0.5621184030844232</v>
+        <v>444.4009129142731</v>
       </c>
       <c r="S7" t="n">
-        <v>33.54503958462508</v>
+        <v>0.3915896685106009</v>
       </c>
       <c r="T7" t="n">
-        <v>0.9136454636409094</v>
+        <v>0.608410331489399</v>
       </c>
       <c r="U7" t="n">
-        <v>38.99600607569731</v>
+        <v>33.09325310766859</v>
       </c>
       <c r="V7" t="n">
         <v>0.9136454636409094</v>
       </c>
+      <c r="W7" t="n">
+        <v>33.46118363492415</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.9136454636409094</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>41697.35378362358</v>
+        <v>42310.36743168381</v>
       </c>
       <c r="C8" t="n">
-        <v>42683.80482942199</v>
+        <v>42497.58043498894</v>
       </c>
       <c r="D8" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="F8" t="n">
-        <v>127.309085859375</v>
+        <v>115.184411015625</v>
       </c>
       <c r="G8" t="n">
-        <v>127.309085859375</v>
+        <v>115.184411015625</v>
       </c>
       <c r="H8" t="n">
-        <v>434.47695</v>
+        <v>454.56743</v>
       </c>
       <c r="I8" t="n">
         <v>205</v>
       </c>
       <c r="J8" t="n">
-        <v>496.1676199241591</v>
+        <v>516.6906664963788</v>
       </c>
       <c r="K8" t="n">
         <v>0</v>
       </c>
       <c r="L8" t="n">
-        <v>296.5443773955216</v>
+        <v>396.9284044518008</v>
       </c>
       <c r="M8" t="n">
-        <v>131.9325731009216</v>
+        <v>49.63902471250258</v>
       </c>
       <c r="N8" t="n">
-        <v>462.4467784323514</v>
+        <v>401.0667607315838</v>
       </c>
       <c r="O8" t="n">
-        <v>33.72084149180769</v>
+        <v>36.89404720089886</v>
       </c>
       <c r="P8" t="n">
-        <v>496.1676199241591</v>
+        <v>453.4942995641816</v>
       </c>
       <c r="Q8" t="n">
-        <v>0.4633963840846841</v>
+        <v>63.19636693219712</v>
       </c>
       <c r="R8" t="n">
-        <v>0.5366036159153159</v>
+        <v>516.6906664963788</v>
       </c>
       <c r="S8" t="n">
-        <v>33.92069547959342</v>
+        <v>0.458765130169103</v>
       </c>
       <c r="T8" t="n">
-        <v>0.9145591091045502</v>
+        <v>0.5412348698308971</v>
       </c>
       <c r="U8" t="n">
-        <v>40.26831454497373</v>
+        <v>31.53732007377936</v>
       </c>
       <c r="V8" t="n">
         <v>0.9145591091045502</v>
       </c>
+      <c r="W8" t="n">
+        <v>31.96133242475637</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.9145591091045502</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>46273.95153137077</v>
+        <v>55021.86209571135</v>
       </c>
       <c r="C9" t="n">
-        <v>46651.09506454022</v>
+        <v>49155.37670945867</v>
       </c>
       <c r="D9" t="n">
         <v>140</v>
       </c>
       <c r="E9" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="F9" t="n">
-        <v>133.6745401523438</v>
+        <v>120.9436315664063</v>
       </c>
       <c r="G9" t="n">
-        <v>133.6745401523438</v>
+        <v>120.9436315664063</v>
       </c>
       <c r="H9" t="n">
-        <v>442.78218</v>
+        <v>478.44603</v>
       </c>
       <c r="I9" t="n">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J9" t="n">
-        <v>503.295240264729</v>
+        <v>550</v>
       </c>
       <c r="K9" t="n">
         <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>339.1605753358522</v>
+        <v>359.4444627311539</v>
       </c>
       <c r="M9" t="n">
-        <v>110.6216088860033</v>
+        <v>128.0015678058211</v>
       </c>
       <c r="N9" t="n">
-        <v>385.7259233426732</v>
+        <v>331.4505845202464</v>
       </c>
       <c r="O9" t="n">
-        <v>117.5693169220558</v>
+        <v>50.62354076052143</v>
       </c>
       <c r="P9" t="n">
-        <v>503.295240264729</v>
+        <v>513.7058369252353</v>
       </c>
       <c r="Q9" t="n">
-        <v>0.4719261758446852</v>
+        <v>66.85016318333462</v>
       </c>
       <c r="R9" t="n">
-        <v>0.5280738241553149</v>
+        <v>550</v>
       </c>
       <c r="S9" t="n">
-        <v>30.67786414632006</v>
+        <v>0.3969064703083515</v>
       </c>
       <c r="T9" t="n">
-        <v>0.9154736682136546</v>
+        <v>0.6030935296916485</v>
       </c>
       <c r="U9" t="n">
-        <v>39.98280256059779</v>
+        <v>31.1113523463954</v>
       </c>
       <c r="V9" t="n">
         <v>0.9154736682136546</v>
       </c>
+      <c r="W9" t="n">
+        <v>30.65474569917685</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.9154736682136546</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>63149.48426447746</v>
+        <v>60868.44635839289</v>
       </c>
       <c r="C10" t="n">
-        <v>36409.75922306693</v>
+        <v>49131.81255536452</v>
       </c>
       <c r="D10" t="n">
         <v>140</v>
       </c>
       <c r="E10" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F10" t="n">
-        <v>140.3582671599609</v>
+        <v>126.9908131447266</v>
       </c>
       <c r="G10" t="n">
-        <v>140.3582671599609</v>
+        <v>126.9908131447266</v>
       </c>
       <c r="H10" t="n">
-        <v>521.83478</v>
+        <v>546.83277</v>
       </c>
       <c r="I10" t="n">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="J10" t="n">
-        <v>368.9112306741479</v>
+        <v>517.0052977465056</v>
       </c>
       <c r="K10" t="n">
         <v>0</v>
       </c>
       <c r="L10" t="n">
-        <v>401.4005686462548</v>
+        <v>417.7837959822628</v>
       </c>
       <c r="M10" t="n">
-        <v>123.4342121901775</v>
+        <v>127.0489701890893</v>
       </c>
       <c r="N10" t="n">
-        <v>292.4116410322715</v>
+        <v>308.3818748213961</v>
       </c>
       <c r="O10" t="n">
-        <v>76.4995896418764</v>
+        <v>82.55306636349336</v>
       </c>
       <c r="P10" t="n">
-        <v>368.9112306741479</v>
+        <v>413.1002109638156</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.5872303474108642</v>
+        <v>103.9050867826899</v>
       </c>
       <c r="R10" t="n">
-        <v>0.4127696525891357</v>
+        <v>517.0052977465056</v>
       </c>
       <c r="S10" t="n">
-        <v>32.26964625853161</v>
+        <v>0.4305734280980898</v>
       </c>
       <c r="T10" t="n">
-        <v>0.9163891418818682</v>
+        <v>0.5694265719019103</v>
       </c>
       <c r="U10" t="n">
-        <v>40.29686977814153</v>
+        <v>31.17791620524712</v>
       </c>
       <c r="V10" t="n">
         <v>0.9163891418818682</v>
       </c>
+      <c r="W10" t="n">
+        <v>30.98439541603122</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.9163891418818682</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>52849.08196628255</v>
+        <v>51608.1706641993</v>
       </c>
       <c r="C11" t="n">
-        <v>48563.07470131683</v>
+        <v>54897.94569941166</v>
       </c>
       <c r="D11" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E11" t="n">
         <v>200</v>
@@ -1180,60 +1244,66 @@
         <v>133.3403538019629</v>
       </c>
       <c r="H11" t="n">
-        <v>532.2457000000001</v>
+        <v>416.17603</v>
       </c>
       <c r="I11" t="n">
         <v>195</v>
       </c>
       <c r="J11" t="n">
-        <v>550</v>
+        <v>534.5074777812131</v>
       </c>
       <c r="K11" t="n">
         <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>441.9791788355208</v>
+        <v>316.9385031047915</v>
       </c>
       <c r="M11" t="n">
-        <v>90.26652301319515</v>
+        <v>102.2375276173189</v>
       </c>
       <c r="N11" t="n">
-        <v>432.2879722487801</v>
+        <v>376.7363457469071</v>
       </c>
       <c r="O11" t="n">
-        <v>146.0744778018056</v>
+        <v>66.00945978205108</v>
       </c>
       <c r="P11" t="n">
-        <v>550</v>
+        <v>436.0379127995345</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.4792380651434067</v>
+        <v>98.46956498167864</v>
       </c>
       <c r="R11" t="n">
-        <v>0.5207619348565934</v>
+        <v>534.5074777812131</v>
       </c>
       <c r="S11" t="n">
-        <v>32.59247759926652</v>
+        <v>0.4530512335853004</v>
       </c>
       <c r="T11" t="n">
-        <v>0.9173055310237499</v>
+        <v>0.5469487664146995</v>
       </c>
       <c r="U11" t="n">
-        <v>44.12654881399946</v>
+        <v>29.59374486769991</v>
       </c>
       <c r="V11" t="n">
         <v>0.9173055310237499</v>
       </c>
+      <c r="W11" t="n">
+        <v>29.68892506713</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.9173055310237499</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>49077.43725691797</v>
+        <v>54396.22972703744</v>
       </c>
       <c r="C12" t="n">
-        <v>33547.47782926211</v>
+        <v>56580.0013493665</v>
       </c>
       <c r="D12" t="n">
         <v>140</v>
@@ -1248,66 +1318,72 @@
         <v>140.0073714920611</v>
       </c>
       <c r="H12" t="n">
-        <v>480.9242</v>
+        <v>540.78316</v>
       </c>
       <c r="I12" t="n">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="J12" t="n">
-        <v>355.8705990502691</v>
+        <v>518.0195814924426</v>
       </c>
       <c r="K12" t="n">
         <v>0</v>
       </c>
       <c r="L12" t="n">
-        <v>376.9807155430238</v>
+        <v>357.3969356367538</v>
       </c>
       <c r="M12" t="n">
-        <v>103.9434839243798</v>
+        <v>181.3862216234869</v>
       </c>
       <c r="N12" t="n">
-        <v>308.5285892716266</v>
+        <v>410.5678750302009</v>
       </c>
       <c r="O12" t="n">
-        <v>47.34200977864254</v>
+        <v>125.4043495366455</v>
       </c>
       <c r="P12" t="n">
-        <v>355.8705990502691</v>
+        <v>410.503028334192</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.5747217840255812</v>
+        <v>107.5165531582507</v>
       </c>
       <c r="R12" t="n">
-        <v>0.4252782159744188</v>
+        <v>518.0195814924426</v>
       </c>
       <c r="S12" t="n">
-        <v>31.76812152502584</v>
+        <v>0.5085165003044596</v>
       </c>
       <c r="T12" t="n">
-        <v>0.9182228365547735</v>
+        <v>0.4914834996955403</v>
       </c>
       <c r="U12" t="n">
-        <v>44.3194993266027</v>
+        <v>30.52363038971367</v>
       </c>
       <c r="V12" t="n">
         <v>0.9182228365547735</v>
       </c>
+      <c r="W12" t="n">
+        <v>29.80878837092395</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.9182228365547735</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>47715.28028071964</v>
+        <v>59112.56133347522</v>
       </c>
       <c r="C13" t="n">
-        <v>32634.73181086302</v>
+        <v>53118.7059220802</v>
       </c>
       <c r="D13" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E13" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F13" t="n">
         <v>133.007002917458</v>
@@ -1316,60 +1392,66 @@
         <v>133.007002917458</v>
       </c>
       <c r="H13" t="n">
-        <v>516.28211</v>
+        <v>520.96186</v>
       </c>
       <c r="I13" t="n">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="J13" t="n">
-        <v>375.8397429208078</v>
+        <v>517.7177929667129</v>
       </c>
       <c r="K13" t="n">
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>381.9585519602342</v>
+        <v>474.9128290229036</v>
       </c>
       <c r="M13" t="n">
-        <v>124.3235558191957</v>
+        <v>46.04903450310047</v>
       </c>
       <c r="N13" t="n">
-        <v>291.9915037696224</v>
+        <v>340.4246160444152</v>
       </c>
       <c r="O13" t="n">
-        <v>83.84823915118537</v>
+        <v>80.74387490253893</v>
       </c>
       <c r="P13" t="n">
-        <v>375.8397429208078</v>
+        <v>396.978455257525</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.5739367042971872</v>
+        <v>120.7393377091878</v>
       </c>
       <c r="R13" t="n">
-        <v>0.4260632957028127</v>
+        <v>517.7177929667129</v>
       </c>
       <c r="S13" t="n">
-        <v>33.1136542827613</v>
+        <v>0.4485830692843327</v>
       </c>
       <c r="T13" t="n">
-        <v>0.9191410593913283</v>
+        <v>0.5514169307156673</v>
       </c>
       <c r="U13" t="n">
-        <v>44.83043293584442</v>
+        <v>30.10875699746264</v>
       </c>
       <c r="V13" t="n">
         <v>0.9191410593913283</v>
       </c>
+      <c r="W13" t="n">
+        <v>29.42888713074941</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.9191410593913283</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>59827.89166597795</v>
+        <v>58413.36016678347</v>
       </c>
       <c r="C14" t="n">
-        <v>50618.91103160613</v>
+        <v>60289.69405547007</v>
       </c>
       <c r="D14" t="n">
         <v>140</v>
@@ -1378,13 +1460,13 @@
         <v>200</v>
       </c>
       <c r="F14" t="n">
-        <v>139.6573530633309</v>
+        <v>139.657353063331</v>
       </c>
       <c r="G14" t="n">
-        <v>139.6573530633309</v>
+        <v>139.657353063331</v>
       </c>
       <c r="H14" t="n">
-        <v>499.82719</v>
+        <v>512.61964</v>
       </c>
       <c r="I14" t="n">
         <v>204</v>
@@ -1396,184 +1478,202 @@
         <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>386.0768327359721</v>
+        <v>442.6095890307263</v>
       </c>
       <c r="M14" t="n">
-        <v>114.7503621102284</v>
+        <v>63.01005498979498</v>
       </c>
       <c r="N14" t="n">
-        <v>382.7300531507968</v>
+        <v>422.7172844232662</v>
       </c>
       <c r="O14" t="n">
-        <v>171.1913671172319</v>
+        <v>87.76523956884772</v>
       </c>
       <c r="P14" t="n">
+        <v>425.836311808594</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>125.2084996879976</v>
+      </c>
+      <c r="R14" t="n">
         <v>550</v>
       </c>
-      <c r="Q14" t="n">
-        <v>0.4748308626998869</v>
-      </c>
-      <c r="R14" t="n">
-        <v>0.5251691373001129</v>
-      </c>
       <c r="S14" t="n">
-        <v>32.5290511483698</v>
+        <v>0.4808943744789184</v>
       </c>
       <c r="T14" t="n">
-        <v>0.9200602004507196</v>
+        <v>0.5191056255210817</v>
       </c>
       <c r="U14" t="n">
-        <v>46.70290916905083</v>
+        <v>29.72956749224302</v>
       </c>
       <c r="V14" t="n">
         <v>0.9200602004507196</v>
       </c>
+      <c r="W14" t="n">
+        <v>29.11966730748012</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.9200602004507196</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>53555.35487970871</v>
+        <v>54427.28160795144</v>
       </c>
       <c r="C15" t="n">
-        <v>33753.29313192119</v>
+        <v>44177.57780474015</v>
       </c>
       <c r="D15" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="F15" t="n">
-        <v>146.6402207164974</v>
+        <v>132.6744854101644</v>
       </c>
       <c r="G15" t="n">
-        <v>146.6402207164974</v>
+        <v>132.6744854101644</v>
       </c>
       <c r="H15" t="n">
-        <v>519.24235</v>
+        <v>537.78541</v>
       </c>
       <c r="I15" t="n">
         <v>204</v>
       </c>
       <c r="J15" t="n">
-        <v>339.2318227604081</v>
+        <v>428.2557303419504</v>
       </c>
       <c r="K15" t="n">
         <v>0</v>
       </c>
       <c r="L15" t="n">
-        <v>407.3682908706897</v>
+        <v>458.187370609966</v>
       </c>
       <c r="M15" t="n">
-        <v>111.8740562314191</v>
+        <v>79.59803490700558</v>
       </c>
       <c r="N15" t="n">
-        <v>272.1072689520378</v>
+        <v>419.4447740891852</v>
       </c>
       <c r="O15" t="n">
-        <v>67.12455380837029</v>
+        <v>78.60529129114448</v>
       </c>
       <c r="P15" t="n">
-        <v>339.2318227604081</v>
+        <v>310.431714961374</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.6048432967823184</v>
+        <v>117.8240153805763</v>
       </c>
       <c r="R15" t="n">
-        <v>0.3951567032176815</v>
+        <v>428.2557303419504</v>
       </c>
       <c r="S15" t="n">
-        <v>30.78823105742433</v>
+        <v>0.5376734850201157</v>
       </c>
       <c r="T15" t="n">
-        <v>0.9209802606511701</v>
+        <v>0.4623265149798844</v>
       </c>
       <c r="U15" t="n">
-        <v>45.64783151049923</v>
+        <v>28.93397703609598</v>
       </c>
       <c r="V15" t="n">
         <v>0.9209802606511701</v>
       </c>
+      <c r="W15" t="n">
+        <v>28.33468612150278</v>
+      </c>
+      <c r="X15" t="n">
+        <v>0.9209802606511701</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>51887.24769209996</v>
+        <v>50758.08848537369</v>
       </c>
       <c r="C16" t="n">
-        <v>49443.62197447198</v>
+        <v>31801.33902204601</v>
       </c>
       <c r="D16" t="n">
         <v>140</v>
       </c>
       <c r="E16" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F16" t="n">
-        <v>139.3082096806725</v>
+        <v>139.3082096806726</v>
       </c>
       <c r="G16" t="n">
-        <v>139.3082096806725</v>
+        <v>139.3082096806726</v>
       </c>
       <c r="H16" t="n">
-        <v>445.74767</v>
+        <v>441.75155</v>
       </c>
       <c r="I16" t="n">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="J16" t="n">
-        <v>535.3442926479256</v>
+        <v>287.4744838290169</v>
       </c>
       <c r="K16" t="n">
         <v>0</v>
       </c>
       <c r="L16" t="n">
-        <v>389.3528590257251</v>
+        <v>370.0718241218638</v>
       </c>
       <c r="M16" t="n">
-        <v>59.39481060401015</v>
+        <v>80.67972451319993</v>
       </c>
       <c r="N16" t="n">
-        <v>403.9457559163288</v>
+        <v>208.5098303589337</v>
       </c>
       <c r="O16" t="n">
-        <v>131.3985367315968</v>
+        <v>66.04919910672835</v>
       </c>
       <c r="P16" t="n">
-        <v>535.3442926479256</v>
+        <v>211.6315905735236</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.4560017628750039</v>
+        <v>75.84289325549328</v>
       </c>
       <c r="R16" t="n">
-        <v>0.5439982371249961</v>
+        <v>287.4744838290169</v>
       </c>
       <c r="S16" t="n">
-        <v>30.49274269858121</v>
+        <v>0.4885100674089313</v>
       </c>
       <c r="T16" t="n">
-        <v>0.9219012409118212</v>
+        <v>0.5114899325910689</v>
       </c>
       <c r="U16" t="n">
-        <v>46.00252146663189</v>
+        <v>29.57245341028847</v>
       </c>
       <c r="V16" t="n">
         <v>0.9219012409118212</v>
       </c>
+      <c r="W16" t="n">
+        <v>26.92124484742579</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.9219012409118212</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>50722.91625493036</v>
+        <v>56612.68258688097</v>
       </c>
       <c r="C17" t="n">
-        <v>34749.73632533621</v>
+        <v>64132.69917101652</v>
       </c>
       <c r="D17" t="n">
         <v>140</v>
@@ -1582,412 +1682,448 @@
         <v>120</v>
       </c>
       <c r="F17" t="n">
-        <v>146.2736201647062</v>
+        <v>146.2736201647063</v>
       </c>
       <c r="G17" t="n">
-        <v>146.2736201647062</v>
+        <v>146.2736201647063</v>
       </c>
       <c r="H17" t="n">
-        <v>509.26284</v>
+        <v>549.65647</v>
       </c>
       <c r="I17" t="n">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="J17" t="n">
-        <v>358.959495467147</v>
+        <v>550</v>
       </c>
       <c r="K17" t="n">
         <v>0</v>
       </c>
       <c r="L17" t="n">
-        <v>367.7082013346006</v>
+        <v>438.4991865163782</v>
       </c>
       <c r="M17" t="n">
-        <v>137.5546377639953</v>
+        <v>106.1572865942763</v>
       </c>
       <c r="N17" t="n">
-        <v>284.714260690528</v>
+        <v>461.9854474442073</v>
       </c>
       <c r="O17" t="n">
-        <v>74.24523477661897</v>
+        <v>189.8533433217115</v>
       </c>
       <c r="P17" t="n">
-        <v>358.959495467147</v>
+        <v>405.0638785467998</v>
       </c>
       <c r="Q17" t="n">
-        <v>0.5846445051116179</v>
+        <v>155.8523176189119</v>
       </c>
       <c r="R17" t="n">
-        <v>0.4153554948883821</v>
+        <v>550</v>
       </c>
       <c r="S17" t="n">
-        <v>32.09587358741736</v>
+        <v>0.5374859702000685</v>
       </c>
       <c r="T17" t="n">
-        <v>0.922823142152733</v>
+        <v>0.4625140297999315</v>
       </c>
       <c r="U17" t="n">
-        <v>48.05281949292936</v>
+        <v>30.21619155786729</v>
       </c>
       <c r="V17" t="n">
         <v>0.922823142152733</v>
       </c>
+      <c r="W17" t="n">
+        <v>28.74588943888713</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.922823142152733</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>45114.67687402766</v>
+        <v>57066.80542678919</v>
       </c>
       <c r="C18" t="n">
-        <v>35129.39246061951</v>
+        <v>49979.61679037339</v>
       </c>
       <c r="D18" t="n">
         <v>140</v>
       </c>
       <c r="E18" t="n">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="F18" t="n">
-        <v>138.9599391564709</v>
+        <v>138.959939156471</v>
       </c>
       <c r="G18" t="n">
-        <v>138.9599391564709</v>
+        <v>138.959939156471</v>
       </c>
       <c r="H18" t="n">
-        <v>446.59257</v>
+        <v>511.38283</v>
       </c>
       <c r="I18" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J18" t="n">
-        <v>384.5492507554991</v>
+        <v>455.2907711794456</v>
       </c>
       <c r="K18" t="n">
         <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>348.0637303070332</v>
+        <v>413.6202235656147</v>
       </c>
       <c r="M18" t="n">
-        <v>99.52884196863896</v>
+        <v>94.76260836401693</v>
       </c>
       <c r="N18" t="n">
-        <v>298.1432997361724</v>
+        <v>350.6453230421221</v>
       </c>
       <c r="O18" t="n">
-        <v>86.40595101932668</v>
+        <v>84.014852904648</v>
       </c>
       <c r="P18" t="n">
-        <v>384.5492507554991</v>
+        <v>358.5776913560793</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.5378801544251979</v>
+        <v>96.7130798233663</v>
       </c>
       <c r="R18" t="n">
-        <v>0.462119845574802</v>
+        <v>455.2907711794456</v>
       </c>
       <c r="S18" t="n">
-        <v>32.78524343627451</v>
+        <v>0.4884091391220524</v>
       </c>
       <c r="T18" t="n">
-        <v>0.9237459652948856</v>
+        <v>0.5115908608779477</v>
       </c>
       <c r="U18" t="n">
-        <v>46.28662703450705</v>
+        <v>29.50428142010049</v>
       </c>
       <c r="V18" t="n">
         <v>0.9237459652948856</v>
       </c>
+      <c r="W18" t="n">
+        <v>28.0688772961666</v>
+      </c>
+      <c r="X18" t="n">
+        <v>0.9237459652948856</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>43220.79283610545</v>
+        <v>53687.68712844462</v>
       </c>
       <c r="C19" t="n">
-        <v>47162.20190060836</v>
+        <v>49008.57895627069</v>
       </c>
       <c r="D19" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E19" t="n">
         <v>160</v>
       </c>
       <c r="F19" t="n">
-        <v>132.0119421986473</v>
+        <v>145.9079361142945</v>
       </c>
       <c r="G19" t="n">
-        <v>132.0119421986473</v>
+        <v>145.9079361142945</v>
       </c>
       <c r="H19" t="n">
-        <v>470.54006</v>
+        <v>483.33191</v>
       </c>
       <c r="I19" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J19" t="n">
-        <v>550</v>
+        <v>423.2160911618784</v>
       </c>
       <c r="K19" t="n">
         <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>416.8101796705075</v>
+        <v>424.5903043947074</v>
       </c>
       <c r="M19" t="n">
-        <v>59.72987608733069</v>
+        <v>61.74160528792019</v>
       </c>
       <c r="N19" t="n">
-        <v>390.2724233636423</v>
+        <v>391.5977814820505</v>
       </c>
       <c r="O19" t="n">
-        <v>182.3647032153246</v>
+        <v>70.47858347503301</v>
       </c>
       <c r="P19" t="n">
-        <v>550</v>
+        <v>345.9355961625741</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.4542036023853024</v>
+        <v>77.28049499930434</v>
       </c>
       <c r="R19" t="n">
-        <v>0.5457963976146976</v>
+        <v>423.2160911618784</v>
       </c>
       <c r="S19" t="n">
-        <v>32.8317222493984</v>
+        <v>0.5219477041324654</v>
       </c>
       <c r="T19" t="n">
-        <v>0.9246697112601803</v>
+        <v>0.4780522958675346</v>
       </c>
       <c r="U19" t="n">
-        <v>45.33781448628105</v>
+        <v>30.46569797489379</v>
       </c>
       <c r="V19" t="n">
         <v>0.9246697112601803</v>
       </c>
+      <c r="W19" t="n">
+        <v>28.90589311181406</v>
+      </c>
+      <c r="X19" t="n">
+        <v>0.9246697112601803</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>55794.83269871862</v>
+        <v>55715.31689338661</v>
       </c>
       <c r="C20" t="n">
-        <v>35764.84451163365</v>
+        <v>59979.68332082509</v>
       </c>
       <c r="D20" t="n">
         <v>140</v>
       </c>
       <c r="E20" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F20" t="n">
-        <v>138.6125393085797</v>
+        <v>138.6125393085798</v>
       </c>
       <c r="G20" t="n">
-        <v>138.6125393085797</v>
+        <v>138.6125393085798</v>
       </c>
       <c r="H20" t="n">
-        <v>496.27488</v>
+        <v>486.11469</v>
       </c>
       <c r="I20" t="n">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="J20" t="n">
-        <v>387.4681315058095</v>
+        <v>550</v>
       </c>
       <c r="K20" t="n">
         <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>397.1453173096644</v>
+        <v>425.0059324572871</v>
       </c>
       <c r="M20" t="n">
-        <v>102.1295666700782</v>
+        <v>59.10876031991822</v>
       </c>
       <c r="N20" t="n">
-        <v>324.8349969334972</v>
+        <v>433.637609450222</v>
       </c>
       <c r="O20" t="n">
-        <v>62.63313457231234</v>
+        <v>88.76145007148283</v>
       </c>
       <c r="P20" t="n">
-        <v>387.4681315058095</v>
+        <v>446.7899364180898</v>
       </c>
       <c r="Q20" t="n">
-        <v>0.5630434920385087</v>
+        <v>127.5533564166422</v>
       </c>
       <c r="R20" t="n">
-        <v>0.4369565079614913</v>
+        <v>550</v>
       </c>
       <c r="S20" t="n">
-        <v>30.72322637469101</v>
+        <v>0.4763188531921736</v>
       </c>
       <c r="T20" t="n">
-        <v>0.9255943809714404</v>
+        <v>0.5236811468078264</v>
       </c>
       <c r="U20" t="n">
-        <v>44.99472026318531</v>
+        <v>30.22782299601548</v>
       </c>
       <c r="V20" t="n">
         <v>0.9255943809714404</v>
       </c>
+      <c r="W20" t="n">
+        <v>28.63297525338092</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.9255943809714404</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>54801.7074868314</v>
+        <v>52359.02186569505</v>
       </c>
       <c r="C21" t="n">
-        <v>38503.47287796492</v>
+        <v>44739.00749611144</v>
       </c>
       <c r="D21" t="n">
         <v>140</v>
       </c>
       <c r="E21" t="n">
+        <v>160</v>
+      </c>
+      <c r="F21" t="n">
+        <v>145.5431662740088</v>
+      </c>
+      <c r="G21" t="n">
+        <v>145.5431662740088</v>
+      </c>
+      <c r="H21" t="n">
+        <v>477.15635</v>
+      </c>
+      <c r="I21" t="n">
         <v>200</v>
       </c>
-      <c r="F21" t="n">
-        <v>145.5431662740087</v>
-      </c>
-      <c r="G21" t="n">
-        <v>145.5431662740087</v>
-      </c>
-      <c r="H21" t="n">
-        <v>484.78334</v>
-      </c>
-      <c r="I21" t="n">
-        <v>204</v>
-      </c>
       <c r="J21" t="n">
-        <v>383.9187883793818</v>
+        <v>396.9052017582044</v>
       </c>
       <c r="K21" t="n">
         <v>0</v>
       </c>
       <c r="L21" t="n">
-        <v>405.5409085121213</v>
+        <v>438.4456703860713</v>
       </c>
       <c r="M21" t="n">
-        <v>70.24242901728226</v>
+        <v>40.71068009149108</v>
       </c>
       <c r="N21" t="n">
-        <v>280.8768869865422</v>
+        <v>330.0118747595414</v>
       </c>
       <c r="O21" t="n">
-        <v>103.0419013928396</v>
+        <v>93.86171716602567</v>
       </c>
       <c r="P21" t="n">
-        <v>383.9187883793818</v>
+        <v>293.7274764052016</v>
       </c>
       <c r="Q21" t="n">
-        <v>0.5534281272440221</v>
+        <v>103.1777253530028</v>
       </c>
       <c r="R21" t="n">
-        <v>0.4465718727559779</v>
+        <v>396.9052017582044</v>
       </c>
       <c r="S21" t="n">
-        <v>31.15808295284697</v>
+        <v>0.5164285373689571</v>
       </c>
       <c r="T21" t="n">
-        <v>0.9265199753524118</v>
+        <v>0.4835714626310429</v>
       </c>
       <c r="U21" t="n">
-        <v>43.92516776684333</v>
+        <v>30.6555593707381</v>
       </c>
       <c r="V21" t="n">
         <v>0.9265199753524118</v>
       </c>
+      <c r="W21" t="n">
+        <v>31.53963776867862</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.9265199753524118</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>57112.5932396433</v>
+        <v>52775.78923094754</v>
       </c>
       <c r="C22" t="n">
-        <v>46975.36191033527</v>
+        <v>49831.4670217379</v>
       </c>
       <c r="D22" t="n">
         <v>140</v>
       </c>
       <c r="E22" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F22" t="n">
-        <v>138.2660079603082</v>
+        <v>138.2660079603083</v>
       </c>
       <c r="G22" t="n">
-        <v>138.2660079603082</v>
+        <v>138.2660079603083</v>
       </c>
       <c r="H22" t="n">
-        <v>503.83804</v>
+        <v>512.86643</v>
       </c>
       <c r="I22" t="n">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="J22" t="n">
-        <v>511.4072421696271</v>
+        <v>471.9225908222924</v>
       </c>
       <c r="K22" t="n">
         <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>444.4844476545041</v>
+        <v>356.1626382343459</v>
       </c>
       <c r="M22" t="n">
-        <v>58.35359028171051</v>
+        <v>157.7037906841103</v>
       </c>
       <c r="N22" t="n">
-        <v>386.4060802741128</v>
+        <v>352.405175922681</v>
       </c>
       <c r="O22" t="n">
-        <v>125.0011618955143</v>
+        <v>122.2121752727775</v>
       </c>
       <c r="P22" t="n">
-        <v>511.4072421696271</v>
+        <v>365.8304938351143</v>
       </c>
       <c r="Q22" t="n">
-        <v>0.4957755759866498</v>
+        <v>106.0920969871782</v>
       </c>
       <c r="R22" t="n">
-        <v>0.5042244240133502</v>
+        <v>471.9225908222924</v>
       </c>
       <c r="S22" t="n">
-        <v>31.4899841939269</v>
+        <v>0.5014234794822401</v>
       </c>
       <c r="T22" t="n">
-        <v>0.927446495327764</v>
+        <v>0.4985765205177599</v>
       </c>
       <c r="U22" t="n">
-        <v>45.41347563927544</v>
+        <v>29.44887508336984</v>
       </c>
       <c r="V22" t="n">
         <v>0.927446495327764</v>
       </c>
+      <c r="W22" t="n">
+        <v>31.5926603113825</v>
+      </c>
+      <c r="X22" t="n">
+        <v>0.927446495327764</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>55851.86731133786</v>
+        <v>55380.63813759504</v>
       </c>
       <c r="C23" t="n">
-        <v>37681.79487348394</v>
+        <v>44625.75640999018</v>
       </c>
       <c r="D23" t="n">
         <v>140</v>
       </c>
       <c r="E23" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F23" t="n">
         <v>145.1793083583237</v>
@@ -1996,128 +2132,140 @@
         <v>145.1793083583237</v>
       </c>
       <c r="H23" t="n">
-        <v>471.56289</v>
+        <v>484.80967</v>
       </c>
       <c r="I23" t="n">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="J23" t="n">
-        <v>378.4033601995516</v>
+        <v>403.2228927734443</v>
       </c>
       <c r="K23" t="n">
         <v>0</v>
       </c>
       <c r="L23" t="n">
-        <v>386.0183732699164</v>
+        <v>371.8153892539989</v>
       </c>
       <c r="M23" t="n">
-        <v>87.54451785531303</v>
+        <v>114.9942830170438</v>
       </c>
       <c r="N23" t="n">
-        <v>292.7553501303394</v>
+        <v>338.3002455399545</v>
       </c>
       <c r="O23" t="n">
-        <v>85.64801006921218</v>
+        <v>90.60745766696847</v>
       </c>
       <c r="P23" t="n">
-        <v>378.4033601995516</v>
+        <v>303.3733694382249</v>
       </c>
       <c r="Q23" t="n">
-        <v>0.5558470073067494</v>
+        <v>99.8495233352194</v>
       </c>
       <c r="R23" t="n">
-        <v>0.4441529926932506</v>
+        <v>403.2228927734443</v>
       </c>
       <c r="S23" t="n">
-        <v>31.34895294561951</v>
+        <v>0.5154331607067147</v>
       </c>
       <c r="T23" t="n">
-        <v>0.9283739418230917</v>
+        <v>0.4845668392932853</v>
       </c>
       <c r="U23" t="n">
-        <v>44.24891355066171</v>
+        <v>29.22383122574499</v>
       </c>
       <c r="V23" t="n">
         <v>0.9283739418230917</v>
       </c>
+      <c r="W23" t="n">
+        <v>33.24032154252979</v>
+      </c>
+      <c r="X23" t="n">
+        <v>0.9283739418230917</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>45972.07909366864</v>
+        <v>49318.00094702316</v>
       </c>
       <c r="C24" t="n">
-        <v>35504.29080584079</v>
+        <v>36319.85175718849</v>
       </c>
       <c r="D24" t="n">
         <v>140</v>
       </c>
       <c r="E24" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F24" t="n">
-        <v>137.9203429404075</v>
+        <v>137.9203429404076</v>
       </c>
       <c r="G24" t="n">
-        <v>137.9203429404075</v>
+        <v>137.9203429404076</v>
       </c>
       <c r="H24" t="n">
-        <v>415.12559</v>
+        <v>428.82503</v>
       </c>
       <c r="I24" t="n">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="J24" t="n">
-        <v>402.1459513098379</v>
+        <v>356.7176763936033</v>
       </c>
       <c r="K24" t="n">
         <v>0</v>
       </c>
       <c r="L24" t="n">
-        <v>353.1720530940439</v>
+        <v>360.7614213492092</v>
       </c>
       <c r="M24" t="n">
-        <v>60.95353472353397</v>
+        <v>62.06361332770209</v>
       </c>
       <c r="N24" t="n">
-        <v>311.6419901453093</v>
+        <v>283.4380373601511</v>
       </c>
       <c r="O24" t="n">
-        <v>90.50396116452853</v>
+        <v>41.73384827747133</v>
       </c>
       <c r="P24" t="n">
-        <v>402.1459513098379</v>
+        <v>296.4537102533232</v>
       </c>
       <c r="Q24" t="n">
-        <v>0.507338021683658</v>
+        <v>60.26396614028016</v>
       </c>
       <c r="R24" t="n">
-        <v>0.4926619783163418</v>
+        <v>356.7176763936033</v>
       </c>
       <c r="S24" t="n">
-        <v>29.64273443511933</v>
+        <v>0.4768688417358878</v>
       </c>
       <c r="T24" t="n">
-        <v>0.9293023157649147</v>
+        <v>0.5231311582641122</v>
       </c>
       <c r="U24" t="n">
-        <v>48.36229327658523</v>
+        <v>29.57897404854341</v>
       </c>
       <c r="V24" t="n">
         <v>0.9293023157649147</v>
       </c>
+      <c r="W24" t="n">
+        <v>34.67071314011755</v>
+      </c>
+      <c r="X24" t="n">
+        <v>0.9293023157649147</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>54681.09092238462</v>
+        <v>52142.84939819178</v>
       </c>
       <c r="C25" t="n">
-        <v>34255.51701002513</v>
+        <v>50521.48171851912</v>
       </c>
       <c r="D25" t="n">
         <v>120</v>
@@ -2126,134 +2274,146 @@
         <v>200</v>
       </c>
       <c r="F25" t="n">
-        <v>131.0243257933871</v>
+        <v>131.0243257933872</v>
       </c>
       <c r="G25" t="n">
-        <v>131.0243257933871</v>
+        <v>131.0243257933872</v>
       </c>
       <c r="H25" t="n">
-        <v>529.92362</v>
+        <v>515.65807</v>
       </c>
       <c r="I25" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J25" t="n">
-        <v>427.7150762050836</v>
+        <v>524.3198860199514</v>
       </c>
       <c r="K25" t="n">
         <v>0</v>
       </c>
       <c r="L25" t="n">
-        <v>452.5668588398378</v>
+        <v>443.3630629741593</v>
       </c>
       <c r="M25" t="n">
-        <v>82.35676374842123</v>
+        <v>75.29500491993052</v>
       </c>
       <c r="N25" t="n">
-        <v>338.7533819587925</v>
+        <v>498.7756600771572</v>
       </c>
       <c r="O25" t="n">
-        <v>88.96169424629107</v>
+        <v>93.00101373573538</v>
       </c>
       <c r="P25" t="n">
-        <v>427.7150762050836</v>
+        <v>383.236485044875</v>
       </c>
       <c r="Q25" t="n">
-        <v>0.555684727051572</v>
+        <v>141.0834009750764</v>
       </c>
       <c r="R25" t="n">
-        <v>0.444315272948428</v>
+        <v>524.3198860199514</v>
       </c>
       <c r="S25" t="n">
-        <v>28.66197490524348</v>
+        <v>0.5302199604499471</v>
       </c>
       <c r="T25" t="n">
-        <v>0.9302316180806796</v>
+        <v>0.4697800395500529</v>
       </c>
       <c r="U25" t="n">
-        <v>49.73856727292021</v>
+        <v>29.49258944546154</v>
       </c>
       <c r="V25" t="n">
         <v>0.9302316180806796</v>
       </c>
+      <c r="W25" t="n">
+        <v>33.69231442176128</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.9302316180806796</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>43191.96554050998</v>
+        <v>59676.88064092662</v>
       </c>
       <c r="C26" t="n">
-        <v>48385.91802936214</v>
+        <v>52467.4136609074</v>
       </c>
       <c r="D26" t="n">
         <v>140</v>
       </c>
       <c r="E26" t="n">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="F26" t="n">
-        <v>137.5755420830564</v>
+        <v>137.5755420830565</v>
       </c>
       <c r="G26" t="n">
-        <v>137.5755420830564</v>
+        <v>137.5755420830565</v>
       </c>
       <c r="H26" t="n">
-        <v>431.06774</v>
+        <v>491.99627</v>
       </c>
       <c r="I26" t="n">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J26" t="n">
-        <v>550</v>
+        <v>522.5827066253061</v>
       </c>
       <c r="K26" t="n">
         <v>0</v>
       </c>
       <c r="L26" t="n">
-        <v>378.3329210886134</v>
+        <v>402.2241221709222</v>
       </c>
       <c r="M26" t="n">
-        <v>50.7348218182229</v>
+        <v>90.77214481187868</v>
       </c>
       <c r="N26" t="n">
-        <v>454.7839262940262</v>
+        <v>380.2502868315967</v>
       </c>
       <c r="O26" t="n">
-        <v>110.4397283806792</v>
+        <v>84.19564835320196</v>
       </c>
       <c r="P26" t="n">
-        <v>550</v>
+        <v>400.7092615904712</v>
       </c>
       <c r="Q26" t="n">
-        <v>0.4315311828609565</v>
+        <v>121.8734450348349</v>
       </c>
       <c r="R26" t="n">
-        <v>0.5684688171390435</v>
+        <v>522.5827066253061</v>
       </c>
       <c r="S26" t="n">
-        <v>29.97044070154588</v>
+        <v>0.470549602626581</v>
       </c>
       <c r="T26" t="n">
-        <v>0.9311618496987601</v>
+        <v>0.529450397373419</v>
       </c>
       <c r="U26" t="n">
-        <v>48.6699838163356</v>
+        <v>28.20912932539898</v>
       </c>
       <c r="V26" t="n">
         <v>0.9311618496987601</v>
       </c>
+      <c r="W26" t="n">
+        <v>36.19531651001954</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.9311618496987601</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>51157.29431207268</v>
+        <v>56130.14491382247</v>
       </c>
       <c r="C27" t="n">
-        <v>28085.44017267059</v>
+        <v>25506.16137264417</v>
       </c>
       <c r="D27" t="n">
         <v>120</v>
@@ -2262,66 +2422,72 @@
         <v>200</v>
       </c>
       <c r="F27" t="n">
-        <v>130.6967649789036</v>
+        <v>130.6967649789037</v>
       </c>
       <c r="G27" t="n">
-        <v>130.6967649789036</v>
+        <v>130.6967649789037</v>
       </c>
       <c r="H27" t="n">
-        <v>516.3436799999999</v>
+        <v>531.82681</v>
       </c>
       <c r="I27" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="J27" t="n">
-        <v>349.4777586227689</v>
+        <v>273.7134418544128</v>
       </c>
       <c r="K27" t="n">
         <v>0</v>
       </c>
       <c r="L27" t="n">
-        <v>437.5117025152972</v>
+        <v>431.4303713603553</v>
       </c>
       <c r="M27" t="n">
-        <v>81.83198210925831</v>
+        <v>99.39644141660206</v>
       </c>
       <c r="N27" t="n">
-        <v>277.2477699888021</v>
+        <v>282.6807487751033</v>
       </c>
       <c r="O27" t="n">
-        <v>72.22998863396684</v>
+        <v>36.09017462767059</v>
       </c>
       <c r="P27" t="n">
-        <v>349.4777586227689</v>
+        <v>218.8330952632002</v>
       </c>
       <c r="Q27" t="n">
-        <v>0.5977565225409794</v>
+        <v>54.88034659121256</v>
       </c>
       <c r="R27" t="n">
-        <v>0.4022434774590207</v>
+        <v>273.7134418544128</v>
       </c>
       <c r="S27" t="n">
-        <v>32.54006179617226</v>
+        <v>0.5380241945530515</v>
       </c>
       <c r="T27" t="n">
-        <v>0.9320930115484587</v>
+        <v>0.4619758054469484</v>
       </c>
       <c r="U27" t="n">
-        <v>48.86583118293805</v>
+        <v>27.46784573795542</v>
       </c>
       <c r="V27" t="n">
         <v>0.9320930115484587</v>
       </c>
+      <c r="W27" t="n">
+        <v>35.63817979317817</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.9320930115484587</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>56625.19636365365</v>
+        <v>60030.13936905122</v>
       </c>
       <c r="C28" t="n">
-        <v>35968.69923914089</v>
+        <v>56025.91171311292</v>
       </c>
       <c r="D28" t="n">
         <v>140</v>
@@ -2330,72 +2496,78 @@
         <v>200</v>
       </c>
       <c r="F28" t="n">
-        <v>137.2316032278488</v>
+        <v>137.2316032278489</v>
       </c>
       <c r="G28" t="n">
-        <v>137.2316032278488</v>
+        <v>137.2316032278489</v>
       </c>
       <c r="H28" t="n">
-        <v>481.83172</v>
+        <v>481.55965</v>
       </c>
       <c r="I28" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="J28" t="n">
-        <v>423.4534530945882</v>
+        <v>550</v>
       </c>
       <c r="K28" t="n">
         <v>0</v>
       </c>
       <c r="L28" t="n">
-        <v>400.3204899384583</v>
+        <v>367.462375549989</v>
       </c>
       <c r="M28" t="n">
-        <v>80.51122531913356</v>
+        <v>113.0972722025417</v>
       </c>
       <c r="N28" t="n">
-        <v>326.303848413437</v>
+        <v>430.5240619961158</v>
       </c>
       <c r="O28" t="n">
-        <v>97.14960468115115</v>
+        <v>109.8178759064671</v>
       </c>
       <c r="P28" t="n">
-        <v>423.4534530945882</v>
+        <v>457.1074084198019</v>
       </c>
       <c r="Q28" t="n">
-        <v>0.5317257565263181</v>
+        <v>159.3463646560239</v>
       </c>
       <c r="R28" t="n">
-        <v>0.4682742434736819</v>
+        <v>550</v>
       </c>
       <c r="S28" t="n">
-        <v>30.32335331523883</v>
+        <v>0.4671023005830182</v>
       </c>
       <c r="T28" t="n">
-        <v>0.933025104560007</v>
+        <v>0.5328976994169817</v>
       </c>
       <c r="U28" t="n">
-        <v>51.07841973143318</v>
+        <v>27.24248977452239</v>
       </c>
       <c r="V28" t="n">
         <v>0.933025104560007</v>
       </c>
+      <c r="W28" t="n">
+        <v>34.43328409944718</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.933025104560007</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>60305.96066072677</v>
+        <v>56141.70882360678</v>
       </c>
       <c r="C29" t="n">
-        <v>38824.19028570787</v>
+        <v>52992.0074636495</v>
       </c>
       <c r="D29" t="n">
         <v>140</v>
       </c>
       <c r="E29" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F29" t="n">
         <v>144.0931833892413</v>
@@ -2404,66 +2576,72 @@
         <v>144.0931833892413</v>
       </c>
       <c r="H29" t="n">
-        <v>531.78799</v>
+        <v>448.79861</v>
       </c>
       <c r="I29" t="n">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J29" t="n">
-        <v>432.8915119916538</v>
+        <v>479.2803870258147</v>
       </c>
       <c r="K29" t="n">
         <v>0</v>
       </c>
       <c r="L29" t="n">
-        <v>369.7312582739909</v>
+        <v>331.7631359760433</v>
       </c>
       <c r="M29" t="n">
-        <v>157.056732138471</v>
+        <v>118.0354718727595</v>
       </c>
       <c r="N29" t="n">
-        <v>339.9183959423884</v>
+        <v>397.4326476150481</v>
       </c>
       <c r="O29" t="n">
-        <v>92.97311604926543</v>
+        <v>82.92239555753216</v>
       </c>
       <c r="P29" t="n">
-        <v>432.8915119916538</v>
+        <v>364.5188040207257</v>
       </c>
       <c r="Q29" t="n">
-        <v>0.5489207481172547</v>
+        <v>114.761583005089</v>
       </c>
       <c r="R29" t="n">
-        <v>0.4510792518827454</v>
+        <v>479.2803870258147</v>
       </c>
       <c r="S29" t="n">
-        <v>29.45500079547077</v>
+        <v>0.5005599293820068</v>
       </c>
       <c r="T29" t="n">
-        <v>0.9339581296645668</v>
+        <v>0.4994400706179932</v>
       </c>
       <c r="U29" t="n">
-        <v>53.22083739188704</v>
+        <v>28.96298546084103</v>
       </c>
       <c r="V29" t="n">
         <v>0.9339581296645668</v>
       </c>
+      <c r="W29" t="n">
+        <v>32.45564118352797</v>
+      </c>
+      <c r="X29" t="n">
+        <v>0.9339581296645668</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>50966.81314194256</v>
+        <v>54088.03812727136</v>
       </c>
       <c r="C30" t="n">
-        <v>27974.24476165893</v>
+        <v>57112.18093307033</v>
       </c>
       <c r="D30" t="n">
         <v>140</v>
       </c>
       <c r="E30" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F30" t="n">
         <v>136.8885242197792</v>
@@ -2472,116 +2650,128 @@
         <v>136.8885242197792</v>
       </c>
       <c r="H30" t="n">
-        <v>456.7827</v>
+        <v>445.97488</v>
       </c>
       <c r="I30" t="n">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J30" t="n">
-        <v>339.4728309308985</v>
+        <v>550</v>
       </c>
       <c r="K30" t="n">
         <v>0</v>
       </c>
       <c r="L30" t="n">
-        <v>386.700516898553</v>
+        <v>365.135696094813</v>
       </c>
       <c r="M30" t="n">
-        <v>73.08218104050339</v>
+        <v>80.83918389766922</v>
       </c>
       <c r="N30" t="n">
-        <v>253.545083774512</v>
+        <v>477.1074579405463</v>
       </c>
       <c r="O30" t="n">
-        <v>85.92774715638647</v>
+        <v>52.07947936405007</v>
       </c>
       <c r="P30" t="n">
-        <v>339.4728309308985</v>
+        <v>510.3850625778426</v>
       </c>
       <c r="Q30" t="n">
-        <v>0.5752637064508397</v>
+        <v>75.75040236961595</v>
       </c>
       <c r="R30" t="n">
-        <v>0.4247362935491603</v>
+        <v>550</v>
       </c>
       <c r="S30" t="n">
-        <v>30.53578329925493</v>
+        <v>0.4744699256789464</v>
       </c>
       <c r="T30" t="n">
-        <v>0.9348920877942314</v>
+        <v>0.5255300743210537</v>
       </c>
       <c r="U30" t="n">
-        <v>52.96889114686108</v>
+        <v>27.54550986649624</v>
       </c>
       <c r="V30" t="n">
         <v>0.9348920877942314</v>
       </c>
+      <c r="W30" t="n">
+        <v>32.11330316276623</v>
+      </c>
+      <c r="X30" t="n">
+        <v>0.9348920877942314</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>56316.78834044827</v>
+        <v>51614.32055060698</v>
       </c>
       <c r="C31" t="n">
-        <v>18785.48498174032</v>
+        <v>53715.64942791841</v>
       </c>
       <c r="D31" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E31" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F31" t="n">
-        <v>143.7329504307681</v>
+        <v>130.0440980087903</v>
       </c>
       <c r="G31" t="n">
-        <v>143.7329504307681</v>
+        <v>130.0440980087903</v>
       </c>
       <c r="H31" t="n">
-        <v>469.76452</v>
+        <v>534.45641</v>
       </c>
       <c r="I31" t="n">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="J31" t="n">
-        <v>222.1961594018204</v>
+        <v>550</v>
       </c>
       <c r="K31" t="n">
         <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>382.1679312163329</v>
+        <v>442.2518720539908</v>
       </c>
       <c r="M31" t="n">
-        <v>90.59659163333808</v>
+        <v>91.20454074521908</v>
       </c>
       <c r="N31" t="n">
-        <v>172.569568659441</v>
+        <v>502.0359931535815</v>
       </c>
       <c r="O31" t="n">
-        <v>49.62659074237939</v>
+        <v>126.7266974115259</v>
       </c>
       <c r="P31" t="n">
-        <v>222.1961594018204</v>
+        <v>394.5145326258906</v>
       </c>
       <c r="Q31" t="n">
-        <v>0.6802752082578791</v>
+        <v>155.8032192824016</v>
       </c>
       <c r="R31" t="n">
-        <v>0.3197247917421209</v>
+        <v>550</v>
       </c>
       <c r="S31" t="n">
-        <v>30.6437266006612</v>
+        <v>0.5332653039737723</v>
       </c>
       <c r="T31" t="n">
+        <v>0.4667346960262276</v>
+      </c>
+      <c r="U31" t="n">
+        <v>28.31274074563323</v>
+      </c>
+      <c r="V31" t="n">
         <v>0.9358269798820255</v>
       </c>
-      <c r="U31" t="n">
-        <v>56.87190894096946</v>
-      </c>
-      <c r="V31" t="n">
+      <c r="W31" t="n">
+        <v>31.44345388723841</v>
+      </c>
+      <c r="X31" t="n">
         <v>0.9358269798820255</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Einführen eines Erros in der Nachfrage
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X31"/>
+  <dimension ref="A1:Y31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,35 +521,40 @@
       </c>
       <c r="R1" s="1" t="inlineStr">
         <is>
+          <t>Verkaufte_Menge_A</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
           <t>Verkaufte_Menge_B</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_A</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_B</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Var_Kosten_A_Einheit</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Fix_Kosten_A_Einheit</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>Var_Kosten_B_Einheit</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>Fix_Kosten_B_Einheit</t>
         </is>
@@ -560,16 +565,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>23471.26401655808</v>
+        <v>18733.36417912387</v>
       </c>
       <c r="C2" t="n">
-        <v>35406.15686931537</v>
+        <v>19435.33097964252</v>
       </c>
       <c r="D2" t="n">
         <v>120</v>
       </c>
       <c r="E2" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F2" t="n">
         <v>105</v>
@@ -578,55 +583,58 @@
         <v>105</v>
       </c>
       <c r="H2" t="n">
-        <v>540.68737</v>
+        <v>460.46641</v>
       </c>
       <c r="I2" t="n">
-        <v>201</v>
+        <v>150.1771850071813</v>
       </c>
       <c r="J2" t="n">
-        <v>512.9450981330766</v>
+        <v>550</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
+        <v>33.31466374165871</v>
       </c>
       <c r="L2" t="n">
-        <v>276.3164434010242</v>
+        <v>344.879640681565</v>
       </c>
       <c r="M2" t="n">
-        <v>63.37092974021979</v>
+        <v>94.58676801844989</v>
       </c>
       <c r="N2" t="n">
         <v>271.0098883321972</v>
       </c>
       <c r="O2" t="n">
-        <v>71.73646543176002</v>
+        <v>60.27933666062149</v>
       </c>
       <c r="P2" t="n">
         <v>404.2992447175371</v>
       </c>
       <c r="Q2" t="n">
-        <v>108.6458534155395</v>
+        <v>112.3860915408043</v>
       </c>
       <c r="R2" t="n">
-        <v>512.9450981330766</v>
+        <v>331.2892249928187</v>
       </c>
       <c r="S2" t="n">
-        <v>0.4005489981278909</v>
+        <v>516.6853362583413</v>
       </c>
       <c r="T2" t="n">
-        <v>0.5994510018721091</v>
+        <v>0.3906829758006087</v>
       </c>
       <c r="U2" t="n">
-        <v>35</v>
+        <v>0.6093170241993914</v>
       </c>
       <c r="V2" t="n">
-        <v>0.9090909090909091</v>
+        <v>45</v>
       </c>
       <c r="W2" t="n">
-        <v>35</v>
+        <v>18.18181818181818</v>
       </c>
       <c r="X2" t="n">
-        <v>0.9090909090909091</v>
+        <v>45</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>18.18181818181818</v>
       </c>
     </row>
     <row r="3">
@@ -634,73 +642,76 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>41257.47841285834</v>
+        <v>20501.78587001723</v>
       </c>
       <c r="C3" t="n">
-        <v>35040.7315396596</v>
+        <v>15083.99566808814</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>140</v>
       </c>
       <c r="E3" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F3" t="n">
-        <v>99.75</v>
+        <v>110.25</v>
       </c>
       <c r="G3" t="n">
-        <v>99.75</v>
+        <v>110.25</v>
       </c>
       <c r="H3" t="n">
-        <v>514.54252</v>
+        <v>265.82661</v>
       </c>
       <c r="I3" t="n">
-        <v>198</v>
+        <v>49.84414024786673</v>
       </c>
       <c r="J3" t="n">
         <v>550</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>119.6787814358214</v>
       </c>
       <c r="L3" t="n">
-        <v>392.4545575610027</v>
+        <v>268.2830090240139</v>
       </c>
       <c r="M3" t="n">
-        <v>125.0879660788822</v>
+        <v>128.7207834765261</v>
       </c>
       <c r="N3" t="n">
-        <v>419.2106912013869</v>
+        <v>173.2043444305178</v>
       </c>
       <c r="O3" t="n">
-        <v>94.28463709200997</v>
+        <v>61.77812532161548</v>
       </c>
       <c r="P3" t="n">
-        <v>422.3705558783609</v>
+        <v>353.4559237991413</v>
       </c>
       <c r="Q3" t="n">
-        <v>149.9385981432077</v>
+        <v>110.179958506696</v>
       </c>
       <c r="R3" t="n">
-        <v>550</v>
+        <v>234.9824697521333</v>
       </c>
       <c r="S3" t="n">
-        <v>0.472916935467618</v>
+        <v>463.6358823058373</v>
       </c>
       <c r="T3" t="n">
-        <v>0.5270830645323821</v>
+        <v>0.3363531305181555</v>
       </c>
       <c r="U3" t="n">
-        <v>33.24419508782885</v>
+        <v>0.6636468694818445</v>
       </c>
       <c r="V3" t="n">
-        <v>0.9099999999999999</v>
+        <v>46.25598473676393</v>
       </c>
       <c r="W3" t="n">
-        <v>35.12957901880074</v>
+        <v>18.2</v>
       </c>
       <c r="X3" t="n">
-        <v>0.9099999999999999</v>
+        <v>46.87727780592505</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>18.2</v>
       </c>
     </row>
     <row r="4">
@@ -708,10 +719,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>36016.13368424537</v>
+        <v>10918.61253982624</v>
       </c>
       <c r="C4" t="n">
-        <v>38449.99869790149</v>
+        <v>5709.225355142524</v>
       </c>
       <c r="D4" t="n">
         <v>120</v>
@@ -720,61 +731,64 @@
         <v>160</v>
       </c>
       <c r="F4" t="n">
-        <v>104.7375</v>
+        <v>115.7625</v>
       </c>
       <c r="G4" t="n">
-        <v>104.7375</v>
+        <v>115.7625</v>
       </c>
       <c r="H4" t="n">
-        <v>390.30485</v>
+        <v>441.05599</v>
       </c>
       <c r="I4" t="n">
-        <v>202</v>
+        <v>189.8168698651084</v>
       </c>
       <c r="J4" t="n">
-        <v>547.9905723108342</v>
+        <v>405.4692759088001</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>212.4185598809564</v>
       </c>
       <c r="L4" t="n">
-        <v>309.3134917627625</v>
+        <v>348.8114478030581</v>
       </c>
       <c r="M4" t="n">
-        <v>76.99135331187259</v>
+        <v>125.0886848316272</v>
       </c>
       <c r="N4" t="n">
-        <v>329.5692621236929</v>
+        <v>215.496719001635</v>
       </c>
       <c r="O4" t="n">
-        <v>34.67514564357283</v>
+        <v>52.74240113325661</v>
       </c>
       <c r="P4" t="n">
-        <v>495.3486824185978</v>
+        <v>240.0356039751379</v>
       </c>
       <c r="Q4" t="n">
-        <v>52.64188989223639</v>
+        <v>72.69389348852722</v>
       </c>
       <c r="R4" t="n">
-        <v>547.9905723108342</v>
+        <v>268.2391201348916</v>
       </c>
       <c r="S4" t="n">
-        <v>0.3992879200226255</v>
+        <v>312.7294974636652</v>
       </c>
       <c r="T4" t="n">
-        <v>0.6007120799773745</v>
+        <v>0.4617101716159168</v>
       </c>
       <c r="U4" t="n">
-        <v>32.06493938567698</v>
+        <v>0.5382898283840831</v>
       </c>
       <c r="V4" t="n">
-        <v>0.9109099999999998</v>
+        <v>47.36461721476797</v>
       </c>
       <c r="W4" t="n">
-        <v>33.65781146877562</v>
+        <v>18.21819999999999</v>
       </c>
       <c r="X4" t="n">
-        <v>0.9109099999999998</v>
+        <v>49.44462420808044</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>18.21819999999999</v>
       </c>
     </row>
     <row r="5">
@@ -782,73 +796,76 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>43101.15689658331</v>
+        <v>27838.56629176844</v>
       </c>
       <c r="C5" t="n">
-        <v>41840.32016475205</v>
+        <v>30279.10687866205</v>
       </c>
       <c r="D5" t="n">
         <v>140</v>
       </c>
       <c r="E5" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F5" t="n">
-        <v>109.974375</v>
+        <v>121.550625</v>
       </c>
       <c r="G5" t="n">
-        <v>109.974375</v>
+        <v>121.550625</v>
       </c>
       <c r="H5" t="n">
-        <v>357.51269</v>
+        <v>273.65286</v>
       </c>
       <c r="I5" t="n">
-        <v>198</v>
+        <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>550</v>
+        <v>499.369591283113</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>169.2429028871031</v>
       </c>
       <c r="L5" t="n">
-        <v>270.6952865229658</v>
+        <v>365.0582114078035</v>
       </c>
       <c r="M5" t="n">
-        <v>90.81740427164588</v>
+        <v>81.41152253280774</v>
       </c>
       <c r="N5" t="n">
-        <v>292.7177300325081</v>
+        <v>273.6162274371555</v>
       </c>
       <c r="O5" t="n">
-        <v>82.48798358795894</v>
+        <v>94.94528244070065</v>
       </c>
       <c r="P5" t="n">
-        <v>601.783434087286</v>
+        <v>417.7809195015354</v>
       </c>
       <c r="Q5" t="n">
-        <v>147.4532428108741</v>
+        <v>124.7643287754309</v>
       </c>
       <c r="R5" t="n">
-        <v>550</v>
+        <v>290.65286</v>
       </c>
       <c r="S5" t="n">
-        <v>0.3336815801184895</v>
+        <v>542.5452482769663</v>
       </c>
       <c r="T5" t="n">
-        <v>0.6663184198815105</v>
+        <v>0.4045206630058025</v>
       </c>
       <c r="U5" t="n">
-        <v>33.73911726171475</v>
+        <v>0.5954793369941975</v>
       </c>
       <c r="V5" t="n">
-        <v>0.9118209099999997</v>
+        <v>46.96765861767919</v>
       </c>
       <c r="W5" t="n">
-        <v>32.98924469954176</v>
+        <v>18.23641819999999</v>
       </c>
       <c r="X5" t="n">
-        <v>0.9118209099999997</v>
+        <v>50.66205825509726</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>18.23641819999999</v>
       </c>
     </row>
     <row r="6">
@@ -856,16 +873,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>46617.93930746317</v>
+        <v>29967.87916114506</v>
       </c>
       <c r="C6" t="n">
-        <v>44391.10454247082</v>
+        <v>21926.7444354405</v>
       </c>
       <c r="D6" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E6" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="F6" t="n">
         <v>115.47309375</v>
@@ -874,55 +891,58 @@
         <v>115.47309375</v>
       </c>
       <c r="H6" t="n">
-        <v>461.66965</v>
+        <v>434.14251</v>
       </c>
       <c r="I6" t="n">
-        <v>197</v>
+        <v>28.90795948721927</v>
       </c>
       <c r="J6" t="n">
         <v>550</v>
       </c>
       <c r="K6" t="n">
-        <v>0</v>
+        <v>198.4929186755003</v>
       </c>
       <c r="L6" t="n">
-        <v>352.2975066197536</v>
+        <v>328.5659771748254</v>
       </c>
       <c r="M6" t="n">
-        <v>110.3721402511483</v>
+        <v>86.57653756514298</v>
       </c>
       <c r="N6" t="n">
-        <v>281.9616781226598</v>
+        <v>348.1335682624377</v>
       </c>
       <c r="O6" t="n">
-        <v>157.9488936708956</v>
+        <v>76.10098225034299</v>
       </c>
       <c r="P6" t="n">
-        <v>501.6015827935475</v>
+        <v>390.6978866068342</v>
       </c>
       <c r="Q6" t="n">
-        <v>164.1402063779627</v>
+        <v>130.0520976047686</v>
       </c>
       <c r="R6" t="n">
-        <v>550</v>
+        <v>424.2345505127807</v>
       </c>
       <c r="S6" t="n">
-        <v>0.3978742209798933</v>
+        <v>520.7499842116029</v>
       </c>
       <c r="T6" t="n">
-        <v>0.6021257790201066</v>
+        <v>0.4489327972298658</v>
       </c>
       <c r="U6" t="n">
-        <v>32.60419099986242</v>
+        <v>0.5510672027701342</v>
       </c>
       <c r="V6" t="n">
-        <v>0.9127327309099995</v>
+        <v>48.10045204146028</v>
       </c>
       <c r="W6" t="n">
-        <v>33.84926185096127</v>
+        <v>18.25465461819999</v>
       </c>
       <c r="X6" t="n">
-        <v>0.9127327309099995</v>
+        <v>50.48876624431989</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>18.25465461819999</v>
       </c>
     </row>
     <row r="7">
@@ -930,16 +950,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>49356.75472915149</v>
+        <v>28369.87792530596</v>
       </c>
       <c r="C7" t="n">
-        <v>38509.4801339573</v>
+        <v>25519.95566755506</v>
       </c>
       <c r="D7" t="n">
         <v>140</v>
       </c>
       <c r="E7" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F7" t="n">
         <v>121.2467484375</v>
@@ -948,55 +968,58 @@
         <v>121.2467484375</v>
       </c>
       <c r="H7" t="n">
-        <v>426.18336</v>
+        <v>436.68227</v>
       </c>
       <c r="I7" t="n">
-        <v>197</v>
+        <v>100.5242976136779</v>
       </c>
       <c r="J7" t="n">
-        <v>444.4009129142731</v>
+        <v>550</v>
       </c>
       <c r="K7" t="n">
-        <v>0</v>
+        <v>222.7531014509499</v>
       </c>
       <c r="L7" t="n">
-        <v>347.9936538005721</v>
+        <v>333.7567568280439</v>
       </c>
       <c r="M7" t="n">
-        <v>78.1897100241527</v>
+        <v>115.8334719975742</v>
       </c>
       <c r="N7" t="n">
-        <v>239.531322688979</v>
+        <v>279.782594778259</v>
       </c>
       <c r="O7" t="n">
-        <v>46.49736086065403</v>
+        <v>72.3753776080631</v>
       </c>
       <c r="P7" t="n">
-        <v>368.4799274421143</v>
+        <v>430.3999538186617</v>
       </c>
       <c r="Q7" t="n">
-        <v>75.92098547215878</v>
+        <v>95.33986340588866</v>
       </c>
       <c r="R7" t="n">
-        <v>444.4009129142731</v>
+        <v>352.1579723863221</v>
       </c>
       <c r="S7" t="n">
-        <v>0.3915896685106009</v>
+        <v>525.7398172245504</v>
       </c>
       <c r="T7" t="n">
-        <v>0.608410331489399</v>
+        <v>0.4011377822723712</v>
       </c>
       <c r="U7" t="n">
-        <v>33.09325310766859</v>
+        <v>0.5988622177276288</v>
       </c>
       <c r="V7" t="n">
-        <v>0.9136454636409094</v>
+        <v>47.47431035739504</v>
       </c>
       <c r="W7" t="n">
-        <v>33.46118363492415</v>
+        <v>18.27290927281819</v>
       </c>
       <c r="X7" t="n">
-        <v>0.9136454636409094</v>
+        <v>50.41578434926424</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>18.27290927281819</v>
       </c>
     </row>
     <row r="8">
@@ -1004,16 +1027,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>42310.36743168381</v>
+        <v>22019.22838426387</v>
       </c>
       <c r="C8" t="n">
-        <v>42497.58043498894</v>
+        <v>17509.73523690392</v>
       </c>
       <c r="D8" t="n">
         <v>120</v>
       </c>
       <c r="E8" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F8" t="n">
         <v>115.184411015625</v>
@@ -1022,55 +1045,58 @@
         <v>115.184411015625</v>
       </c>
       <c r="H8" t="n">
-        <v>454.56743</v>
+        <v>459.00749</v>
       </c>
       <c r="I8" t="n">
-        <v>205</v>
+        <v>119.8133477167801</v>
       </c>
       <c r="J8" t="n">
-        <v>516.6906664963788</v>
+        <v>432.5274601780798</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>233.4937099682066</v>
       </c>
       <c r="L8" t="n">
-        <v>396.9284044518008</v>
+        <v>418.6636074521576</v>
       </c>
       <c r="M8" t="n">
-        <v>49.63902471250258</v>
+        <v>116.8681814326885</v>
       </c>
       <c r="N8" t="n">
-        <v>401.0667607315838</v>
+        <v>319.482049352196</v>
       </c>
       <c r="O8" t="n">
-        <v>36.89404720089886</v>
+        <v>43.71209293102388</v>
       </c>
       <c r="P8" t="n">
-        <v>453.4942995641816</v>
+        <v>361.2448160251992</v>
       </c>
       <c r="Q8" t="n">
-        <v>63.19636693219712</v>
+        <v>60.54203563562387</v>
       </c>
       <c r="R8" t="n">
-        <v>516.6906664963788</v>
+        <v>363.1941422832199</v>
       </c>
       <c r="S8" t="n">
-        <v>0.458765130169103</v>
+        <v>421.786851660823</v>
       </c>
       <c r="T8" t="n">
-        <v>0.5412348698308971</v>
+        <v>0.4626788993430204</v>
       </c>
       <c r="U8" t="n">
-        <v>31.53732007377936</v>
+        <v>0.5373211006569797</v>
       </c>
       <c r="V8" t="n">
-        <v>0.9145591091045502</v>
+        <v>46.45772118944935</v>
       </c>
       <c r="W8" t="n">
-        <v>31.96133242475637</v>
+        <v>18.291182182091</v>
       </c>
       <c r="X8" t="n">
-        <v>0.9145591091045502</v>
+        <v>47.50310469822417</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>18.291182182091</v>
       </c>
     </row>
     <row r="9">
@@ -1078,16 +1104,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>55021.86209571135</v>
+        <v>41918.58162653436</v>
       </c>
       <c r="C9" t="n">
-        <v>49155.37670945867</v>
+        <v>40644.64042143602</v>
       </c>
       <c r="D9" t="n">
         <v>140</v>
       </c>
       <c r="E9" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="F9" t="n">
         <v>120.9436315664063</v>
@@ -1096,55 +1122,58 @@
         <v>120.9436315664063</v>
       </c>
       <c r="H9" t="n">
-        <v>478.44603</v>
+        <v>437.6083</v>
       </c>
       <c r="I9" t="n">
-        <v>196</v>
+        <v>8.042744050732722</v>
       </c>
       <c r="J9" t="n">
         <v>550</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
+        <v>139.0746300573609</v>
       </c>
       <c r="L9" t="n">
-        <v>359.4444627311539</v>
+        <v>388.2162802304384</v>
       </c>
       <c r="M9" t="n">
-        <v>128.0015678058211</v>
+        <v>150.2053633923694</v>
       </c>
       <c r="N9" t="n">
-        <v>331.4505845202464</v>
+        <v>357.4730139523981</v>
       </c>
       <c r="O9" t="n">
-        <v>50.62354076052143</v>
+        <v>91.09254199686919</v>
       </c>
       <c r="P9" t="n">
-        <v>513.7058369252353</v>
+        <v>554.0372604151671</v>
       </c>
       <c r="Q9" t="n">
-        <v>66.85016318333462</v>
+        <v>90.38181949567866</v>
       </c>
       <c r="R9" t="n">
-        <v>550</v>
+        <v>448.5655559492673</v>
       </c>
       <c r="S9" t="n">
-        <v>0.3969064703083515</v>
+        <v>644.4190799108458</v>
       </c>
       <c r="T9" t="n">
-        <v>0.6030935296916485</v>
+        <v>0.4104042648287304</v>
       </c>
       <c r="U9" t="n">
-        <v>31.1113523463954</v>
+        <v>0.5895957351712696</v>
       </c>
       <c r="V9" t="n">
-        <v>0.9154736682136546</v>
+        <v>47.67850773913931</v>
       </c>
       <c r="W9" t="n">
-        <v>30.65474569917685</v>
+        <v>18.30947336427309</v>
       </c>
       <c r="X9" t="n">
-        <v>0.9154736682136546</v>
+        <v>48.99160680581618</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>18.30947336427309</v>
       </c>
     </row>
     <row r="10">
@@ -1152,73 +1181,76 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>60868.44635839289</v>
+        <v>23117.72045439906</v>
       </c>
       <c r="C10" t="n">
-        <v>49131.81255536452</v>
+        <v>17437.7523986655</v>
       </c>
       <c r="D10" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E10" t="n">
         <v>160</v>
       </c>
       <c r="F10" t="n">
-        <v>126.9908131447266</v>
+        <v>114.8964499880859</v>
       </c>
       <c r="G10" t="n">
-        <v>126.9908131447266</v>
+        <v>114.8964499880859</v>
       </c>
       <c r="H10" t="n">
-        <v>546.83277</v>
+        <v>522.00622</v>
       </c>
       <c r="I10" t="n">
-        <v>198</v>
+        <v>146.5063169367691</v>
       </c>
       <c r="J10" t="n">
-        <v>517.0052977465056</v>
+        <v>526.9305193509706</v>
       </c>
       <c r="K10" t="n">
-        <v>0</v>
+        <v>204.0577753508649</v>
       </c>
       <c r="L10" t="n">
-        <v>417.7837959822628</v>
+        <v>399.5696940363122</v>
       </c>
       <c r="M10" t="n">
-        <v>127.0489701890893</v>
+        <v>110.4792722270115</v>
       </c>
       <c r="N10" t="n">
-        <v>308.3818748213961</v>
+        <v>349.8326979804371</v>
       </c>
       <c r="O10" t="n">
-        <v>82.55306636349336</v>
+        <v>45.66720508279375</v>
       </c>
       <c r="P10" t="n">
-        <v>413.1002109638156</v>
+        <v>398.5431928658645</v>
       </c>
       <c r="Q10" t="n">
-        <v>103.9050867826899</v>
+        <v>63.40418119160216</v>
       </c>
       <c r="R10" t="n">
-        <v>517.0052977465056</v>
+        <v>395.4999030632309</v>
       </c>
       <c r="S10" t="n">
-        <v>0.4305734280980898</v>
+        <v>461.9473740574666</v>
       </c>
       <c r="T10" t="n">
-        <v>0.5694265719019103</v>
+        <v>0.4612527366012719</v>
       </c>
       <c r="U10" t="n">
-        <v>31.17791620524712</v>
+        <v>0.5387472633987281</v>
       </c>
       <c r="V10" t="n">
-        <v>0.9163891418818682</v>
+        <v>46.07082130039582</v>
       </c>
       <c r="W10" t="n">
-        <v>30.98439541603122</v>
+        <v>18.32778283763736</v>
       </c>
       <c r="X10" t="n">
-        <v>0.9163891418818682</v>
+        <v>47.72918615803693</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>18.32778283763736</v>
       </c>
     </row>
     <row r="11">
@@ -1226,73 +1258,76 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>51608.1706641993</v>
+        <v>32158.81255032499</v>
       </c>
       <c r="C11" t="n">
-        <v>54897.94569941166</v>
+        <v>32547.21631087163</v>
       </c>
       <c r="D11" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E11" t="n">
         <v>200</v>
       </c>
       <c r="F11" t="n">
-        <v>133.3403538019629</v>
+        <v>120.6412724874902</v>
       </c>
       <c r="G11" t="n">
-        <v>133.3403538019629</v>
+        <v>120.6412724874902</v>
       </c>
       <c r="H11" t="n">
-        <v>416.17603</v>
+        <v>403.19585</v>
       </c>
       <c r="I11" t="n">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>534.5074777812131</v>
+        <v>531.586289945841</v>
       </c>
       <c r="K11" t="n">
-        <v>0</v>
+        <v>161.0983872933182</v>
       </c>
       <c r="L11" t="n">
-        <v>316.9385031047915</v>
+        <v>424.3098138570484</v>
       </c>
       <c r="M11" t="n">
-        <v>102.2375276173189</v>
+        <v>107.3923548662012</v>
       </c>
       <c r="N11" t="n">
-        <v>376.7363457469071</v>
+        <v>428.3596246532309</v>
       </c>
       <c r="O11" t="n">
-        <v>66.00945978205108</v>
+        <v>93.25255804532502</v>
       </c>
       <c r="P11" t="n">
-        <v>436.0379127995345</v>
+        <v>421.565008746662</v>
       </c>
       <c r="Q11" t="n">
-        <v>98.46956498167864</v>
+        <v>152.9806692567257</v>
       </c>
       <c r="R11" t="n">
-        <v>534.5074777812131</v>
+        <v>421.19585</v>
       </c>
       <c r="S11" t="n">
-        <v>0.4530512335853004</v>
+        <v>574.5456780033877</v>
       </c>
       <c r="T11" t="n">
-        <v>0.5469487664146995</v>
+        <v>0.4758549853070729</v>
       </c>
       <c r="U11" t="n">
-        <v>29.59374486769991</v>
+        <v>0.524145014692927</v>
       </c>
       <c r="V11" t="n">
-        <v>0.9173055310237499</v>
+        <v>45.59741735852441</v>
       </c>
       <c r="W11" t="n">
-        <v>29.68892506713</v>
+        <v>18.346110620475</v>
       </c>
       <c r="X11" t="n">
-        <v>0.9173055310237499</v>
+        <v>49.57642487823007</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>18.346110620475</v>
       </c>
     </row>
     <row r="12">
@@ -1300,10 +1335,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>54396.22972703744</v>
+        <v>16470.79393406543</v>
       </c>
       <c r="C12" t="n">
-        <v>56580.0013493665</v>
+        <v>18559.48215997264</v>
       </c>
       <c r="D12" t="n">
         <v>140</v>
@@ -1312,61 +1347,64 @@
         <v>120</v>
       </c>
       <c r="F12" t="n">
-        <v>140.0073714920611</v>
+        <v>126.6733361118648</v>
       </c>
       <c r="G12" t="n">
-        <v>140.0073714920611</v>
+        <v>126.6733361118648</v>
       </c>
       <c r="H12" t="n">
-        <v>540.78316</v>
+        <v>548.25229</v>
       </c>
       <c r="I12" t="n">
-        <v>197</v>
+        <v>258.228888806283</v>
       </c>
       <c r="J12" t="n">
-        <v>518.0195814924426</v>
+        <v>397.4275281705242</v>
       </c>
       <c r="K12" t="n">
-        <v>0</v>
+        <v>169.1489643909122</v>
       </c>
       <c r="L12" t="n">
-        <v>357.3969356367538</v>
+        <v>431.2226543568743</v>
       </c>
       <c r="M12" t="n">
-        <v>181.3862216234869</v>
+        <v>101.0296348459306</v>
       </c>
       <c r="N12" t="n">
-        <v>410.5678750302009</v>
+        <v>247.2477018780814</v>
       </c>
       <c r="O12" t="n">
-        <v>125.4043495366455</v>
+        <v>58.7756993156356</v>
       </c>
       <c r="P12" t="n">
-        <v>410.503028334192</v>
+        <v>333.6969060374506</v>
       </c>
       <c r="Q12" t="n">
-        <v>107.5165531582507</v>
+        <v>55.68004503547959</v>
       </c>
       <c r="R12" t="n">
-        <v>518.0195814924426</v>
+        <v>306.023401193717</v>
       </c>
       <c r="S12" t="n">
-        <v>0.5085165003044596</v>
+        <v>389.3769510729301</v>
       </c>
       <c r="T12" t="n">
-        <v>0.4914834996955403</v>
+        <v>0.4400679410015227</v>
       </c>
       <c r="U12" t="n">
-        <v>30.52363038971367</v>
+        <v>0.5599320589984772</v>
       </c>
       <c r="V12" t="n">
-        <v>0.9182228365547735</v>
+        <v>47.16081433137722</v>
       </c>
       <c r="W12" t="n">
-        <v>29.80878837092395</v>
+        <v>18.36445673109547</v>
       </c>
       <c r="X12" t="n">
-        <v>0.9182228365547735</v>
+        <v>51.14252200943762</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>18.36445673109547</v>
       </c>
     </row>
     <row r="13">
@@ -1374,16 +1412,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>59112.56133347522</v>
+        <v>29868.49736513371</v>
       </c>
       <c r="C13" t="n">
-        <v>53118.7059220802</v>
+        <v>35440.58702632471</v>
       </c>
       <c r="D13" t="n">
         <v>140</v>
       </c>
       <c r="E13" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F13" t="n">
         <v>133.007002917458</v>
@@ -1392,55 +1430,58 @@
         <v>133.007002917458</v>
       </c>
       <c r="H13" t="n">
-        <v>520.96186</v>
+        <v>299.00769</v>
       </c>
       <c r="I13" t="n">
-        <v>197</v>
+        <v>0</v>
       </c>
       <c r="J13" t="n">
-        <v>517.7177929667129</v>
+        <v>550</v>
       </c>
       <c r="K13" t="n">
-        <v>0</v>
+        <v>167.3641676982294</v>
       </c>
       <c r="L13" t="n">
-        <v>474.9128290229036</v>
+        <v>358.1650106880967</v>
       </c>
       <c r="M13" t="n">
-        <v>46.04903450310047</v>
+        <v>182.0715702850353</v>
       </c>
       <c r="N13" t="n">
-        <v>340.4246160444152</v>
+        <v>387.9371388587863</v>
       </c>
       <c r="O13" t="n">
-        <v>80.74387490253893</v>
+        <v>110.164902624466</v>
       </c>
       <c r="P13" t="n">
-        <v>396.978455257525</v>
+        <v>452.3841075614</v>
       </c>
       <c r="Q13" t="n">
-        <v>120.7393377091878</v>
+        <v>99.40068913128276</v>
       </c>
       <c r="R13" t="n">
-        <v>517.7177929667129</v>
+        <v>316.00769</v>
       </c>
       <c r="S13" t="n">
-        <v>0.4485830692843327</v>
+        <v>551.7847966926828</v>
       </c>
       <c r="T13" t="n">
-        <v>0.5514169307156673</v>
+        <v>0.474434027907856</v>
       </c>
       <c r="U13" t="n">
-        <v>30.10875699746264</v>
+        <v>0.525565972092144</v>
       </c>
       <c r="V13" t="n">
-        <v>0.9191410593913283</v>
+        <v>48.06759061904492</v>
       </c>
       <c r="W13" t="n">
-        <v>29.42888713074941</v>
+        <v>18.38282118782656</v>
       </c>
       <c r="X13" t="n">
-        <v>0.9191410593913283</v>
+        <v>50.00977281543064</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>18.38282118782656</v>
       </c>
     </row>
     <row r="14">
@@ -1448,73 +1489,76 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>58413.36016678347</v>
+        <v>38388.80730359554</v>
       </c>
       <c r="C14" t="n">
-        <v>60289.69405547007</v>
+        <v>30432.85924208136</v>
       </c>
       <c r="D14" t="n">
         <v>140</v>
       </c>
       <c r="E14" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F14" t="n">
-        <v>139.657353063331</v>
+        <v>139.6573530633309</v>
       </c>
       <c r="G14" t="n">
-        <v>139.657353063331</v>
+        <v>139.6573530633309</v>
       </c>
       <c r="H14" t="n">
-        <v>512.61964</v>
+        <v>538.2058</v>
       </c>
       <c r="I14" t="n">
-        <v>204</v>
+        <v>98.84903118169768</v>
       </c>
       <c r="J14" t="n">
-        <v>550</v>
+        <v>523.37618094684</v>
       </c>
       <c r="K14" t="n">
-        <v>0</v>
+        <v>212.3622319580755</v>
       </c>
       <c r="L14" t="n">
-        <v>442.6095890307263</v>
+        <v>405.9892648968214</v>
       </c>
       <c r="M14" t="n">
-        <v>63.01005498979498</v>
+        <v>107.2165360205653</v>
       </c>
       <c r="N14" t="n">
-        <v>422.7172844232662</v>
+        <v>387.6047299043925</v>
       </c>
       <c r="O14" t="n">
-        <v>87.76523956884772</v>
+        <v>76.75203891390981</v>
       </c>
       <c r="P14" t="n">
-        <v>425.836311808594</v>
+        <v>390.4646786498146</v>
       </c>
       <c r="Q14" t="n">
-        <v>125.2084996879976</v>
+        <v>87.91343803717925</v>
       </c>
       <c r="R14" t="n">
-        <v>550</v>
+        <v>464.3567688183023</v>
       </c>
       <c r="S14" t="n">
-        <v>0.4808943744789184</v>
+        <v>478.3781166869938</v>
       </c>
       <c r="T14" t="n">
-        <v>0.5191056255210817</v>
+        <v>0.4925634724649145</v>
       </c>
       <c r="U14" t="n">
-        <v>29.72956749224302</v>
+        <v>0.5074365275350855</v>
       </c>
       <c r="V14" t="n">
-        <v>0.9200602004507196</v>
+        <v>49.09542459149156</v>
       </c>
       <c r="W14" t="n">
-        <v>29.11966730748012</v>
+        <v>18.40120400901439</v>
       </c>
       <c r="X14" t="n">
-        <v>0.9200602004507196</v>
+        <v>49.35412915093104</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>18.40120400901439</v>
       </c>
     </row>
     <row r="15">
@@ -1522,73 +1566,76 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>54427.28160795144</v>
+        <v>37115.12953782582</v>
       </c>
       <c r="C15" t="n">
-        <v>44177.57780474015</v>
+        <v>28078.02012690582</v>
       </c>
       <c r="D15" t="n">
+        <v>140</v>
+      </c>
+      <c r="E15" t="n">
         <v>120</v>
       </c>
-      <c r="E15" t="n">
-        <v>200</v>
-      </c>
       <c r="F15" t="n">
-        <v>132.6744854101644</v>
+        <v>146.6402207164975</v>
       </c>
       <c r="G15" t="n">
-        <v>132.6744854101644</v>
+        <v>146.6402207164975</v>
       </c>
       <c r="H15" t="n">
-        <v>537.78541</v>
+        <v>536.58134</v>
       </c>
       <c r="I15" t="n">
-        <v>204</v>
+        <v>96.25129788401745</v>
       </c>
       <c r="J15" t="n">
-        <v>428.2557303419504</v>
+        <v>399.0559614719149</v>
       </c>
       <c r="K15" t="n">
-        <v>0</v>
+        <v>211.346293737602</v>
       </c>
       <c r="L15" t="n">
-        <v>458.187370609966</v>
+        <v>474.5349387943427</v>
       </c>
       <c r="M15" t="n">
-        <v>79.59803490700558</v>
+        <v>136.8954370846651</v>
       </c>
       <c r="N15" t="n">
-        <v>419.4447740891852</v>
+        <v>386.3750923616626</v>
       </c>
       <c r="O15" t="n">
-        <v>78.60529129114448</v>
+        <v>77.95494975431997</v>
       </c>
       <c r="P15" t="n">
-        <v>310.431714961374</v>
+        <v>336.2363895734441</v>
       </c>
       <c r="Q15" t="n">
-        <v>117.8240153805763</v>
+        <v>63.83551011894436</v>
       </c>
       <c r="R15" t="n">
-        <v>428.2557303419504</v>
+        <v>464.3300421159825</v>
       </c>
       <c r="S15" t="n">
-        <v>0.5376734850201157</v>
+        <v>400.0718996923885</v>
       </c>
       <c r="T15" t="n">
-        <v>0.4623265149798844</v>
+        <v>0.5371691335451901</v>
       </c>
       <c r="U15" t="n">
-        <v>28.93397703609598</v>
+        <v>0.4628308664548098</v>
       </c>
       <c r="V15" t="n">
-        <v>0.9209802606511701</v>
+        <v>51.6204565791343</v>
       </c>
       <c r="W15" t="n">
-        <v>28.33468612150278</v>
+        <v>18.4196052130234</v>
       </c>
       <c r="X15" t="n">
-        <v>0.9209802606511701</v>
+        <v>50.20633200896671</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>18.4196052130234</v>
       </c>
     </row>
     <row r="16">
@@ -1596,10 +1643,10 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>50758.08848537369</v>
+        <v>33224.40119006937</v>
       </c>
       <c r="C16" t="n">
-        <v>31801.33902204601</v>
+        <v>31570.17431336597</v>
       </c>
       <c r="D16" t="n">
         <v>140</v>
@@ -1614,55 +1661,58 @@
         <v>139.3082096806726</v>
       </c>
       <c r="H16" t="n">
-        <v>441.75155</v>
+        <v>491.16136</v>
       </c>
       <c r="I16" t="n">
-        <v>195</v>
+        <v>82.50804286840025</v>
       </c>
       <c r="J16" t="n">
-        <v>287.4744838290169</v>
+        <v>410.7572961552393</v>
       </c>
       <c r="K16" t="n">
-        <v>0</v>
+        <v>172.4621942926192</v>
       </c>
       <c r="L16" t="n">
-        <v>370.0718241218638</v>
+        <v>441.218681007732</v>
       </c>
       <c r="M16" t="n">
-        <v>80.67972451319993</v>
+        <v>124.1939750460987</v>
       </c>
       <c r="N16" t="n">
-        <v>208.5098303589337</v>
+        <v>336.5814568780494</v>
       </c>
       <c r="O16" t="n">
-        <v>66.04919910672835</v>
+        <v>94.0718602535504</v>
       </c>
       <c r="P16" t="n">
-        <v>211.6315905735236</v>
+        <v>341.6206754090986</v>
       </c>
       <c r="Q16" t="n">
-        <v>75.84289325549328</v>
+        <v>108.0207201911235</v>
       </c>
       <c r="R16" t="n">
-        <v>287.4744838290169</v>
+        <v>430.6533171315998</v>
       </c>
       <c r="S16" t="n">
-        <v>0.4885100674089313</v>
+        <v>449.641395600222</v>
       </c>
       <c r="T16" t="n">
-        <v>0.5114899325910689</v>
+        <v>0.4892149309805028</v>
       </c>
       <c r="U16" t="n">
-        <v>29.57245341028847</v>
+        <v>0.5107850690194972</v>
       </c>
       <c r="V16" t="n">
-        <v>0.9219012409118212</v>
+        <v>54.77231988000401</v>
       </c>
       <c r="W16" t="n">
-        <v>26.92124484742579</v>
+        <v>18.43802481823642</v>
       </c>
       <c r="X16" t="n">
-        <v>0.9219012409118212</v>
+        <v>50.10921451685141</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>18.43802481823642</v>
       </c>
     </row>
     <row r="17">
@@ -1670,73 +1720,76 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>56612.68258688097</v>
+        <v>31600.28867398621</v>
       </c>
       <c r="C17" t="n">
-        <v>64132.69917101652</v>
+        <v>22754.56797439734</v>
       </c>
       <c r="D17" t="n">
         <v>140</v>
       </c>
       <c r="E17" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="F17" t="n">
-        <v>146.2736201647063</v>
+        <v>146.2736201647062</v>
       </c>
       <c r="G17" t="n">
-        <v>146.2736201647063</v>
+        <v>146.2736201647062</v>
       </c>
       <c r="H17" t="n">
-        <v>549.65647</v>
+        <v>342.81635</v>
       </c>
       <c r="I17" t="n">
-        <v>200</v>
+        <v>1.197404616386393</v>
       </c>
       <c r="J17" t="n">
-        <v>550</v>
+        <v>367.4820521104208</v>
       </c>
       <c r="K17" t="n">
-        <v>0</v>
+        <v>191.9949343012536</v>
       </c>
       <c r="L17" t="n">
-        <v>438.4991865163782</v>
+        <v>346.881774276726</v>
       </c>
       <c r="M17" t="n">
-        <v>106.1572865942763</v>
+        <v>61.44261740118136</v>
       </c>
       <c r="N17" t="n">
-        <v>461.9854474442073</v>
+        <v>289.8060488378497</v>
       </c>
       <c r="O17" t="n">
-        <v>189.8533433217115</v>
+        <v>68.81289654576385</v>
       </c>
       <c r="P17" t="n">
-        <v>405.0638785467998</v>
+        <v>254.0988310735904</v>
       </c>
       <c r="Q17" t="n">
-        <v>155.8523176189119</v>
+        <v>93.85048102819594</v>
       </c>
       <c r="R17" t="n">
-        <v>550</v>
+        <v>358.6189453836136</v>
       </c>
       <c r="S17" t="n">
-        <v>0.5374859702000685</v>
+        <v>347.9493121017864</v>
       </c>
       <c r="T17" t="n">
-        <v>0.4625140297999315</v>
+        <v>0.5075503202760617</v>
       </c>
       <c r="U17" t="n">
-        <v>30.21619155786729</v>
+        <v>0.4924496797239383</v>
       </c>
       <c r="V17" t="n">
-        <v>0.922823142152733</v>
+        <v>54.26803263755337</v>
       </c>
       <c r="W17" t="n">
-        <v>28.74588943888713</v>
+        <v>18.45646284305466</v>
       </c>
       <c r="X17" t="n">
-        <v>0.922823142152733</v>
+        <v>47.91034829362857</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>18.45646284305466</v>
       </c>
     </row>
     <row r="18">
@@ -1744,73 +1797,76 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>57066.80542678919</v>
+        <v>37683.20054259532</v>
       </c>
       <c r="C18" t="n">
-        <v>49979.61679037339</v>
+        <v>32650.7259217639</v>
       </c>
       <c r="D18" t="n">
         <v>140</v>
       </c>
       <c r="E18" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="F18" t="n">
-        <v>138.959939156471</v>
+        <v>138.9599391564709</v>
       </c>
       <c r="G18" t="n">
-        <v>138.959939156471</v>
+        <v>138.9599391564709</v>
       </c>
       <c r="H18" t="n">
-        <v>511.38283</v>
+        <v>547.6462299999999</v>
       </c>
       <c r="I18" t="n">
-        <v>203</v>
+        <v>93.9470210282206</v>
       </c>
       <c r="J18" t="n">
-        <v>455.2907711794456</v>
+        <v>451.9952019673597</v>
       </c>
       <c r="K18" t="n">
-        <v>0</v>
+        <v>181.7967420349935</v>
       </c>
       <c r="L18" t="n">
-        <v>413.6202235656147</v>
+        <v>410.2667432170369</v>
       </c>
       <c r="M18" t="n">
-        <v>94.76260836401693</v>
+        <v>118.5768925887393</v>
       </c>
       <c r="N18" t="n">
-        <v>350.6453230421221</v>
+        <v>333.7954258713348</v>
       </c>
       <c r="O18" t="n">
-        <v>84.014852904648</v>
+        <v>139.9037831004446</v>
       </c>
       <c r="P18" t="n">
-        <v>358.5776913560793</v>
+        <v>341.3466124565545</v>
       </c>
       <c r="Q18" t="n">
-        <v>96.7130798233663</v>
+        <v>120.8467817770652</v>
       </c>
       <c r="R18" t="n">
-        <v>455.2907711794456</v>
+        <v>473.6992089717793</v>
       </c>
       <c r="S18" t="n">
-        <v>0.4884091391220524</v>
+        <v>462.1933942336198</v>
       </c>
       <c r="T18" t="n">
-        <v>0.5115908608779477</v>
+        <v>0.5061469738615053</v>
       </c>
       <c r="U18" t="n">
-        <v>29.50428142010049</v>
+        <v>0.4938530261384946</v>
       </c>
       <c r="V18" t="n">
-        <v>0.9237459652948856</v>
+        <v>51.94374235242586</v>
       </c>
       <c r="W18" t="n">
-        <v>28.0688772961666</v>
+        <v>18.47491930589771</v>
       </c>
       <c r="X18" t="n">
-        <v>0.9237459652948856</v>
+        <v>46.57315127577198</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>18.47491930589771</v>
       </c>
     </row>
     <row r="19">
@@ -1818,10 +1874,10 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>53687.68712844462</v>
+        <v>35693.97848181438</v>
       </c>
       <c r="C19" t="n">
-        <v>49008.57895627069</v>
+        <v>26752.26675535211</v>
       </c>
       <c r="D19" t="n">
         <v>140</v>
@@ -1836,55 +1892,58 @@
         <v>145.9079361142945</v>
       </c>
       <c r="H19" t="n">
-        <v>483.33191</v>
+        <v>446.07036</v>
       </c>
       <c r="I19" t="n">
-        <v>200</v>
+        <v>41.1369527970748</v>
       </c>
       <c r="J19" t="n">
-        <v>423.2160911618784</v>
+        <v>416.3728236462944</v>
       </c>
       <c r="K19" t="n">
-        <v>0</v>
+        <v>211.4777629823517</v>
       </c>
       <c r="L19" t="n">
-        <v>424.5903043947074</v>
+        <v>411.0961519635019</v>
       </c>
       <c r="M19" t="n">
-        <v>61.74160528792019</v>
+        <v>113.9212274609715</v>
       </c>
       <c r="N19" t="n">
-        <v>391.5977814820505</v>
+        <v>346.1486407262311</v>
       </c>
       <c r="O19" t="n">
-        <v>70.47858347503301</v>
+        <v>73.78476647669416</v>
       </c>
       <c r="P19" t="n">
-        <v>345.9355961625741</v>
+        <v>305.7860438772229</v>
       </c>
       <c r="Q19" t="n">
-        <v>77.28049499930434</v>
+        <v>80.90575882171325</v>
       </c>
       <c r="R19" t="n">
-        <v>423.2160911618784</v>
+        <v>419.9334072029252</v>
       </c>
       <c r="S19" t="n">
-        <v>0.5219477041324654</v>
+        <v>386.6918026989362</v>
       </c>
       <c r="T19" t="n">
-        <v>0.4780522958675346</v>
+        <v>0.5206053592771006</v>
       </c>
       <c r="U19" t="n">
-        <v>30.46569797489379</v>
+        <v>0.4793946407228994</v>
       </c>
       <c r="V19" t="n">
-        <v>0.9246697112601803</v>
+        <v>51.59370961343632</v>
       </c>
       <c r="W19" t="n">
-        <v>28.90589311181406</v>
+        <v>18.49339422520361</v>
       </c>
       <c r="X19" t="n">
-        <v>0.9246697112601803</v>
+        <v>45.81186056259731</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>18.49339422520361</v>
       </c>
     </row>
     <row r="20">
@@ -1892,16 +1951,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>55715.31689338661</v>
+        <v>35774.46668026772</v>
       </c>
       <c r="C20" t="n">
-        <v>59979.68332082509</v>
+        <v>35830.12457526714</v>
       </c>
       <c r="D20" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E20" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F20" t="n">
         <v>138.6125393085798</v>
@@ -1910,55 +1969,58 @@
         <v>138.6125393085798</v>
       </c>
       <c r="H20" t="n">
-        <v>486.11469</v>
+        <v>485.41782</v>
       </c>
       <c r="I20" t="n">
-        <v>202</v>
+        <v>0</v>
       </c>
       <c r="J20" t="n">
-        <v>550</v>
+        <v>457.1105568575338</v>
       </c>
       <c r="K20" t="n">
-        <v>0</v>
+        <v>169.5147495257698</v>
       </c>
       <c r="L20" t="n">
-        <v>425.0059324572871</v>
+        <v>403.6966422221078</v>
       </c>
       <c r="M20" t="n">
-        <v>59.10876031991822</v>
+        <v>100.8581263623944</v>
       </c>
       <c r="N20" t="n">
-        <v>433.637609450222</v>
+        <v>549.5294884589634</v>
       </c>
       <c r="O20" t="n">
-        <v>88.76145007148283</v>
+        <v>123.2665886172543</v>
       </c>
       <c r="P20" t="n">
-        <v>446.7899364180898</v>
+        <v>356.8223060845501</v>
       </c>
       <c r="Q20" t="n">
-        <v>127.5533564166422</v>
+        <v>142.2512642295655</v>
       </c>
       <c r="R20" t="n">
-        <v>550</v>
+        <v>507.41782</v>
       </c>
       <c r="S20" t="n">
-        <v>0.4763188531921736</v>
+        <v>499.0735703141156</v>
       </c>
       <c r="T20" t="n">
-        <v>0.5236811468078264</v>
+        <v>0.5741219414415969</v>
       </c>
       <c r="U20" t="n">
-        <v>30.22782299601548</v>
+        <v>0.4258780585584032</v>
       </c>
       <c r="V20" t="n">
-        <v>0.9255943809714404</v>
+        <v>51.74031666108237</v>
       </c>
       <c r="W20" t="n">
-        <v>28.63297525338092</v>
+        <v>18.51188761942881</v>
       </c>
       <c r="X20" t="n">
-        <v>0.9255943809714404</v>
+        <v>49.9379466861636</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>18.51188761942881</v>
       </c>
     </row>
     <row r="21">
@@ -1966,73 +2028,76 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>52359.02186569505</v>
+        <v>40432.90249359501</v>
       </c>
       <c r="C21" t="n">
-        <v>44739.00749611144</v>
+        <v>31252.13839167538</v>
       </c>
       <c r="D21" t="n">
         <v>140</v>
       </c>
       <c r="E21" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F21" t="n">
-        <v>145.5431662740088</v>
+        <v>145.5431662740087</v>
       </c>
       <c r="G21" t="n">
-        <v>145.5431662740088</v>
+        <v>145.5431662740087</v>
       </c>
       <c r="H21" t="n">
-        <v>477.15635</v>
+        <v>415.52137</v>
       </c>
       <c r="I21" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>396.9052017582044</v>
+        <v>494.9464480055041</v>
       </c>
       <c r="K21" t="n">
-        <v>0</v>
+        <v>213.4426044867236</v>
       </c>
       <c r="L21" t="n">
-        <v>438.4456703860713</v>
+        <v>348.3216125207679</v>
       </c>
       <c r="M21" t="n">
-        <v>40.71068009149108</v>
+        <v>46.19976123075427</v>
       </c>
       <c r="N21" t="n">
-        <v>330.0118747595414</v>
+        <v>387.189500589682</v>
       </c>
       <c r="O21" t="n">
-        <v>93.86171716602567</v>
+        <v>77.63442665435952</v>
       </c>
       <c r="P21" t="n">
-        <v>293.7274764052016</v>
+        <v>344.6184928395808</v>
       </c>
       <c r="Q21" t="n">
-        <v>103.1777253530028</v>
+        <v>106.4001002049695</v>
       </c>
       <c r="R21" t="n">
-        <v>396.9052017582044</v>
+        <v>436.52137</v>
       </c>
       <c r="S21" t="n">
-        <v>0.5164285373689571</v>
+        <v>451.0185930445503</v>
       </c>
       <c r="T21" t="n">
-        <v>0.4835714626310429</v>
+        <v>0.5075369585347167</v>
       </c>
       <c r="U21" t="n">
-        <v>30.6555593707381</v>
+        <v>0.4924630414652832</v>
       </c>
       <c r="V21" t="n">
-        <v>0.9265199753524118</v>
+        <v>49.76901502419717</v>
       </c>
       <c r="W21" t="n">
-        <v>31.53963776867862</v>
+        <v>18.53039950704824</v>
       </c>
       <c r="X21" t="n">
-        <v>0.9265199753524118</v>
+        <v>48.02929861689351</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>18.53039950704824</v>
       </c>
     </row>
     <row r="22">
@@ -2040,16 +2105,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>52775.78923094754</v>
+        <v>51680.86440675028</v>
       </c>
       <c r="C22" t="n">
-        <v>49831.4670217379</v>
+        <v>37729.05508101021</v>
       </c>
       <c r="D22" t="n">
         <v>140</v>
       </c>
       <c r="E22" t="n">
-        <v>120</v>
+        <v>80</v>
       </c>
       <c r="F22" t="n">
         <v>138.2660079603083</v>
@@ -2058,55 +2123,58 @@
         <v>138.2660079603083</v>
       </c>
       <c r="H22" t="n">
-        <v>512.86643</v>
+        <v>538.88801</v>
       </c>
       <c r="I22" t="n">
-        <v>199</v>
+        <v>0</v>
       </c>
       <c r="J22" t="n">
-        <v>471.9225908222924</v>
+        <v>490.9652805062645</v>
       </c>
       <c r="K22" t="n">
-        <v>0</v>
+        <v>190.324831833944</v>
       </c>
       <c r="L22" t="n">
-        <v>356.1626382343459</v>
+        <v>419.2567026716844</v>
       </c>
       <c r="M22" t="n">
-        <v>157.7037906841103</v>
+        <v>95.63130843365909</v>
       </c>
       <c r="N22" t="n">
-        <v>352.405175922681</v>
+        <v>400.6108558681446</v>
       </c>
       <c r="O22" t="n">
-        <v>122.2121752727775</v>
+        <v>167.5047002656671</v>
       </c>
       <c r="P22" t="n">
-        <v>365.8304938351143</v>
+        <v>415.8726297201322</v>
       </c>
       <c r="Q22" t="n">
-        <v>106.0920969871782</v>
+        <v>98.21042343891189</v>
       </c>
       <c r="R22" t="n">
-        <v>471.9225908222924</v>
+        <v>562.88801</v>
       </c>
       <c r="S22" t="n">
-        <v>0.5014234794822401</v>
+        <v>514.0830531590441</v>
       </c>
       <c r="T22" t="n">
-        <v>0.4985765205177599</v>
+        <v>0.5249642267652119</v>
       </c>
       <c r="U22" t="n">
-        <v>29.44887508336984</v>
+        <v>0.4750357732347881</v>
       </c>
       <c r="V22" t="n">
-        <v>0.927446495327764</v>
+        <v>50.33227032319707</v>
       </c>
       <c r="W22" t="n">
-        <v>31.5926603113825</v>
+        <v>18.54892990655528</v>
       </c>
       <c r="X22" t="n">
-        <v>0.927446495327764</v>
+        <v>46.37516384781094</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>18.54892990655528</v>
       </c>
     </row>
     <row r="23">
@@ -2114,16 +2182,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>55380.63813759504</v>
+        <v>39544.14044163503</v>
       </c>
       <c r="C23" t="n">
-        <v>44625.75640999018</v>
+        <v>32779.9705853888</v>
       </c>
       <c r="D23" t="n">
         <v>140</v>
       </c>
       <c r="E23" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F23" t="n">
         <v>145.1793083583237</v>
@@ -2132,55 +2200,58 @@
         <v>145.1793083583237</v>
       </c>
       <c r="H23" t="n">
-        <v>484.80967</v>
+        <v>481.4344</v>
       </c>
       <c r="I23" t="n">
-        <v>197</v>
+        <v>42.56160146905921</v>
       </c>
       <c r="J23" t="n">
-        <v>403.2228927734443</v>
+        <v>443.1648853825891</v>
       </c>
       <c r="K23" t="n">
-        <v>0</v>
+        <v>195.9931188759207</v>
       </c>
       <c r="L23" t="n">
-        <v>371.8153892539989</v>
+        <v>390.1867025410588</v>
       </c>
       <c r="M23" t="n">
-        <v>114.9942830170438</v>
+        <v>75.24769711249211</v>
       </c>
       <c r="N23" t="n">
-        <v>338.3002455399545</v>
+        <v>392.8632628117987</v>
       </c>
       <c r="O23" t="n">
-        <v>90.60745766696847</v>
+        <v>62.00953571914211</v>
       </c>
       <c r="P23" t="n">
-        <v>303.3733694382249</v>
+        <v>352.30317843099</v>
       </c>
       <c r="Q23" t="n">
-        <v>99.8495233352194</v>
+        <v>85.19341990962238</v>
       </c>
       <c r="R23" t="n">
-        <v>403.2228927734443</v>
+        <v>454.8727985309408</v>
       </c>
       <c r="S23" t="n">
-        <v>0.5154331607067147</v>
+        <v>437.4965983406124</v>
       </c>
       <c r="T23" t="n">
-        <v>0.4845668392932853</v>
+        <v>0.5097359906397763</v>
       </c>
       <c r="U23" t="n">
-        <v>29.22383122574499</v>
+        <v>0.4902640093602238</v>
       </c>
       <c r="V23" t="n">
-        <v>0.9283739418230917</v>
+        <v>49.96096695574425</v>
       </c>
       <c r="W23" t="n">
-        <v>33.24032154252979</v>
+        <v>18.56747883646184</v>
       </c>
       <c r="X23" t="n">
-        <v>0.9283739418230917</v>
+        <v>45.42639554042096</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>18.56747883646184</v>
       </c>
     </row>
     <row r="24">
@@ -2188,73 +2259,76 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>49318.00094702316</v>
+        <v>45803.0652335039</v>
       </c>
       <c r="C24" t="n">
-        <v>36319.85175718849</v>
+        <v>42638.49338636606</v>
       </c>
       <c r="D24" t="n">
         <v>140</v>
       </c>
       <c r="E24" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F24" t="n">
-        <v>137.9203429404076</v>
+        <v>137.9203429404075</v>
       </c>
       <c r="G24" t="n">
-        <v>137.9203429404076</v>
+        <v>137.9203429404075</v>
       </c>
       <c r="H24" t="n">
-        <v>428.82503</v>
+        <v>447.57332</v>
       </c>
       <c r="I24" t="n">
-        <v>203</v>
+        <v>0</v>
       </c>
       <c r="J24" t="n">
-        <v>356.7176763936033</v>
+        <v>550</v>
       </c>
       <c r="K24" t="n">
-        <v>0</v>
+        <v>179.0200017853022</v>
       </c>
       <c r="L24" t="n">
-        <v>360.7614213492092</v>
+        <v>346.3003760281439</v>
       </c>
       <c r="M24" t="n">
-        <v>62.06361332770209</v>
+        <v>118.8345429999317</v>
       </c>
       <c r="N24" t="n">
-        <v>283.4380373601511</v>
+        <v>447.5728451764754</v>
       </c>
       <c r="O24" t="n">
-        <v>41.73384827747133</v>
+        <v>85.2298860650511</v>
       </c>
       <c r="P24" t="n">
-        <v>296.4537102533232</v>
+        <v>468.1257032294731</v>
       </c>
       <c r="Q24" t="n">
-        <v>60.26396614028016</v>
+        <v>98.84741386114554</v>
       </c>
       <c r="R24" t="n">
-        <v>356.7176763936033</v>
+        <v>472.57332</v>
       </c>
       <c r="S24" t="n">
-        <v>0.4768688417358878</v>
+        <v>566.9731170906186</v>
       </c>
       <c r="T24" t="n">
-        <v>0.5231311582641122</v>
+        <v>0.4844648407669104</v>
       </c>
       <c r="U24" t="n">
-        <v>29.57897404854341</v>
+        <v>0.5155351592330897</v>
       </c>
       <c r="V24" t="n">
-        <v>0.9293023157649147</v>
+        <v>45.48349657324549</v>
       </c>
       <c r="W24" t="n">
-        <v>34.67071314011755</v>
+        <v>18.5860463152983</v>
       </c>
       <c r="X24" t="n">
-        <v>0.9293023157649147</v>
+        <v>45.41503251596223</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>18.5860463152983</v>
       </c>
     </row>
     <row r="25">
@@ -2262,73 +2336,76 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>52142.84939819178</v>
+        <v>24383.70742697809</v>
       </c>
       <c r="C25" t="n">
-        <v>50521.48171851912</v>
+        <v>23500.92592623192</v>
       </c>
       <c r="D25" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E25" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F25" t="n">
-        <v>131.0243257933872</v>
+        <v>144.8163600874279</v>
       </c>
       <c r="G25" t="n">
-        <v>131.0243257933872</v>
+        <v>144.8163600874279</v>
       </c>
       <c r="H25" t="n">
-        <v>515.65807</v>
+        <v>518.6442500000001</v>
       </c>
       <c r="I25" t="n">
-        <v>200</v>
+        <v>189.5826010537876</v>
       </c>
       <c r="J25" t="n">
-        <v>524.3198860199514</v>
+        <v>328.6535057280738</v>
       </c>
       <c r="K25" t="n">
-        <v>0</v>
+        <v>174.985511598456</v>
       </c>
       <c r="L25" t="n">
-        <v>443.3630629741593</v>
+        <v>376.8265772375016</v>
       </c>
       <c r="M25" t="n">
-        <v>75.29500491993052</v>
+        <v>117.8176764878082</v>
       </c>
       <c r="N25" t="n">
-        <v>498.7756600771572</v>
+        <v>285.0266072134901</v>
       </c>
       <c r="O25" t="n">
-        <v>93.00101373573538</v>
+        <v>68.03504173272232</v>
       </c>
       <c r="P25" t="n">
-        <v>383.236485044875</v>
+        <v>257.5258498178787</v>
       </c>
       <c r="Q25" t="n">
-        <v>141.0834009750764</v>
+        <v>75.16214609704129</v>
       </c>
       <c r="R25" t="n">
-        <v>524.3198860199514</v>
+        <v>353.0616489462125</v>
       </c>
       <c r="S25" t="n">
-        <v>0.5302199604499471</v>
+        <v>332.68799591492</v>
       </c>
       <c r="T25" t="n">
-        <v>0.4697800395500529</v>
+        <v>0.5148550226631311</v>
       </c>
       <c r="U25" t="n">
-        <v>29.49258944546154</v>
+        <v>0.4851449773368688</v>
       </c>
       <c r="V25" t="n">
-        <v>0.9302316180806796</v>
+        <v>47.55814457286296</v>
       </c>
       <c r="W25" t="n">
-        <v>33.69231442176128</v>
+        <v>18.60463236161359</v>
       </c>
       <c r="X25" t="n">
-        <v>0.9302316180806796</v>
+        <v>42.8877818711777</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>18.60463236161359</v>
       </c>
     </row>
     <row r="26">
@@ -2336,16 +2413,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>59676.88064092662</v>
+        <v>41302.77714535171</v>
       </c>
       <c r="C26" t="n">
-        <v>52467.4136609074</v>
+        <v>27560.35541450699</v>
       </c>
       <c r="D26" t="n">
         <v>140</v>
       </c>
       <c r="E26" t="n">
-        <v>200</v>
+        <v>80</v>
       </c>
       <c r="F26" t="n">
         <v>137.5755420830565</v>
@@ -2354,55 +2431,58 @@
         <v>137.5755420830565</v>
       </c>
       <c r="H26" t="n">
-        <v>491.99627</v>
+        <v>474.81596</v>
       </c>
       <c r="I26" t="n">
-        <v>199</v>
+        <v>42.08008476711359</v>
       </c>
       <c r="J26" t="n">
-        <v>522.5827066253061</v>
+        <v>466.8991446442613</v>
       </c>
       <c r="K26" t="n">
-        <v>0</v>
+        <v>216.4222774482309</v>
       </c>
       <c r="L26" t="n">
-        <v>402.2241221709222</v>
+        <v>486.9958519540866</v>
       </c>
       <c r="M26" t="n">
-        <v>90.77214481187868</v>
+        <v>158.4027107979167</v>
       </c>
       <c r="N26" t="n">
-        <v>380.2502868315967</v>
+        <v>342.9072496975735</v>
       </c>
       <c r="O26" t="n">
-        <v>84.19564835320196</v>
+        <v>108.828625535313</v>
       </c>
       <c r="P26" t="n">
-        <v>400.7092615904712</v>
+        <v>361.3570208329328</v>
       </c>
       <c r="Q26" t="n">
-        <v>121.8734450348349</v>
+        <v>64.10535796155345</v>
       </c>
       <c r="R26" t="n">
-        <v>522.5827066253061</v>
+        <v>451.7358752328864</v>
       </c>
       <c r="S26" t="n">
-        <v>0.470549602626581</v>
+        <v>425.4623787944863</v>
       </c>
       <c r="T26" t="n">
-        <v>0.529450397373419</v>
+        <v>0.5149758029714342</v>
       </c>
       <c r="U26" t="n">
-        <v>28.20912932539898</v>
+        <v>0.4850241970285658</v>
       </c>
       <c r="V26" t="n">
-        <v>0.9311618496987601</v>
+        <v>46.03064567947159</v>
       </c>
       <c r="W26" t="n">
-        <v>36.19531651001954</v>
+        <v>18.6232369939752</v>
       </c>
       <c r="X26" t="n">
-        <v>0.9311618496987601</v>
+        <v>43.47242293188006</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>18.6232369939752</v>
       </c>
     </row>
     <row r="27">
@@ -2410,16 +2490,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>56130.14491382247</v>
+        <v>41058.14572675453</v>
       </c>
       <c r="C27" t="n">
-        <v>25506.16137264417</v>
+        <v>31423.87078506264</v>
       </c>
       <c r="D27" t="n">
         <v>120</v>
       </c>
       <c r="E27" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F27" t="n">
         <v>130.6967649789037</v>
@@ -2428,55 +2508,58 @@
         <v>130.6967649789037</v>
       </c>
       <c r="H27" t="n">
-        <v>531.82681</v>
+        <v>515.68597</v>
       </c>
       <c r="I27" t="n">
-        <v>200</v>
+        <v>0</v>
       </c>
       <c r="J27" t="n">
-        <v>273.7134418544128</v>
+        <v>502.03319493983</v>
       </c>
       <c r="K27" t="n">
-        <v>0</v>
+        <v>229.6572401688507</v>
       </c>
       <c r="L27" t="n">
-        <v>431.4303713603553</v>
+        <v>450.0671797718276</v>
       </c>
       <c r="M27" t="n">
-        <v>99.39644141660206</v>
+        <v>91.69887837682478</v>
       </c>
       <c r="N27" t="n">
-        <v>282.6807487751033</v>
+        <v>478.1351452232685</v>
       </c>
       <c r="O27" t="n">
-        <v>36.09017462767059</v>
+        <v>96.99217411556569</v>
       </c>
       <c r="P27" t="n">
-        <v>218.8330952632002</v>
+        <v>370.1412078350306</v>
       </c>
       <c r="Q27" t="n">
-        <v>54.88034659121256</v>
+        <v>118.6570243841796</v>
       </c>
       <c r="R27" t="n">
-        <v>273.7134418544128</v>
+        <v>531.68597</v>
       </c>
       <c r="S27" t="n">
-        <v>0.5380241945530515</v>
+        <v>488.7982322192102</v>
       </c>
       <c r="T27" t="n">
-        <v>0.4619758054469484</v>
+        <v>0.5405710188054047</v>
       </c>
       <c r="U27" t="n">
-        <v>27.46784573795542</v>
+        <v>0.4594289811945953</v>
       </c>
       <c r="V27" t="n">
-        <v>0.9320930115484587</v>
+        <v>44.10469160765701</v>
       </c>
       <c r="W27" t="n">
-        <v>35.63817979317817</v>
+        <v>18.64186023096918</v>
       </c>
       <c r="X27" t="n">
-        <v>0.9320930115484587</v>
+        <v>43.32012206609343</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>18.64186023096918</v>
       </c>
     </row>
     <row r="28">
@@ -2484,10 +2567,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>60030.13936905122</v>
+        <v>31977.6958561637</v>
       </c>
       <c r="C28" t="n">
-        <v>56025.91171311292</v>
+        <v>31837.29373139142</v>
       </c>
       <c r="D28" t="n">
         <v>140</v>
@@ -2502,55 +2585,58 @@
         <v>137.2316032278489</v>
       </c>
       <c r="H28" t="n">
-        <v>481.55965</v>
+        <v>474.98114</v>
       </c>
       <c r="I28" t="n">
-        <v>201</v>
+        <v>119.7366893311528</v>
       </c>
       <c r="J28" t="n">
-        <v>550</v>
+        <v>372.0145741775597</v>
       </c>
       <c r="K28" t="n">
-        <v>0</v>
+        <v>177.2588560645775</v>
       </c>
       <c r="L28" t="n">
-        <v>367.462375549989</v>
+        <v>360.7947511089586</v>
       </c>
       <c r="M28" t="n">
-        <v>113.0972722025417</v>
+        <v>92.18639281912597</v>
       </c>
       <c r="N28" t="n">
-        <v>430.5240619961158</v>
+        <v>315.9100280689236</v>
       </c>
       <c r="O28" t="n">
-        <v>109.8178759064671</v>
+        <v>61.33442259992366</v>
       </c>
       <c r="P28" t="n">
-        <v>457.1074084198019</v>
+        <v>335.4163610621032</v>
       </c>
       <c r="Q28" t="n">
-        <v>159.3463646560239</v>
+        <v>88.99659721972971</v>
       </c>
       <c r="R28" t="n">
-        <v>550</v>
+        <v>377.2444506688472</v>
       </c>
       <c r="S28" t="n">
-        <v>0.4671023005830182</v>
+        <v>424.412958281833</v>
       </c>
       <c r="T28" t="n">
-        <v>0.5328976994169817</v>
+        <v>0.470580632645355</v>
       </c>
       <c r="U28" t="n">
-        <v>27.24248977452239</v>
+        <v>0.5294193673546449</v>
       </c>
       <c r="V28" t="n">
-        <v>0.933025104560007</v>
+        <v>43.36394042679801</v>
       </c>
       <c r="W28" t="n">
-        <v>34.43328409944718</v>
+        <v>18.66050209120014</v>
       </c>
       <c r="X28" t="n">
-        <v>0.933025104560007</v>
+        <v>42.43861450028577</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>18.66050209120014</v>
       </c>
     </row>
     <row r="29">
@@ -2558,16 +2644,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>56141.70882360678</v>
+        <v>37030.7224089188</v>
       </c>
       <c r="C29" t="n">
-        <v>52992.0074636495</v>
+        <v>27726.45414861419</v>
       </c>
       <c r="D29" t="n">
         <v>140</v>
       </c>
       <c r="E29" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F29" t="n">
         <v>144.0931833892413</v>
@@ -2576,55 +2662,58 @@
         <v>144.0931833892413</v>
       </c>
       <c r="H29" t="n">
-        <v>448.79861</v>
+        <v>518.50339</v>
       </c>
       <c r="I29" t="n">
-        <v>200</v>
+        <v>108.5439138658128</v>
       </c>
       <c r="J29" t="n">
-        <v>479.2803870258147</v>
+        <v>418.2238253975313</v>
       </c>
       <c r="K29" t="n">
-        <v>0</v>
+        <v>206.2824500989175</v>
       </c>
       <c r="L29" t="n">
-        <v>331.7631359760433</v>
+        <v>485.9773790347368</v>
       </c>
       <c r="M29" t="n">
-        <v>118.0354718727595</v>
+        <v>128.2627032333014</v>
       </c>
       <c r="N29" t="n">
-        <v>397.4326476150481</v>
+        <v>328.9118615334429</v>
       </c>
       <c r="O29" t="n">
-        <v>82.92239555753216</v>
+        <v>105.0476146007442</v>
       </c>
       <c r="P29" t="n">
-        <v>364.5188040207257</v>
+        <v>301.6726459536626</v>
       </c>
       <c r="Q29" t="n">
-        <v>114.761583005089</v>
+        <v>87.52758540952865</v>
       </c>
       <c r="R29" t="n">
-        <v>479.2803870258147</v>
+        <v>433.9594761341871</v>
       </c>
       <c r="S29" t="n">
-        <v>0.5005599293820068</v>
+        <v>389.2002313631913</v>
       </c>
       <c r="T29" t="n">
-        <v>0.4994400706179932</v>
+        <v>0.527187460928497</v>
       </c>
       <c r="U29" t="n">
-        <v>28.96298546084103</v>
+        <v>0.4728125390715031</v>
       </c>
       <c r="V29" t="n">
-        <v>0.9339581296645668</v>
+        <v>45.33531867966335</v>
       </c>
       <c r="W29" t="n">
-        <v>32.45564118352797</v>
+        <v>18.67916259329134</v>
       </c>
       <c r="X29" t="n">
-        <v>0.9339581296645668</v>
+        <v>42.24661715777397</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>18.67916259329134</v>
       </c>
     </row>
     <row r="30">
@@ -2632,16 +2721,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>54088.03812727136</v>
+        <v>29942.56688168814</v>
       </c>
       <c r="C30" t="n">
-        <v>57112.18093307033</v>
+        <v>27762.66202382493</v>
       </c>
       <c r="D30" t="n">
         <v>140</v>
       </c>
       <c r="E30" t="n">
-        <v>200</v>
+        <v>120</v>
       </c>
       <c r="F30" t="n">
         <v>136.8885242197792</v>
@@ -2650,55 +2739,58 @@
         <v>136.8885242197792</v>
       </c>
       <c r="H30" t="n">
-        <v>445.97488</v>
+        <v>520.84849</v>
       </c>
       <c r="I30" t="n">
-        <v>200</v>
+        <v>162.7731043728166</v>
       </c>
       <c r="J30" t="n">
-        <v>550</v>
+        <v>387.0810183629328</v>
       </c>
       <c r="K30" t="n">
-        <v>0</v>
+        <v>197.0475718127254</v>
       </c>
       <c r="L30" t="n">
-        <v>365.135696094813</v>
+        <v>483.1418344872918</v>
       </c>
       <c r="M30" t="n">
-        <v>80.83918389766922</v>
+        <v>122.2505739947209</v>
       </c>
       <c r="N30" t="n">
-        <v>477.1074579405463</v>
+        <v>317.7669112372794</v>
       </c>
       <c r="O30" t="n">
-        <v>52.07947936405007</v>
+        <v>64.30847438990396</v>
       </c>
       <c r="P30" t="n">
-        <v>510.3850625778426</v>
+        <v>339.9307266691621</v>
       </c>
       <c r="Q30" t="n">
-        <v>75.75040236961595</v>
+        <v>56.38516997996278</v>
       </c>
       <c r="R30" t="n">
-        <v>550</v>
+        <v>382.0753856271834</v>
       </c>
       <c r="S30" t="n">
-        <v>0.4744699256789464</v>
+        <v>396.3158966491249</v>
       </c>
       <c r="T30" t="n">
-        <v>0.5255300743210537</v>
+        <v>0.4908526011620423</v>
       </c>
       <c r="U30" t="n">
-        <v>27.54550986649624</v>
+        <v>0.5091473988379578</v>
       </c>
       <c r="V30" t="n">
-        <v>0.9348920877942314</v>
+        <v>44.58578904082432</v>
       </c>
       <c r="W30" t="n">
-        <v>32.11330316276623</v>
+        <v>18.69784175588463</v>
       </c>
       <c r="X30" t="n">
-        <v>0.9348920877942314</v>
+        <v>40.84552673447329</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>18.69784175588463</v>
       </c>
     </row>
     <row r="31">
@@ -2706,73 +2798,76 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>51614.32055060698</v>
+        <v>41695.02831058641</v>
       </c>
       <c r="C31" t="n">
-        <v>53715.64942791841</v>
+        <v>28772.95256186561</v>
       </c>
       <c r="D31" t="n">
+        <v>140</v>
+      </c>
+      <c r="E31" t="n">
         <v>120</v>
       </c>
-      <c r="E31" t="n">
-        <v>160</v>
-      </c>
       <c r="F31" t="n">
-        <v>130.0440980087903</v>
+        <v>143.7329504307682</v>
       </c>
       <c r="G31" t="n">
-        <v>130.0440980087903</v>
+        <v>143.7329504307682</v>
       </c>
       <c r="H31" t="n">
-        <v>534.45641</v>
+        <v>402.75775</v>
       </c>
       <c r="I31" t="n">
-        <v>201</v>
+        <v>0</v>
       </c>
       <c r="J31" t="n">
-        <v>550</v>
+        <v>371.5820501681176</v>
       </c>
       <c r="K31" t="n">
-        <v>0</v>
+        <v>184.9370864610624</v>
       </c>
       <c r="L31" t="n">
-        <v>442.2518720539908</v>
+        <v>450.3400142725828</v>
       </c>
       <c r="M31" t="n">
-        <v>91.20454074521908</v>
+        <v>100.1908357809609</v>
       </c>
       <c r="N31" t="n">
-        <v>502.0359931535815</v>
+        <v>342.1615237368266</v>
       </c>
       <c r="O31" t="n">
-        <v>126.7266974115259</v>
+        <v>80.81326868864612</v>
       </c>
       <c r="P31" t="n">
-        <v>394.5145326258906</v>
+        <v>316.1900760809001</v>
       </c>
       <c r="Q31" t="n">
-        <v>155.8032192824016</v>
+        <v>67.50245943888054</v>
       </c>
       <c r="R31" t="n">
-        <v>550</v>
+        <v>417.75775</v>
       </c>
       <c r="S31" t="n">
-        <v>0.5332653039737723</v>
+        <v>383.6925355197806</v>
       </c>
       <c r="T31" t="n">
-        <v>0.4667346960262276</v>
+        <v>0.5243484863864215</v>
       </c>
       <c r="U31" t="n">
-        <v>28.31274074563323</v>
+        <v>0.4756515136135785</v>
       </c>
       <c r="V31" t="n">
-        <v>0.9358269798820255</v>
+        <v>41.69021375606948</v>
       </c>
       <c r="W31" t="n">
-        <v>31.44345388723841</v>
+        <v>18.71653959764052</v>
       </c>
       <c r="X31" t="n">
-        <v>0.9358269798820255</v>
+        <v>42.28497223674159</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>18.71653959764052</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Inkluidierung divereser RAW Data
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y31"/>
+  <dimension ref="A1:AD31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -511,50 +511,75 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>B_Frühbucher_Nachfrage</t>
+          <t>B_Frühbucher_Nachfrage_Tatsächlich</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
         <is>
-          <t>B_LastMinute_Nachfrage</t>
+          <t>B_LastMinute_Nachfrage_Tatsächlich</t>
         </is>
       </c>
       <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>B_Frühbucher_Nachfrage_Geschätzt</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>B_LastMinute_Nachfrage_Geschätzt</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
         <is>
           <t>Verkaufte_Menge_A</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Verkaufte_Menge_B</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_A</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Marktanteil_B</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Gesamtnachfrage</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>OEE_A</t>
+        </is>
+      </c>
+      <c r="Z1" s="1" t="inlineStr">
+        <is>
+          <t>OEE_B</t>
+        </is>
+      </c>
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>Var_Kosten_A_Einheit</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>Fix_Kosten_A_Einheit</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>Var_Kosten_B_Einheit</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
         <is>
           <t>Fix_Kosten_B_Einheit</t>
         </is>
@@ -613,27 +638,42 @@
         <v>112.3860915408043</v>
       </c>
       <c r="R2" t="n">
+        <v>399.3940034220185</v>
+      </c>
+      <c r="S2" t="n">
+        <v>105.6815689345646</v>
+      </c>
+      <c r="T2" t="n">
         <v>331.2892249928187</v>
       </c>
-      <c r="S2" t="n">
+      <c r="U2" t="n">
         <v>516.6853362583413</v>
       </c>
-      <c r="T2" t="n">
+      <c r="V2" t="n">
         <v>0.3906829758006087</v>
       </c>
-      <c r="U2" t="n">
+      <c r="W2" t="n">
         <v>0.6093170241993914</v>
       </c>
-      <c r="V2" t="n">
+      <c r="X2" t="n">
+        <v>847.9745612511599</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.8372116545454545</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="n">
         <v>45</v>
       </c>
-      <c r="W2" t="n">
+      <c r="AB2" t="n">
         <v>18.18181818181818</v>
       </c>
-      <c r="X2" t="n">
+      <c r="AC2" t="n">
         <v>45</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="AD2" t="n">
         <v>18.18181818181818</v>
       </c>
     </row>
@@ -690,27 +730,42 @@
         <v>110.179958506696</v>
       </c>
       <c r="R3" t="n">
+        <v>342.7963699780718</v>
+      </c>
+      <c r="S3" t="n">
+        <v>115.1591159711511</v>
+      </c>
+      <c r="T3" t="n">
         <v>234.9824697521333</v>
       </c>
-      <c r="S3" t="n">
+      <c r="U3" t="n">
         <v>463.6358823058373</v>
       </c>
-      <c r="T3" t="n">
+      <c r="V3" t="n">
         <v>0.3363531305181555</v>
       </c>
-      <c r="U3" t="n">
+      <c r="W3" t="n">
         <v>0.6636468694818445</v>
       </c>
-      <c r="V3" t="n">
+      <c r="X3" t="n">
+        <v>698.6183520579706</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>0.4833211090909091</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="n">
         <v>46.25598473676393</v>
       </c>
-      <c r="W3" t="n">
+      <c r="AB3" t="n">
         <v>18.2</v>
       </c>
-      <c r="X3" t="n">
+      <c r="AC3" t="n">
         <v>46.87727780592505</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="AD3" t="n">
         <v>18.2</v>
       </c>
     </row>
@@ -767,27 +822,42 @@
         <v>72.69389348852722</v>
       </c>
       <c r="R4" t="n">
+        <v>255.7756508449141</v>
+      </c>
+      <c r="S4" t="n">
+        <v>69.3724064997074</v>
+      </c>
+      <c r="T4" t="n">
         <v>268.2391201348916</v>
       </c>
-      <c r="S4" t="n">
+      <c r="U4" t="n">
         <v>312.7294974636652</v>
       </c>
-      <c r="T4" t="n">
+      <c r="V4" t="n">
         <v>0.4617101716159168</v>
       </c>
-      <c r="U4" t="n">
+      <c r="W4" t="n">
         <v>0.5382898283840831</v>
       </c>
-      <c r="V4" t="n">
+      <c r="X4" t="n">
+        <v>580.9686175985568</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>0.8019199818181818</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>0.7372168652887274</v>
+      </c>
+      <c r="AA4" t="n">
         <v>47.36461721476797</v>
       </c>
-      <c r="W4" t="n">
+      <c r="AB4" t="n">
         <v>18.21819999999999</v>
       </c>
-      <c r="X4" t="n">
+      <c r="AC4" t="n">
         <v>49.44462420808044</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="AD4" t="n">
         <v>18.21819999999999</v>
       </c>
     </row>
@@ -844,27 +914,42 @@
         <v>124.7643287754309</v>
       </c>
       <c r="R5" t="n">
+        <v>376.9083803515171</v>
+      </c>
+      <c r="S5" t="n">
+        <v>134.8797708125523</v>
+      </c>
+      <c r="T5" t="n">
         <v>290.65286</v>
       </c>
-      <c r="S5" t="n">
+      <c r="U5" t="n">
         <v>542.5452482769663</v>
       </c>
-      <c r="T5" t="n">
+      <c r="V5" t="n">
         <v>0.4045206630058025</v>
       </c>
-      <c r="U5" t="n">
+      <c r="W5" t="n">
         <v>0.5954793369941975</v>
       </c>
-      <c r="V5" t="n">
+      <c r="X5" t="n">
+        <v>911.1067581548224</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>0.4975506545454545</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>0.9079447114238419</v>
+      </c>
+      <c r="AA5" t="n">
         <v>46.96765861767919</v>
       </c>
-      <c r="W5" t="n">
+      <c r="AB5" t="n">
         <v>18.23641819999999</v>
       </c>
-      <c r="X5" t="n">
+      <c r="AC5" t="n">
         <v>50.66205825509726</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="AD5" t="n">
         <v>18.23641819999999</v>
       </c>
     </row>
@@ -921,27 +1006,42 @@
         <v>130.0520976047686</v>
       </c>
       <c r="R6" t="n">
+        <v>397.0398995201982</v>
+      </c>
+      <c r="S6" t="n">
+        <v>140.9550555713583</v>
+      </c>
+      <c r="T6" t="n">
         <v>424.2345505127807</v>
       </c>
-      <c r="S6" t="n">
+      <c r="U6" t="n">
         <v>520.7499842116029</v>
       </c>
-      <c r="T6" t="n">
+      <c r="V6" t="n">
         <v>0.4489327972298658</v>
       </c>
-      <c r="U6" t="n">
+      <c r="W6" t="n">
         <v>0.5510672027701342</v>
       </c>
-      <c r="V6" t="n">
+      <c r="X6" t="n">
+        <v>944.9845347243836</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.7893500181818182</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="n">
         <v>48.10045204146028</v>
       </c>
-      <c r="W6" t="n">
+      <c r="AB6" t="n">
         <v>18.25465461819999</v>
       </c>
-      <c r="X6" t="n">
+      <c r="AC6" t="n">
         <v>50.48876624431989</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="AD6" t="n">
         <v>18.25465461819999</v>
       </c>
     </row>
@@ -998,27 +1098,42 @@
         <v>95.33986340588866</v>
       </c>
       <c r="R7" t="n">
+        <v>456.7577571550914</v>
+      </c>
+      <c r="S7" t="n">
+        <v>100.0736723999619</v>
+      </c>
+      <c r="T7" t="n">
         <v>352.1579723863221</v>
       </c>
-      <c r="S7" t="n">
+      <c r="U7" t="n">
         <v>525.7398172245504</v>
       </c>
-      <c r="T7" t="n">
+      <c r="V7" t="n">
         <v>0.4011377822723712</v>
       </c>
-      <c r="U7" t="n">
+      <c r="W7" t="n">
         <v>0.5988622177276288</v>
       </c>
-      <c r="V7" t="n">
+      <c r="X7" t="n">
+        <v>877.8977896108725</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.7939677636363637</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="n">
         <v>47.47431035739504</v>
       </c>
-      <c r="W7" t="n">
+      <c r="AB7" t="n">
         <v>18.27290927281819</v>
       </c>
-      <c r="X7" t="n">
+      <c r="AC7" t="n">
         <v>50.41578434926424</v>
       </c>
-      <c r="Y7" t="n">
+      <c r="AD7" t="n">
         <v>18.27290927281819</v>
       </c>
     </row>
@@ -1075,27 +1190,42 @@
         <v>60.54203563562387</v>
       </c>
       <c r="R8" t="n">
+        <v>392.0553447389427</v>
+      </c>
+      <c r="S8" t="n">
+        <v>63.22521689008691</v>
+      </c>
+      <c r="T8" t="n">
         <v>363.1941422832199</v>
       </c>
-      <c r="S8" t="n">
+      <c r="U8" t="n">
         <v>421.786851660823</v>
       </c>
-      <c r="T8" t="n">
+      <c r="V8" t="n">
         <v>0.4626788993430204</v>
       </c>
-      <c r="U8" t="n">
+      <c r="W8" t="n">
         <v>0.5373211006569797</v>
       </c>
-      <c r="V8" t="n">
+      <c r="X8" t="n">
+        <v>784.9809939440429</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.8345590727272728</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.7864135639601451</v>
+      </c>
+      <c r="AA8" t="n">
         <v>46.45772118944935</v>
       </c>
-      <c r="W8" t="n">
+      <c r="AB8" t="n">
         <v>18.291182182091</v>
       </c>
-      <c r="X8" t="n">
+      <c r="AC8" t="n">
         <v>47.50310469822417</v>
       </c>
-      <c r="Y8" t="n">
+      <c r="AD8" t="n">
         <v>18.291182182091</v>
       </c>
     </row>
@@ -1152,27 +1282,42 @@
         <v>90.38181949567866</v>
       </c>
       <c r="R9" t="n">
+        <v>548.7426521898858</v>
+      </c>
+      <c r="S9" t="n">
+        <v>85.40367605907485</v>
+      </c>
+      <c r="T9" t="n">
         <v>448.5655559492673</v>
       </c>
-      <c r="S9" t="n">
+      <c r="U9" t="n">
         <v>644.4190799108458</v>
       </c>
-      <c r="T9" t="n">
+      <c r="V9" t="n">
         <v>0.4104042648287304</v>
       </c>
-      <c r="U9" t="n">
+      <c r="W9" t="n">
         <v>0.5895957351712696</v>
       </c>
-      <c r="V9" t="n">
+      <c r="X9" t="n">
+        <v>1092.984635860113</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.7956514545454545</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="n">
         <v>47.67850773913931</v>
       </c>
-      <c r="W9" t="n">
+      <c r="AB9" t="n">
         <v>18.30947336427309</v>
       </c>
-      <c r="X9" t="n">
+      <c r="AC9" t="n">
         <v>48.99160680581618</v>
       </c>
-      <c r="Y9" t="n">
+      <c r="AD9" t="n">
         <v>18.30947336427309</v>
       </c>
     </row>
@@ -1229,27 +1374,42 @@
         <v>63.40418119160216</v>
       </c>
       <c r="R10" t="n">
+        <v>399.5361756560255</v>
+      </c>
+      <c r="S10" t="n">
+        <v>66.46897375230596</v>
+      </c>
+      <c r="T10" t="n">
         <v>395.4999030632309</v>
       </c>
-      <c r="S10" t="n">
+      <c r="U10" t="n">
         <v>461.9473740574666</v>
       </c>
-      <c r="T10" t="n">
+      <c r="V10" t="n">
         <v>0.4612527366012719</v>
       </c>
-      <c r="U10" t="n">
+      <c r="W10" t="n">
         <v>0.5387472633987281</v>
       </c>
-      <c r="V10" t="n">
+      <c r="X10" t="n">
+        <v>857.4472771206974</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.9491022181818182</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.9580554897290374</v>
+      </c>
+      <c r="AA10" t="n">
         <v>46.07082130039582</v>
       </c>
-      <c r="W10" t="n">
+      <c r="AB10" t="n">
         <v>18.32778283763736</v>
       </c>
-      <c r="X10" t="n">
+      <c r="AC10" t="n">
         <v>47.72918615803693</v>
       </c>
-      <c r="Y10" t="n">
+      <c r="AD10" t="n">
         <v>18.32778283763736</v>
       </c>
     </row>
@@ -1306,27 +1466,42 @@
         <v>152.9806692567257</v>
       </c>
       <c r="R11" t="n">
+        <v>384.035825856692</v>
+      </c>
+      <c r="S11" t="n">
+        <v>151.6082394400139</v>
+      </c>
+      <c r="T11" t="n">
         <v>421.19585</v>
       </c>
-      <c r="S11" t="n">
+      <c r="U11" t="n">
         <v>574.5456780033877</v>
       </c>
-      <c r="T11" t="n">
+      <c r="V11" t="n">
         <v>0.4758549853070729</v>
       </c>
-      <c r="U11" t="n">
+      <c r="W11" t="n">
         <v>0.524145014692927</v>
       </c>
-      <c r="V11" t="n">
+      <c r="X11" t="n">
+        <v>1096.157860701944</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.7330833636363636</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.9665205271742564</v>
+      </c>
+      <c r="AA11" t="n">
         <v>45.59741735852441</v>
       </c>
-      <c r="W11" t="n">
+      <c r="AB11" t="n">
         <v>18.346110620475</v>
       </c>
-      <c r="X11" t="n">
+      <c r="AC11" t="n">
         <v>49.57642487823007</v>
       </c>
-      <c r="Y11" t="n">
+      <c r="AD11" t="n">
         <v>18.346110620475</v>
       </c>
     </row>
@@ -1383,27 +1558,42 @@
         <v>55.68004503547959</v>
       </c>
       <c r="R12" t="n">
+        <v>300.6663943003705</v>
+      </c>
+      <c r="S12" t="n">
+        <v>57.85952116347181</v>
+      </c>
+      <c r="T12" t="n">
         <v>306.023401193717</v>
       </c>
-      <c r="S12" t="n">
+      <c r="U12" t="n">
         <v>389.3769510729301</v>
       </c>
-      <c r="T12" t="n">
+      <c r="V12" t="n">
         <v>0.4400679410015227</v>
       </c>
-      <c r="U12" t="n">
+      <c r="W12" t="n">
         <v>0.5599320589984772</v>
       </c>
-      <c r="V12" t="n">
+      <c r="X12" t="n">
+        <v>695.4003522666471</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.9968223454545455</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.7225955057645894</v>
+      </c>
+      <c r="AA12" t="n">
         <v>47.16081433137722</v>
       </c>
-      <c r="W12" t="n">
+      <c r="AB12" t="n">
         <v>18.36445673109547</v>
       </c>
-      <c r="X12" t="n">
+      <c r="AC12" t="n">
         <v>51.14252200943762</v>
       </c>
-      <c r="Y12" t="n">
+      <c r="AD12" t="n">
         <v>18.36445673109547</v>
       </c>
     </row>
@@ -1460,27 +1650,42 @@
         <v>99.40068913128276</v>
       </c>
       <c r="R13" t="n">
+        <v>427.9512586383945</v>
+      </c>
+      <c r="S13" t="n">
+        <v>93.69717110559675</v>
+      </c>
+      <c r="T13" t="n">
         <v>316.00769</v>
       </c>
-      <c r="S13" t="n">
+      <c r="U13" t="n">
         <v>551.7847966926828</v>
       </c>
-      <c r="T13" t="n">
+      <c r="V13" t="n">
         <v>0.474434027907856</v>
       </c>
-      <c r="U13" t="n">
+      <c r="W13" t="n">
         <v>0.525565972092144</v>
       </c>
-      <c r="V13" t="n">
+      <c r="X13" t="n">
+        <v>1049.886838175935</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.5436503454545455</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="n">
         <v>48.06759061904492</v>
       </c>
-      <c r="W13" t="n">
+      <c r="AB13" t="n">
         <v>18.38282118782656</v>
       </c>
-      <c r="X13" t="n">
+      <c r="AC13" t="n">
         <v>50.00977281543064</v>
       </c>
-      <c r="Y13" t="n">
+      <c r="AD13" t="n">
         <v>18.38282118782656</v>
       </c>
     </row>
@@ -1537,27 +1742,42 @@
         <v>87.91343803717925</v>
       </c>
       <c r="R14" t="n">
+        <v>402.8586347618499</v>
+      </c>
+      <c r="S14" t="n">
+        <v>87.88171388321956</v>
+      </c>
+      <c r="T14" t="n">
         <v>464.3567688183023</v>
       </c>
-      <c r="S14" t="n">
+      <c r="U14" t="n">
         <v>478.3781166869938</v>
       </c>
-      <c r="T14" t="n">
+      <c r="V14" t="n">
         <v>0.4925634724649145</v>
       </c>
-      <c r="U14" t="n">
+      <c r="W14" t="n">
         <v>0.5074365275350855</v>
       </c>
-      <c r="V14" t="n">
+      <c r="X14" t="n">
+        <v>942.7348855052961</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.9785559999999999</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.9515930562669819</v>
+      </c>
+      <c r="AA14" t="n">
         <v>49.09542459149156</v>
       </c>
-      <c r="W14" t="n">
+      <c r="AB14" t="n">
         <v>18.40120400901439</v>
       </c>
-      <c r="X14" t="n">
+      <c r="AC14" t="n">
         <v>49.35412915093104</v>
       </c>
-      <c r="Y14" t="n">
+      <c r="AD14" t="n">
         <v>18.40120400901439</v>
       </c>
     </row>
@@ -1614,27 +1834,42 @@
         <v>63.83551011894436</v>
       </c>
       <c r="R15" t="n">
+        <v>348.8928562351055</v>
+      </c>
+      <c r="S15" t="n">
+        <v>62.52533719488495</v>
+      </c>
+      <c r="T15" t="n">
         <v>464.3300421159825</v>
       </c>
-      <c r="S15" t="n">
+      <c r="U15" t="n">
         <v>400.0718996923885</v>
       </c>
-      <c r="T15" t="n">
+      <c r="V15" t="n">
         <v>0.5371691335451901</v>
       </c>
-      <c r="U15" t="n">
+      <c r="W15" t="n">
         <v>0.4628308664548098</v>
       </c>
-      <c r="V15" t="n">
+      <c r="X15" t="n">
+        <v>864.401941808371</v>
+      </c>
+      <c r="Y15" t="n">
+        <v>0.9756024363636363</v>
+      </c>
+      <c r="Z15" t="n">
+        <v>0.7255562935852998</v>
+      </c>
+      <c r="AA15" t="n">
         <v>51.6204565791343</v>
       </c>
-      <c r="W15" t="n">
+      <c r="AB15" t="n">
         <v>18.4196052130234</v>
       </c>
-      <c r="X15" t="n">
+      <c r="AC15" t="n">
         <v>50.20633200896671</v>
       </c>
-      <c r="Y15" t="n">
+      <c r="AD15" t="n">
         <v>18.4196052130234</v>
       </c>
     </row>
@@ -1691,27 +1926,42 @@
         <v>108.0207201911235</v>
       </c>
       <c r="R16" t="n">
+        <v>314.388098251263</v>
+      </c>
+      <c r="S16" t="n">
+        <v>107.7154916415781</v>
+      </c>
+      <c r="T16" t="n">
         <v>430.6533171315998</v>
       </c>
-      <c r="S16" t="n">
+      <c r="U16" t="n">
         <v>449.641395600222</v>
       </c>
-      <c r="T16" t="n">
+      <c r="V16" t="n">
         <v>0.4892149309805028</v>
       </c>
-      <c r="U16" t="n">
+      <c r="W16" t="n">
         <v>0.5107850690194972</v>
       </c>
-      <c r="V16" t="n">
+      <c r="X16" t="n">
+        <v>880.2947127318218</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.8930206545454545</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.7468314475549804</v>
+      </c>
+      <c r="AA16" t="n">
         <v>54.77231988000401</v>
       </c>
-      <c r="W16" t="n">
+      <c r="AB16" t="n">
         <v>18.43802481823642</v>
       </c>
-      <c r="X16" t="n">
+      <c r="AC16" t="n">
         <v>50.10921451685141</v>
       </c>
-      <c r="Y16" t="n">
+      <c r="AD16" t="n">
         <v>18.43802481823642</v>
       </c>
     </row>
@@ -1768,27 +2018,42 @@
         <v>93.85048102819594</v>
       </c>
       <c r="R17" t="n">
+        <v>251.9063974922246</v>
+      </c>
+      <c r="S17" t="n">
+        <v>88.03784891081534</v>
+      </c>
+      <c r="T17" t="n">
         <v>358.6189453836136</v>
       </c>
-      <c r="S17" t="n">
+      <c r="U17" t="n">
         <v>347.9493121017864</v>
       </c>
-      <c r="T17" t="n">
+      <c r="V17" t="n">
         <v>0.5075503202760617</v>
       </c>
-      <c r="U17" t="n">
+      <c r="W17" t="n">
         <v>0.4924496797239383</v>
       </c>
-      <c r="V17" t="n">
+      <c r="X17" t="n">
+        <v>706.5682574854</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.6233024545454545</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.6681491856553106</v>
+      </c>
+      <c r="AA17" t="n">
         <v>54.26803263755337</v>
       </c>
-      <c r="W17" t="n">
+      <c r="AB17" t="n">
         <v>18.45646284305466</v>
       </c>
-      <c r="X17" t="n">
+      <c r="AC17" t="n">
         <v>47.91034829362857</v>
       </c>
-      <c r="Y17" t="n">
+      <c r="AD17" t="n">
         <v>18.45646284305466</v>
       </c>
     </row>
@@ -1845,27 +2110,42 @@
         <v>120.8467817770652</v>
       </c>
       <c r="R18" t="n">
+        <v>311.182754123581</v>
+      </c>
+      <c r="S18" t="n">
+        <v>132.8073821450322</v>
+      </c>
+      <c r="T18" t="n">
         <v>473.6992089717793</v>
       </c>
-      <c r="S18" t="n">
+      <c r="U18" t="n">
         <v>462.1933942336198</v>
       </c>
-      <c r="T18" t="n">
+      <c r="V18" t="n">
         <v>0.5061469738615053</v>
       </c>
-      <c r="U18" t="n">
+      <c r="W18" t="n">
         <v>0.4938530261384946</v>
       </c>
-      <c r="V18" t="n">
+      <c r="X18" t="n">
+        <v>935.8926032053992</v>
+      </c>
+      <c r="Y18" t="n">
+        <v>0.9957204181818181</v>
+      </c>
+      <c r="Z18" t="n">
+        <v>0.8218094581224721</v>
+      </c>
+      <c r="AA18" t="n">
         <v>51.94374235242586</v>
       </c>
-      <c r="W18" t="n">
+      <c r="AB18" t="n">
         <v>18.47491930589771</v>
       </c>
-      <c r="X18" t="n">
+      <c r="AC18" t="n">
         <v>46.57315127577198</v>
       </c>
-      <c r="Y18" t="n">
+      <c r="AD18" t="n">
         <v>18.47491930589771</v>
       </c>
     </row>
@@ -1922,27 +2202,42 @@
         <v>80.90575882171325</v>
       </c>
       <c r="R19" t="n">
+        <v>312.8199159754594</v>
+      </c>
+      <c r="S19" t="n">
+        <v>85.3496497058285</v>
+      </c>
+      <c r="T19" t="n">
         <v>419.9334072029252</v>
       </c>
-      <c r="S19" t="n">
+      <c r="U19" t="n">
         <v>386.6918026989362</v>
       </c>
-      <c r="T19" t="n">
+      <c r="V19" t="n">
         <v>0.5206053592771006</v>
       </c>
-      <c r="U19" t="n">
+      <c r="W19" t="n">
         <v>0.4793946407228994</v>
       </c>
-      <c r="V19" t="n">
+      <c r="X19" t="n">
+        <v>806.6252099018614</v>
+      </c>
+      <c r="Y19" t="n">
+        <v>0.8110370181818182</v>
+      </c>
+      <c r="Z19" t="n">
+        <v>0.7570414975387171</v>
+      </c>
+      <c r="AA19" t="n">
         <v>51.59370961343632</v>
       </c>
-      <c r="W19" t="n">
+      <c r="AB19" t="n">
         <v>18.49339422520361</v>
       </c>
-      <c r="X19" t="n">
+      <c r="AC19" t="n">
         <v>45.81186056259731</v>
       </c>
-      <c r="Y19" t="n">
+      <c r="AD19" t="n">
         <v>18.49339422520361</v>
       </c>
     </row>
@@ -1999,27 +2294,42 @@
         <v>142.2512642295655</v>
       </c>
       <c r="R20" t="n">
+        <v>336.6410857042395</v>
+      </c>
+      <c r="S20" t="n">
+        <v>131.947234135646</v>
+      </c>
+      <c r="T20" t="n">
         <v>507.41782</v>
       </c>
-      <c r="S20" t="n">
+      <c r="U20" t="n">
         <v>499.0735703141156</v>
       </c>
-      <c r="T20" t="n">
+      <c r="V20" t="n">
         <v>0.5741219414415969</v>
       </c>
-      <c r="U20" t="n">
+      <c r="W20" t="n">
         <v>0.4258780585584032</v>
       </c>
-      <c r="V20" t="n">
+      <c r="X20" t="n">
+        <v>1171.869647390333</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.8825778545454546</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.8311101033773342</v>
+      </c>
+      <c r="AA20" t="n">
         <v>51.74031666108237</v>
       </c>
-      <c r="W20" t="n">
+      <c r="AB20" t="n">
         <v>18.51188761942881</v>
       </c>
-      <c r="X20" t="n">
+      <c r="AC20" t="n">
         <v>49.9379466861636</v>
       </c>
-      <c r="Y20" t="n">
+      <c r="AD20" t="n">
         <v>18.51188761942881</v>
       </c>
     </row>
@@ -2076,27 +2386,42 @@
         <v>106.4001002049695</v>
       </c>
       <c r="R21" t="n">
+        <v>348.7655065798838</v>
+      </c>
+      <c r="S21" t="n">
+        <v>115.69569095139</v>
+      </c>
+      <c r="T21" t="n">
         <v>436.52137</v>
       </c>
-      <c r="S21" t="n">
+      <c r="U21" t="n">
         <v>451.0185930445503</v>
       </c>
-      <c r="T21" t="n">
+      <c r="V21" t="n">
         <v>0.5075369585347167</v>
       </c>
-      <c r="U21" t="n">
+      <c r="W21" t="n">
         <v>0.4924630414652832</v>
       </c>
-      <c r="V21" t="n">
+      <c r="X21" t="n">
+        <v>915.8425202885918</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.7554934</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.8999026327372801</v>
+      </c>
+      <c r="AA21" t="n">
         <v>49.76901502419717</v>
       </c>
-      <c r="W21" t="n">
+      <c r="AB21" t="n">
         <v>18.53039950704824</v>
       </c>
-      <c r="X21" t="n">
+      <c r="AC21" t="n">
         <v>48.02929861689351</v>
       </c>
-      <c r="Y21" t="n">
+      <c r="AD21" t="n">
         <v>18.53039950704824</v>
       </c>
     </row>
@@ -2153,27 +2478,42 @@
         <v>98.21042343891189</v>
       </c>
       <c r="R22" t="n">
+        <v>400.3324672107321</v>
+      </c>
+      <c r="S22" t="n">
+        <v>104.075417782256</v>
+      </c>
+      <c r="T22" t="n">
         <v>562.88801</v>
       </c>
-      <c r="S22" t="n">
+      <c r="U22" t="n">
         <v>514.0830531590441</v>
       </c>
-      <c r="T22" t="n">
+      <c r="V22" t="n">
         <v>0.5249642267652119</v>
       </c>
-      <c r="U22" t="n">
+      <c r="W22" t="n">
         <v>0.4750357732347881</v>
       </c>
-      <c r="V22" t="n">
+      <c r="X22" t="n">
+        <v>1082.198609292856</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.9797963818181818</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0.8926641463750263</v>
+      </c>
+      <c r="AA22" t="n">
         <v>50.33227032319707</v>
       </c>
-      <c r="W22" t="n">
+      <c r="AB22" t="n">
         <v>18.54892990655528</v>
       </c>
-      <c r="X22" t="n">
+      <c r="AC22" t="n">
         <v>46.37516384781094</v>
       </c>
-      <c r="Y22" t="n">
+      <c r="AD22" t="n">
         <v>18.54892990655528</v>
       </c>
     </row>
@@ -2230,27 +2570,42 @@
         <v>85.19341990962238</v>
       </c>
       <c r="R23" t="n">
+        <v>355.1708189668503</v>
+      </c>
+      <c r="S23" t="n">
+        <v>78.31889824968276</v>
+      </c>
+      <c r="T23" t="n">
         <v>454.8727985309408</v>
       </c>
-      <c r="S23" t="n">
+      <c r="U23" t="n">
         <v>437.4965983406124</v>
       </c>
-      <c r="T23" t="n">
+      <c r="V23" t="n">
         <v>0.5097359906397763</v>
       </c>
-      <c r="U23" t="n">
+      <c r="W23" t="n">
         <v>0.4902640093602238</v>
       </c>
-      <c r="V23" t="n">
+      <c r="X23" t="n">
+        <v>892.3693968715531</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.8753352727272727</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0.8057543370592529</v>
+      </c>
+      <c r="AA23" t="n">
         <v>49.96096695574425</v>
       </c>
-      <c r="W23" t="n">
+      <c r="AB23" t="n">
         <v>18.56747883646184</v>
       </c>
-      <c r="X23" t="n">
+      <c r="AC23" t="n">
         <v>45.42639554042096</v>
       </c>
-      <c r="Y23" t="n">
+      <c r="AD23" t="n">
         <v>18.56747883646184</v>
       </c>
     </row>
@@ -2307,27 +2662,42 @@
         <v>98.84741386114554</v>
       </c>
       <c r="R24" t="n">
+        <v>503.9147143069497</v>
+      </c>
+      <c r="S24" t="n">
+        <v>102.2268686484356</v>
+      </c>
+      <c r="T24" t="n">
         <v>472.57332</v>
       </c>
-      <c r="S24" t="n">
+      <c r="U24" t="n">
         <v>566.9731170906186</v>
       </c>
-      <c r="T24" t="n">
+      <c r="V24" t="n">
         <v>0.4844648407669104</v>
       </c>
-      <c r="U24" t="n">
+      <c r="W24" t="n">
         <v>0.5155351592330897</v>
       </c>
-      <c r="V24" t="n">
+      <c r="X24" t="n">
+        <v>1099.775848332145</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>0.8137696727272727</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>1</v>
+      </c>
+      <c r="AA24" t="n">
         <v>45.48349657324549</v>
       </c>
-      <c r="W24" t="n">
+      <c r="AB24" t="n">
         <v>18.5860463152983</v>
       </c>
-      <c r="X24" t="n">
+      <c r="AC24" t="n">
         <v>45.41503251596223</v>
       </c>
-      <c r="Y24" t="n">
+      <c r="AD24" t="n">
         <v>18.5860463152983</v>
       </c>
     </row>
@@ -2384,27 +2754,42 @@
         <v>75.16214609704129</v>
       </c>
       <c r="R25" t="n">
+        <v>236.8878416666772</v>
+      </c>
+      <c r="S25" t="n">
+        <v>70.78566584669868</v>
+      </c>
+      <c r="T25" t="n">
         <v>353.0616489462125</v>
       </c>
-      <c r="S25" t="n">
+      <c r="U25" t="n">
         <v>332.68799591492</v>
       </c>
-      <c r="T25" t="n">
+      <c r="V25" t="n">
         <v>0.5148550226631311</v>
       </c>
-      <c r="U25" t="n">
+      <c r="W25" t="n">
         <v>0.4851449773368688</v>
       </c>
-      <c r="V25" t="n">
+      <c r="X25" t="n">
+        <v>685.7496448611324</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>0.9429895454545456</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0.5975518285964977</v>
+      </c>
+      <c r="AA25" t="n">
         <v>47.55814457286296</v>
       </c>
-      <c r="W25" t="n">
+      <c r="AB25" t="n">
         <v>18.60463236161359</v>
       </c>
-      <c r="X25" t="n">
+      <c r="AC25" t="n">
         <v>42.8877818711777</v>
       </c>
-      <c r="Y25" t="n">
+      <c r="AD25" t="n">
         <v>18.60463236161359</v>
       </c>
     </row>
@@ -2461,27 +2846,42 @@
         <v>64.10535796155345</v>
       </c>
       <c r="R26" t="n">
+        <v>374.9239564324091</v>
+      </c>
+      <c r="S26" t="n">
+        <v>66.96069981030816</v>
+      </c>
+      <c r="T26" t="n">
         <v>451.7358752328864</v>
       </c>
-      <c r="S26" t="n">
+      <c r="U26" t="n">
         <v>425.4623787944863</v>
       </c>
-      <c r="T26" t="n">
+      <c r="V26" t="n">
         <v>0.5149758029714342</v>
       </c>
-      <c r="U26" t="n">
+      <c r="W26" t="n">
         <v>0.4850241970285658</v>
       </c>
-      <c r="V26" t="n">
+      <c r="X26" t="n">
+        <v>877.1982540273727</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>0.8633017454545455</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0.8489075357168387</v>
+      </c>
+      <c r="AA26" t="n">
         <v>46.03064567947159</v>
       </c>
-      <c r="W26" t="n">
+      <c r="AB26" t="n">
         <v>18.6232369939752</v>
       </c>
-      <c r="X26" t="n">
+      <c r="AC26" t="n">
         <v>43.47242293188006</v>
       </c>
-      <c r="Y26" t="n">
+      <c r="AD26" t="n">
         <v>18.6232369939752</v>
       </c>
     </row>
@@ -2538,27 +2938,42 @@
         <v>118.6570243841796</v>
       </c>
       <c r="R27" t="n">
+        <v>395.6253339358569</v>
+      </c>
+      <c r="S27" t="n">
+        <v>122.830138452204</v>
+      </c>
+      <c r="T27" t="n">
         <v>531.68597</v>
       </c>
-      <c r="S27" t="n">
+      <c r="U27" t="n">
         <v>488.7982322192102</v>
       </c>
-      <c r="T27" t="n">
+      <c r="V27" t="n">
         <v>0.5405710188054047</v>
       </c>
-      <c r="U27" t="n">
+      <c r="W27" t="n">
         <v>0.4594289811945953</v>
       </c>
-      <c r="V27" t="n">
+      <c r="X27" t="n">
+        <v>1063.925551558044</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>0.9376108545454546</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0.9127876271633272</v>
+      </c>
+      <c r="AA27" t="n">
         <v>44.10469160765701</v>
       </c>
-      <c r="W27" t="n">
+      <c r="AB27" t="n">
         <v>18.64186023096918</v>
       </c>
-      <c r="X27" t="n">
+      <c r="AC27" t="n">
         <v>43.32012206609343</v>
       </c>
-      <c r="Y27" t="n">
+      <c r="AD27" t="n">
         <v>18.64186023096918</v>
       </c>
     </row>
@@ -2615,27 +3030,42 @@
         <v>88.99659721972971</v>
       </c>
       <c r="R28" t="n">
+        <v>317.1854999736415</v>
+      </c>
+      <c r="S28" t="n">
+        <v>84.48631437276885</v>
+      </c>
+      <c r="T28" t="n">
         <v>377.2444506688472</v>
       </c>
-      <c r="S28" t="n">
+      <c r="U28" t="n">
         <v>424.412958281833</v>
       </c>
-      <c r="T28" t="n">
+      <c r="V28" t="n">
         <v>0.470580632645355</v>
       </c>
-      <c r="U28" t="n">
+      <c r="W28" t="n">
         <v>0.5294193673546449</v>
       </c>
-      <c r="V28" t="n">
+      <c r="X28" t="n">
+        <v>801.6574089506802</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.8636020727272727</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0.6763901348682904</v>
+      </c>
+      <c r="AA28" t="n">
         <v>43.36394042679801</v>
       </c>
-      <c r="W28" t="n">
+      <c r="AB28" t="n">
         <v>18.66050209120014</v>
       </c>
-      <c r="X28" t="n">
+      <c r="AC28" t="n">
         <v>42.43861450028577</v>
       </c>
-      <c r="Y28" t="n">
+      <c r="AD28" t="n">
         <v>18.66050209120014</v>
       </c>
     </row>
@@ -2692,27 +3122,42 @@
         <v>87.52758540952865</v>
       </c>
       <c r="R29" t="n">
+        <v>302.5585750795016</v>
+      </c>
+      <c r="S29" t="n">
+        <v>92.92410638260714</v>
+      </c>
+      <c r="T29" t="n">
         <v>433.9594761341871</v>
       </c>
-      <c r="S29" t="n">
+      <c r="U29" t="n">
         <v>389.2002313631913</v>
       </c>
-      <c r="T29" t="n">
+      <c r="V29" t="n">
         <v>0.527187460928497</v>
       </c>
-      <c r="U29" t="n">
+      <c r="W29" t="n">
         <v>0.4728125390715031</v>
       </c>
-      <c r="V29" t="n">
+      <c r="X29" t="n">
+        <v>823.1597074973783</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.9427334363636363</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0.7604069552682388</v>
+      </c>
+      <c r="AA29" t="n">
         <v>45.33531867966335</v>
       </c>
-      <c r="W29" t="n">
+      <c r="AB29" t="n">
         <v>18.67916259329134</v>
       </c>
-      <c r="X29" t="n">
+      <c r="AC29" t="n">
         <v>42.24661715777397</v>
       </c>
-      <c r="Y29" t="n">
+      <c r="AD29" t="n">
         <v>18.67916259329134</v>
       </c>
     </row>
@@ -2769,27 +3214,42 @@
         <v>56.38516997996278</v>
       </c>
       <c r="R30" t="n">
+        <v>334.1158523193758</v>
+      </c>
+      <c r="S30" t="n">
+        <v>59.24761614247447</v>
+      </c>
+      <c r="T30" t="n">
         <v>382.0753856271834</v>
       </c>
-      <c r="S30" t="n">
+      <c r="U30" t="n">
         <v>396.3158966491249</v>
       </c>
-      <c r="T30" t="n">
+      <c r="V30" t="n">
         <v>0.4908526011620423</v>
       </c>
-      <c r="U30" t="n">
+      <c r="W30" t="n">
         <v>0.5091473988379578</v>
       </c>
-      <c r="V30" t="n">
+      <c r="X30" t="n">
+        <v>778.3912822763082</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.9469972545454545</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0.7037836697507869</v>
+      </c>
+      <c r="AA30" t="n">
         <v>44.58578904082432</v>
       </c>
-      <c r="W30" t="n">
+      <c r="AB30" t="n">
         <v>18.69784175588463</v>
       </c>
-      <c r="X30" t="n">
+      <c r="AC30" t="n">
         <v>40.84552673447329</v>
       </c>
-      <c r="Y30" t="n">
+      <c r="AD30" t="n">
         <v>18.69784175588463</v>
       </c>
     </row>
@@ -2846,27 +3306,42 @@
         <v>67.50245943888054</v>
       </c>
       <c r="R31" t="n">
+        <v>302.0449404584951</v>
+      </c>
+      <c r="S31" t="n">
+        <v>66.58468152234785</v>
+      </c>
+      <c r="T31" t="n">
         <v>417.75775</v>
       </c>
-      <c r="S31" t="n">
+      <c r="U31" t="n">
         <v>383.6925355197806</v>
       </c>
-      <c r="T31" t="n">
+      <c r="V31" t="n">
         <v>0.5243484863864215</v>
       </c>
-      <c r="U31" t="n">
+      <c r="W31" t="n">
         <v>0.4756515136135785</v>
       </c>
-      <c r="V31" t="n">
+      <c r="X31" t="n">
+        <v>806.6673279452533</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.7322868181818182</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.6756037275783956</v>
+      </c>
+      <c r="AA31" t="n">
         <v>41.69021375606948</v>
       </c>
-      <c r="W31" t="n">
+      <c r="AB31" t="n">
         <v>18.71653959764052</v>
       </c>
-      <c r="X31" t="n">
+      <c r="AC31" t="n">
         <v>42.28497223674159</v>
       </c>
-      <c r="Y31" t="n">
+      <c r="AD31" t="n">
         <v>18.71653959764052</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Entfernen Redundante Infos (Unsicherheit)
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -590,16 +590,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>18733.36417912387</v>
+        <v>5679.821430338987</v>
       </c>
       <c r="C2" t="n">
-        <v>19435.33097964252</v>
+        <v>7038.958685885242</v>
       </c>
       <c r="D2" t="n">
         <v>120</v>
       </c>
       <c r="E2" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F2" t="n">
         <v>105</v>
@@ -608,58 +608,58 @@
         <v>105</v>
       </c>
       <c r="H2" t="n">
-        <v>460.46641</v>
+        <v>482.68944</v>
       </c>
       <c r="I2" t="n">
-        <v>150.1771850071813</v>
+        <v>270.8351358168936</v>
       </c>
       <c r="J2" t="n">
         <v>550</v>
       </c>
       <c r="K2" t="n">
-        <v>33.31466374165871</v>
+        <v>149.1686104122874</v>
       </c>
       <c r="L2" t="n">
-        <v>344.879640681565</v>
+        <v>375.7246723676083</v>
       </c>
       <c r="M2" t="n">
-        <v>94.58676801844989</v>
+        <v>85.96476708572624</v>
       </c>
       <c r="N2" t="n">
-        <v>271.0098883321972</v>
+        <v>208.3202128865276</v>
       </c>
       <c r="O2" t="n">
-        <v>60.27933666062149</v>
+        <v>24.53409129657886</v>
       </c>
       <c r="P2" t="n">
-        <v>404.2992447175371</v>
+        <v>355.1036484297632</v>
       </c>
       <c r="Q2" t="n">
-        <v>112.3860915408043</v>
+        <v>45.72774115794944</v>
       </c>
       <c r="R2" t="n">
-        <v>399.3940034220185</v>
+        <v>379.5499168516393</v>
       </c>
       <c r="S2" t="n">
-        <v>105.6815689345646</v>
+        <v>49.66048086110753</v>
       </c>
       <c r="T2" t="n">
-        <v>331.2892249928187</v>
+        <v>232.8543041831064</v>
       </c>
       <c r="U2" t="n">
-        <v>516.6853362583413</v>
+        <v>400.8313895877126</v>
       </c>
       <c r="V2" t="n">
-        <v>0.3906829758006087</v>
+        <v>0.3674602511498726</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6093170241993914</v>
+        <v>0.6325397488501274</v>
       </c>
       <c r="X2" t="n">
-        <v>847.9745612511599</v>
+        <v>633.6856937708189</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.8372116545454545</v>
+        <v>0.8776171636363637</v>
       </c>
       <c r="Z2" t="n">
         <v>1</v>
@@ -682,88 +682,88 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>20501.78587001723</v>
+        <v>22319.71931434115</v>
       </c>
       <c r="C3" t="n">
-        <v>15083.99566808814</v>
+        <v>11586.13502190949</v>
       </c>
       <c r="D3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E3" t="n">
         <v>140</v>
       </c>
-      <c r="E3" t="n">
-        <v>200</v>
-      </c>
       <c r="F3" t="n">
-        <v>110.25</v>
+        <v>99.75</v>
       </c>
       <c r="G3" t="n">
-        <v>110.25</v>
+        <v>99.75</v>
       </c>
       <c r="H3" t="n">
-        <v>265.82661</v>
+        <v>432.0445</v>
       </c>
       <c r="I3" t="n">
-        <v>49.84414024786673</v>
+        <v>47.68288049144132</v>
       </c>
       <c r="J3" t="n">
-        <v>550</v>
+        <v>463.3996279601339</v>
       </c>
       <c r="K3" t="n">
-        <v>119.6787814358214</v>
+        <v>177.3523968049869</v>
       </c>
       <c r="L3" t="n">
-        <v>268.2830090240139</v>
+        <v>599.9608859919654</v>
       </c>
       <c r="M3" t="n">
-        <v>128.7207834765261</v>
+        <v>78.91875469625967</v>
       </c>
       <c r="N3" t="n">
-        <v>173.2043444305178</v>
+        <v>373.0809820866488</v>
       </c>
       <c r="O3" t="n">
-        <v>61.77812532161548</v>
+        <v>35.2806374219099</v>
       </c>
       <c r="P3" t="n">
-        <v>353.4559237991413</v>
+        <v>376.8352245987208</v>
       </c>
       <c r="Q3" t="n">
-        <v>110.179958506696</v>
+        <v>58.38061696871356</v>
       </c>
       <c r="R3" t="n">
-        <v>342.7963699780718</v>
+        <v>348.8860655823793</v>
       </c>
       <c r="S3" t="n">
-        <v>115.1591159711511</v>
+        <v>63.68217279004205</v>
       </c>
       <c r="T3" t="n">
-        <v>234.9824697521333</v>
+        <v>408.3616195085587</v>
       </c>
       <c r="U3" t="n">
-        <v>463.6358823058373</v>
+        <v>435.2158415674344</v>
       </c>
       <c r="V3" t="n">
-        <v>0.3363531305181555</v>
+        <v>0.4840831320785747</v>
       </c>
       <c r="W3" t="n">
-        <v>0.6636468694818445</v>
+        <v>0.5159168679214252</v>
       </c>
       <c r="X3" t="n">
-        <v>698.6183520579706</v>
+        <v>843.5774610759931</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.4833211090909091</v>
+        <v>0.7855354545454546</v>
       </c>
       <c r="Z3" t="n">
-        <v>1</v>
+        <v>0.8425447781093344</v>
       </c>
       <c r="AA3" t="n">
-        <v>46.25598473676393</v>
+        <v>42.63698965160264</v>
       </c>
       <c r="AB3" t="n">
         <v>18.2</v>
       </c>
       <c r="AC3" t="n">
-        <v>46.87727780592505</v>
+        <v>46.31410792301819</v>
       </c>
       <c r="AD3" t="n">
         <v>18.2</v>
@@ -774,88 +774,88 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>10918.61253982624</v>
+        <v>25322.70729049107</v>
       </c>
       <c r="C4" t="n">
-        <v>5709.225355142524</v>
+        <v>12842.96661759865</v>
       </c>
       <c r="D4" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E4" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F4" t="n">
-        <v>115.7625</v>
+        <v>104.7375</v>
       </c>
       <c r="G4" t="n">
-        <v>115.7625</v>
+        <v>104.7375</v>
       </c>
       <c r="H4" t="n">
-        <v>441.05599</v>
+        <v>476.8046</v>
       </c>
       <c r="I4" t="n">
-        <v>189.8168698651084</v>
+        <v>46.94010690297796</v>
       </c>
       <c r="J4" t="n">
-        <v>405.4692759088001</v>
+        <v>486.8486512889439</v>
       </c>
       <c r="K4" t="n">
-        <v>212.4185598809564</v>
+        <v>217.390187979185</v>
       </c>
       <c r="L4" t="n">
-        <v>348.8114478030581</v>
+        <v>418.7938689328366</v>
       </c>
       <c r="M4" t="n">
-        <v>125.0886848316272</v>
+        <v>83.69360905449918</v>
       </c>
       <c r="N4" t="n">
-        <v>215.496719001635</v>
+        <v>410.4880662605666</v>
       </c>
       <c r="O4" t="n">
-        <v>52.74240113325661</v>
+        <v>41.37642683645544</v>
       </c>
       <c r="P4" t="n">
-        <v>240.0356039751379</v>
+        <v>341.1191299112214</v>
       </c>
       <c r="Q4" t="n">
-        <v>72.69389348852722</v>
+        <v>105.6917302035243</v>
       </c>
       <c r="R4" t="n">
-        <v>255.7756508449141</v>
+        <v>356.5442358300962</v>
       </c>
       <c r="S4" t="n">
-        <v>69.3724064997074</v>
+        <v>107.6568122638346</v>
       </c>
       <c r="T4" t="n">
-        <v>268.2391201348916</v>
+        <v>451.864493097022</v>
       </c>
       <c r="U4" t="n">
-        <v>312.7294974636652</v>
+        <v>446.8108601147458</v>
       </c>
       <c r="V4" t="n">
-        <v>0.4617101716159168</v>
+        <v>0.5028117122408082</v>
       </c>
       <c r="W4" t="n">
-        <v>0.5382898283840831</v>
+        <v>0.4971882877591919</v>
       </c>
       <c r="X4" t="n">
-        <v>580.9686175985568</v>
+        <v>898.6753532117677</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8019199818181818</v>
+        <v>0.8669174545454545</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.7372168652887274</v>
+        <v>0.885179365979898</v>
       </c>
       <c r="AA4" t="n">
-        <v>47.36461721476797</v>
+        <v>41.46323631400617</v>
       </c>
       <c r="AB4" t="n">
         <v>18.21819999999999</v>
       </c>
       <c r="AC4" t="n">
-        <v>49.44462420808044</v>
+        <v>48.26981733541643</v>
       </c>
       <c r="AD4" t="n">
         <v>18.21819999999999</v>
@@ -866,88 +866,88 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>27838.56629176844</v>
+        <v>8916.651908028911</v>
       </c>
       <c r="C5" t="n">
-        <v>30279.10687866205</v>
+        <v>11430.68151926779</v>
       </c>
       <c r="D5" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E5" t="n">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F5" t="n">
-        <v>121.550625</v>
+        <v>109.974375</v>
       </c>
       <c r="G5" t="n">
-        <v>121.550625</v>
+        <v>109.974375</v>
       </c>
       <c r="H5" t="n">
-        <v>273.65286</v>
+        <v>331.04876</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>168.4511313251712</v>
       </c>
       <c r="J5" t="n">
-        <v>499.369591283113</v>
+        <v>343.6436667375286</v>
       </c>
       <c r="K5" t="n">
-        <v>169.2429028871031</v>
+        <v>208.2504509184436</v>
       </c>
       <c r="L5" t="n">
-        <v>365.0582114078035</v>
+        <v>295.2392794800062</v>
       </c>
       <c r="M5" t="n">
-        <v>81.41152253280774</v>
+        <v>65.7495863614502</v>
       </c>
       <c r="N5" t="n">
-        <v>273.6162274371555</v>
+        <v>156.3613472699782</v>
       </c>
       <c r="O5" t="n">
-        <v>94.94528244070065</v>
+        <v>23.23628140485065</v>
       </c>
       <c r="P5" t="n">
-        <v>417.7809195015354</v>
+        <v>304.832294121893</v>
       </c>
       <c r="Q5" t="n">
-        <v>124.7643287754309</v>
+        <v>47.95110967637712</v>
       </c>
       <c r="R5" t="n">
-        <v>376.9083803515171</v>
+        <v>315.7847527851116</v>
       </c>
       <c r="S5" t="n">
-        <v>134.8797708125523</v>
+        <v>45.24910193160209</v>
       </c>
       <c r="T5" t="n">
-        <v>290.65286</v>
+        <v>179.5976286748288</v>
       </c>
       <c r="U5" t="n">
-        <v>542.5452482769663</v>
+        <v>352.7834037982701</v>
       </c>
       <c r="V5" t="n">
-        <v>0.4045206630058025</v>
+        <v>0.3373479100871307</v>
       </c>
       <c r="W5" t="n">
-        <v>0.5954793369941975</v>
+        <v>0.6626520899128693</v>
       </c>
       <c r="X5" t="n">
-        <v>911.1067581548224</v>
+        <v>532.3810324730989</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.4975506545454545</v>
+        <v>0.6019068363636364</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.9079447114238419</v>
+        <v>0.6248066667955066</v>
       </c>
       <c r="AA5" t="n">
-        <v>46.96765861767919</v>
+        <v>42.57420434696233</v>
       </c>
       <c r="AB5" t="n">
         <v>18.23641819999999</v>
       </c>
       <c r="AC5" t="n">
-        <v>50.66205825509726</v>
+        <v>49.23682159667435</v>
       </c>
       <c r="AD5" t="n">
         <v>18.23641819999999</v>
@@ -958,10 +958,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>29967.87916114506</v>
+        <v>30814.88400066788</v>
       </c>
       <c r="C6" t="n">
-        <v>21926.7444354405</v>
+        <v>37307.80064994509</v>
       </c>
       <c r="D6" t="n">
         <v>120</v>
@@ -976,70 +976,70 @@
         <v>115.47309375</v>
       </c>
       <c r="H6" t="n">
-        <v>434.14251</v>
+        <v>369.30801</v>
       </c>
       <c r="I6" t="n">
-        <v>28.90795948721927</v>
+        <v>0</v>
       </c>
       <c r="J6" t="n">
         <v>550</v>
       </c>
       <c r="K6" t="n">
-        <v>198.4929186755003</v>
+        <v>120.7063028181639</v>
       </c>
       <c r="L6" t="n">
-        <v>328.5659771748254</v>
+        <v>428.448961551108</v>
       </c>
       <c r="M6" t="n">
-        <v>86.57653756514298</v>
+        <v>86.31017745266422</v>
       </c>
       <c r="N6" t="n">
-        <v>348.1335682624377</v>
+        <v>428.7591868215899</v>
       </c>
       <c r="O6" t="n">
-        <v>76.10098225034299</v>
+        <v>61.54843399851448</v>
       </c>
       <c r="P6" t="n">
-        <v>390.6978866068342</v>
+        <v>500.0425784327534</v>
       </c>
       <c r="Q6" t="n">
-        <v>130.0520976047686</v>
+        <v>137.5015696675262</v>
       </c>
       <c r="R6" t="n">
-        <v>397.0398995201982</v>
+        <v>512.9201567741785</v>
       </c>
       <c r="S6" t="n">
-        <v>140.9550555713583</v>
+        <v>143.9737767651787</v>
       </c>
       <c r="T6" t="n">
-        <v>424.2345505127807</v>
+        <v>392.30801</v>
       </c>
       <c r="U6" t="n">
-        <v>520.7499842116029</v>
+        <v>637.5441481002797</v>
       </c>
       <c r="V6" t="n">
-        <v>0.4489327972298658</v>
+        <v>0.4347270043202953</v>
       </c>
       <c r="W6" t="n">
-        <v>0.5510672027701342</v>
+        <v>0.5652729956797048</v>
       </c>
       <c r="X6" t="n">
-        <v>944.9845347243836</v>
+        <v>1127.851768920384</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.7893500181818182</v>
+        <v>0.6714691090909092</v>
       </c>
       <c r="Z6" t="n">
         <v>1</v>
       </c>
       <c r="AA6" t="n">
-        <v>48.10045204146028</v>
+        <v>44.03391412856743</v>
       </c>
       <c r="AB6" t="n">
         <v>18.25465461819999</v>
       </c>
       <c r="AC6" t="n">
-        <v>50.48876624431989</v>
+        <v>47.32713070501108</v>
       </c>
       <c r="AD6" t="n">
         <v>18.25465461819999</v>
@@ -1050,16 +1050,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>28369.87792530596</v>
+        <v>11004.2914012426</v>
       </c>
       <c r="C7" t="n">
-        <v>25519.95566755506</v>
+        <v>5389.751111758396</v>
       </c>
       <c r="D7" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E7" t="n">
-        <v>160</v>
+        <v>120</v>
       </c>
       <c r="F7" t="n">
         <v>121.2467484375</v>
@@ -1068,70 +1068,70 @@
         <v>121.2467484375</v>
       </c>
       <c r="H7" t="n">
-        <v>436.68227</v>
+        <v>532.04476</v>
       </c>
       <c r="I7" t="n">
-        <v>100.5242976136779</v>
+        <v>260.1490288362075</v>
       </c>
       <c r="J7" t="n">
-        <v>550</v>
+        <v>358.6453278208339</v>
       </c>
       <c r="K7" t="n">
-        <v>222.7531014509499</v>
+        <v>194.7765414514787</v>
       </c>
       <c r="L7" t="n">
-        <v>333.7567568280439</v>
+        <v>382.0614233352869</v>
       </c>
       <c r="M7" t="n">
-        <v>115.8334719975742</v>
+        <v>126.9833371793816</v>
       </c>
       <c r="N7" t="n">
-        <v>279.782594778259</v>
+        <v>230.2846373773471</v>
       </c>
       <c r="O7" t="n">
-        <v>72.3753776080631</v>
+        <v>64.61109378644538</v>
       </c>
       <c r="P7" t="n">
-        <v>430.3999538186617</v>
+        <v>220.9579886862253</v>
       </c>
       <c r="Q7" t="n">
-        <v>95.33986340588866</v>
+        <v>63.61710050129378</v>
       </c>
       <c r="R7" t="n">
-        <v>456.7577571550914</v>
+        <v>213.5780764052037</v>
       </c>
       <c r="S7" t="n">
-        <v>100.0736723999619</v>
+        <v>65.7735542337941</v>
       </c>
       <c r="T7" t="n">
-        <v>352.1579723863221</v>
+        <v>294.8957311637925</v>
       </c>
       <c r="U7" t="n">
-        <v>525.7398172245504</v>
+        <v>284.5750891875191</v>
       </c>
       <c r="V7" t="n">
-        <v>0.4011377822723712</v>
+        <v>0.5089052300942577</v>
       </c>
       <c r="W7" t="n">
-        <v>0.5988622177276288</v>
+        <v>0.4910947699057422</v>
       </c>
       <c r="X7" t="n">
-        <v>877.8977896108725</v>
+        <v>579.4708203513117</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.7939677636363637</v>
+        <v>0.9673541090909091</v>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>0.652082414219698</v>
       </c>
       <c r="AA7" t="n">
-        <v>47.47431035739504</v>
+        <v>44.85129837711415</v>
       </c>
       <c r="AB7" t="n">
         <v>18.27290927281819</v>
       </c>
       <c r="AC7" t="n">
-        <v>50.41578434926424</v>
+        <v>52.06926873704028</v>
       </c>
       <c r="AD7" t="n">
         <v>18.27290927281819</v>
@@ -1142,88 +1142,88 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>22019.22838426387</v>
+        <v>28193.19606571367</v>
       </c>
       <c r="C8" t="n">
-        <v>17509.73523690392</v>
+        <v>26238.0474522385</v>
       </c>
       <c r="D8" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E8" t="n">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F8" t="n">
-        <v>115.184411015625</v>
+        <v>127.3090858593751</v>
       </c>
       <c r="G8" t="n">
-        <v>115.184411015625</v>
+        <v>127.3090858593751</v>
       </c>
       <c r="H8" t="n">
-        <v>459.00749</v>
+        <v>265.78845</v>
       </c>
       <c r="I8" t="n">
-        <v>119.8133477167801</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>432.5274601780798</v>
+        <v>477.164018952656</v>
       </c>
       <c r="K8" t="n">
-        <v>233.4937099682066</v>
+        <v>186.1480004148531</v>
       </c>
       <c r="L8" t="n">
-        <v>418.6636074521576</v>
+        <v>382.7784761141201</v>
       </c>
       <c r="M8" t="n">
-        <v>116.8681814326885</v>
+        <v>119.1590043016204</v>
       </c>
       <c r="N8" t="n">
-        <v>319.482049352196</v>
+        <v>255.767649388604</v>
       </c>
       <c r="O8" t="n">
-        <v>43.71209293102388</v>
+        <v>66.87663830632987</v>
       </c>
       <c r="P8" t="n">
-        <v>361.2448160251992</v>
+        <v>373.9349461488908</v>
       </c>
       <c r="Q8" t="n">
-        <v>60.54203563562387</v>
+        <v>111.8576138403907</v>
       </c>
       <c r="R8" t="n">
-        <v>392.0553447389427</v>
+        <v>371.0599454023582</v>
       </c>
       <c r="S8" t="n">
-        <v>63.22521689008691</v>
+        <v>100.8806150017765</v>
       </c>
       <c r="T8" t="n">
-        <v>363.1941422832199</v>
+        <v>289.78845</v>
       </c>
       <c r="U8" t="n">
-        <v>421.786851660823</v>
+        <v>485.7925599892816</v>
       </c>
       <c r="V8" t="n">
-        <v>0.4626788993430204</v>
+        <v>0.3990964645156332</v>
       </c>
       <c r="W8" t="n">
-        <v>0.5373211006569797</v>
+        <v>0.6009035354843668</v>
       </c>
       <c r="X8" t="n">
-        <v>784.9809939440429</v>
+        <v>808.4368476842154</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.8345590727272728</v>
+        <v>0.4832517272727273</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.7864135639601451</v>
+        <v>0.8675709435502835</v>
       </c>
       <c r="AA8" t="n">
-        <v>46.45772118944935</v>
+        <v>46.56781336542775</v>
       </c>
       <c r="AB8" t="n">
         <v>18.291182182091</v>
       </c>
       <c r="AC8" t="n">
-        <v>47.50310469822417</v>
+        <v>52.76029221893338</v>
       </c>
       <c r="AD8" t="n">
         <v>18.291182182091</v>
@@ -1234,16 +1234,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>41918.58162653436</v>
+        <v>29608.0165144758</v>
       </c>
       <c r="C9" t="n">
-        <v>40644.64042143602</v>
+        <v>27576.43845553474</v>
       </c>
       <c r="D9" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E9" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F9" t="n">
         <v>120.9436315664063</v>
@@ -1252,70 +1252,70 @@
         <v>120.9436315664063</v>
       </c>
       <c r="H9" t="n">
-        <v>437.6083</v>
+        <v>549.03409</v>
       </c>
       <c r="I9" t="n">
-        <v>8.042744050732722</v>
+        <v>101.9789013657778</v>
       </c>
       <c r="J9" t="n">
-        <v>550</v>
+        <v>511.3856329398774</v>
       </c>
       <c r="K9" t="n">
-        <v>139.0746300573609</v>
+        <v>168.9269837990555</v>
       </c>
       <c r="L9" t="n">
-        <v>388.2162802304384</v>
+        <v>435.0043994573223</v>
       </c>
       <c r="M9" t="n">
-        <v>150.2053633923694</v>
+        <v>89.02968660533621</v>
       </c>
       <c r="N9" t="n">
-        <v>357.4730139523981</v>
+        <v>386.63630407365</v>
       </c>
       <c r="O9" t="n">
-        <v>91.09254199686919</v>
+        <v>85.41888456057215</v>
       </c>
       <c r="P9" t="n">
-        <v>554.0372604151671</v>
+        <v>374.7103287484329</v>
       </c>
       <c r="Q9" t="n">
-        <v>90.38181949567866</v>
+        <v>153.8963208072421</v>
       </c>
       <c r="R9" t="n">
-        <v>548.7426521898858</v>
+        <v>355.5506357812835</v>
       </c>
       <c r="S9" t="n">
-        <v>85.40367605907485</v>
+        <v>141.9829975734469</v>
       </c>
       <c r="T9" t="n">
-        <v>448.5655559492673</v>
+        <v>472.0551886342222</v>
       </c>
       <c r="U9" t="n">
-        <v>644.4190799108458</v>
+        <v>528.6066495556749</v>
       </c>
       <c r="V9" t="n">
-        <v>0.4104042648287304</v>
+        <v>0.4717429711201194</v>
       </c>
       <c r="W9" t="n">
-        <v>0.5895957351712696</v>
+        <v>0.5282570288798807</v>
       </c>
       <c r="X9" t="n">
-        <v>1092.984635860113</v>
+        <v>1000.661838189897</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.7956514545454545</v>
+        <v>0.9982438</v>
       </c>
       <c r="Z9" t="n">
-        <v>1</v>
+        <v>0.9297920598906861</v>
       </c>
       <c r="AA9" t="n">
-        <v>47.67850773913931</v>
+        <v>48.87610588788633</v>
       </c>
       <c r="AB9" t="n">
         <v>18.30947336427309</v>
       </c>
       <c r="AC9" t="n">
-        <v>48.99160680581618</v>
+        <v>50.73882295981808</v>
       </c>
       <c r="AD9" t="n">
         <v>18.30947336427309</v>
@@ -1326,88 +1326,88 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>23117.72045439906</v>
+        <v>6694.30867306047</v>
       </c>
       <c r="C10" t="n">
-        <v>17437.7523986655</v>
+        <v>9197.314443436866</v>
       </c>
       <c r="D10" t="n">
         <v>120</v>
       </c>
       <c r="E10" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F10" t="n">
-        <v>114.8964499880859</v>
+        <v>114.896449988086</v>
       </c>
       <c r="G10" t="n">
-        <v>114.8964499880859</v>
+        <v>114.896449988086</v>
       </c>
       <c r="H10" t="n">
-        <v>522.00622</v>
+        <v>473.56287</v>
       </c>
       <c r="I10" t="n">
-        <v>146.5063169367691</v>
+        <v>233.5255713919689</v>
       </c>
       <c r="J10" t="n">
-        <v>526.9305193509706</v>
+        <v>376.9243454402647</v>
       </c>
       <c r="K10" t="n">
-        <v>204.0577753508649</v>
+        <v>210.9829944423477</v>
       </c>
       <c r="L10" t="n">
-        <v>399.5696940363122</v>
+        <v>465.3871663633701</v>
       </c>
       <c r="M10" t="n">
-        <v>110.4792722270115</v>
+        <v>93.15460533518568</v>
       </c>
       <c r="N10" t="n">
-        <v>349.8326979804371</v>
+        <v>229.6397867606142</v>
       </c>
       <c r="O10" t="n">
-        <v>45.66720508279375</v>
+        <v>27.39751184741687</v>
       </c>
       <c r="P10" t="n">
-        <v>398.5431928658645</v>
+        <v>273.23340650222</v>
       </c>
       <c r="Q10" t="n">
-        <v>63.40418119160216</v>
+        <v>61.63492829475249</v>
       </c>
       <c r="R10" t="n">
-        <v>399.5361756560255</v>
+        <v>282.9124616535498</v>
       </c>
       <c r="S10" t="n">
-        <v>66.46897375230596</v>
+        <v>62.93886758577036</v>
       </c>
       <c r="T10" t="n">
-        <v>395.4999030632309</v>
+        <v>257.0372986080311</v>
       </c>
       <c r="U10" t="n">
-        <v>461.9473740574666</v>
+        <v>334.8683347969725</v>
       </c>
       <c r="V10" t="n">
-        <v>0.4612527366012719</v>
+        <v>0.4342538474070523</v>
       </c>
       <c r="W10" t="n">
-        <v>0.5387472633987281</v>
+        <v>0.5657461525929477</v>
       </c>
       <c r="X10" t="n">
-        <v>857.4472771206974</v>
+        <v>591.9056334050035</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.9491022181818182</v>
+        <v>0.8610234</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.9580554897290374</v>
+        <v>0.6853169917095722</v>
       </c>
       <c r="AA10" t="n">
-        <v>46.07082130039582</v>
+        <v>50.01050022591366</v>
       </c>
       <c r="AB10" t="n">
         <v>18.32778283763736</v>
       </c>
       <c r="AC10" t="n">
-        <v>47.72918615803693</v>
+        <v>49.81270675589048</v>
       </c>
       <c r="AD10" t="n">
         <v>18.32778283763736</v>
@@ -1418,88 +1418,88 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>32158.81255032499</v>
+        <v>23418.21892574612</v>
       </c>
       <c r="C11" t="n">
-        <v>32547.21631087163</v>
+        <v>29096.37476075658</v>
       </c>
       <c r="D11" t="n">
         <v>120</v>
       </c>
       <c r="E11" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="F11" t="n">
-        <v>120.6412724874902</v>
+        <v>120.6412724874903</v>
       </c>
       <c r="G11" t="n">
-        <v>120.6412724874902</v>
+        <v>120.6412724874903</v>
       </c>
       <c r="H11" t="n">
-        <v>403.19585</v>
+        <v>295.37939</v>
       </c>
       <c r="I11" t="n">
         <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>531.586289945841</v>
+        <v>550</v>
       </c>
       <c r="K11" t="n">
-        <v>161.0983872933182</v>
+        <v>209.086061456265</v>
       </c>
       <c r="L11" t="n">
-        <v>424.3098138570484</v>
+        <v>372.8828202609234</v>
       </c>
       <c r="M11" t="n">
-        <v>107.3923548662012</v>
+        <v>138.0221364886003</v>
       </c>
       <c r="N11" t="n">
-        <v>428.3596246532309</v>
+        <v>417.8301914009173</v>
       </c>
       <c r="O11" t="n">
-        <v>93.25255804532502</v>
+        <v>114.3410242193857</v>
       </c>
       <c r="P11" t="n">
-        <v>421.565008746662</v>
+        <v>409.0168375773614</v>
       </c>
       <c r="Q11" t="n">
-        <v>152.9806692567257</v>
+        <v>142.8800954087213</v>
       </c>
       <c r="R11" t="n">
-        <v>384.035825856692</v>
+        <v>445.7339482600489</v>
       </c>
       <c r="S11" t="n">
-        <v>151.6082394400139</v>
+        <v>129.4899964389384</v>
       </c>
       <c r="T11" t="n">
-        <v>421.19585</v>
+        <v>313.37939</v>
       </c>
       <c r="U11" t="n">
-        <v>574.5456780033877</v>
+        <v>551.8969329860827</v>
       </c>
       <c r="V11" t="n">
-        <v>0.4758549853070729</v>
+        <v>0.4909019938501385</v>
       </c>
       <c r="W11" t="n">
-        <v>0.524145014692927</v>
+        <v>0.5090980061498614</v>
       </c>
       <c r="X11" t="n">
-        <v>1096.157860701944</v>
+        <v>1084.068148606386</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.7330833636363636</v>
+        <v>0.5370534363636363</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.9665205271742564</v>
+        <v>1</v>
       </c>
       <c r="AA11" t="n">
-        <v>45.59741735852441</v>
+        <v>48.03079820245372</v>
       </c>
       <c r="AB11" t="n">
         <v>18.346110620475</v>
       </c>
       <c r="AC11" t="n">
-        <v>49.57642487823007</v>
+        <v>49.04843736809783</v>
       </c>
       <c r="AD11" t="n">
         <v>18.346110620475</v>
@@ -1510,88 +1510,88 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>16470.79393406543</v>
+        <v>22585.18164498634</v>
       </c>
       <c r="C12" t="n">
-        <v>18559.48215997264</v>
+        <v>20920.61684259318</v>
       </c>
       <c r="D12" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E12" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F12" t="n">
-        <v>126.6733361118648</v>
+        <v>114.6092088631158</v>
       </c>
       <c r="G12" t="n">
-        <v>126.6733361118648</v>
+        <v>114.6092088631158</v>
       </c>
       <c r="H12" t="n">
-        <v>548.25229</v>
+        <v>538.49733</v>
       </c>
       <c r="I12" t="n">
-        <v>258.228888806283</v>
+        <v>163.7976306228127</v>
       </c>
       <c r="J12" t="n">
-        <v>397.4275281705242</v>
+        <v>531.1230447400209</v>
       </c>
       <c r="K12" t="n">
-        <v>169.1489643909122</v>
+        <v>227.5635873602704</v>
       </c>
       <c r="L12" t="n">
-        <v>431.2226543568743</v>
+        <v>410.9122157706648</v>
       </c>
       <c r="M12" t="n">
-        <v>101.0296348459306</v>
+        <v>102.585112339714</v>
       </c>
       <c r="N12" t="n">
-        <v>247.2477018780814</v>
+        <v>356.327550424595</v>
       </c>
       <c r="O12" t="n">
-        <v>58.7756993156356</v>
+        <v>43.37214895259229</v>
       </c>
       <c r="P12" t="n">
-        <v>333.6969060374506</v>
+        <v>428.2351122410087</v>
       </c>
       <c r="Q12" t="n">
-        <v>55.68004503547959</v>
+        <v>84.41040659500683</v>
       </c>
       <c r="R12" t="n">
-        <v>300.6663943003705</v>
+        <v>452.2789595740317</v>
       </c>
       <c r="S12" t="n">
-        <v>57.85952116347181</v>
+        <v>87.93014662225424</v>
       </c>
       <c r="T12" t="n">
-        <v>306.023401193717</v>
+        <v>399.6996993771873</v>
       </c>
       <c r="U12" t="n">
-        <v>389.3769510729301</v>
+        <v>512.6455188360155</v>
       </c>
       <c r="V12" t="n">
-        <v>0.4400679410015227</v>
+        <v>0.4381013802647923</v>
       </c>
       <c r="W12" t="n">
-        <v>0.5599320589984772</v>
+        <v>0.5618986197352077</v>
       </c>
       <c r="X12" t="n">
-        <v>695.4003522666471</v>
+        <v>912.3452182132028</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9968223454545455</v>
+        <v>0.9790860545454546</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.7225955057645894</v>
+        <v>0.9656782631636743</v>
       </c>
       <c r="AA12" t="n">
-        <v>47.16081433137722</v>
+        <v>46.5205408149944</v>
       </c>
       <c r="AB12" t="n">
         <v>18.36445673109547</v>
       </c>
       <c r="AC12" t="n">
-        <v>51.14252200943762</v>
+        <v>51.35853620313758</v>
       </c>
       <c r="AD12" t="n">
         <v>18.36445673109547</v>
@@ -1602,88 +1602,88 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>29868.49736513371</v>
+        <v>32828.40881212088</v>
       </c>
       <c r="C13" t="n">
-        <v>35440.58702632471</v>
+        <v>34383.79959164998</v>
       </c>
       <c r="D13" t="n">
         <v>140</v>
       </c>
       <c r="E13" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F13" t="n">
-        <v>133.007002917458</v>
+        <v>120.3396693062716</v>
       </c>
       <c r="G13" t="n">
-        <v>133.007002917458</v>
+        <v>120.3396693062716</v>
       </c>
       <c r="H13" t="n">
-        <v>299.00769</v>
+        <v>383.01665</v>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>49.91369772353517</v>
       </c>
       <c r="J13" t="n">
         <v>550</v>
       </c>
       <c r="K13" t="n">
-        <v>167.3641676982294</v>
+        <v>170.8302417871137</v>
       </c>
       <c r="L13" t="n">
-        <v>358.1650106880967</v>
+        <v>352.1814714682206</v>
       </c>
       <c r="M13" t="n">
-        <v>182.0715702850353</v>
+        <v>170.6328049625219</v>
       </c>
       <c r="N13" t="n">
-        <v>387.9371388587863</v>
+        <v>276.0263727449985</v>
       </c>
       <c r="O13" t="n">
-        <v>110.164902624466</v>
+        <v>81.07657953146638</v>
       </c>
       <c r="P13" t="n">
-        <v>452.3841075614</v>
+        <v>505.0413972423634</v>
       </c>
       <c r="Q13" t="n">
-        <v>99.40068913128276</v>
+        <v>101.6919483307933</v>
       </c>
       <c r="R13" t="n">
-        <v>427.9512586383945</v>
+        <v>522.9138812971395</v>
       </c>
       <c r="S13" t="n">
-        <v>93.69717110559675</v>
+        <v>108.5644605299877</v>
       </c>
       <c r="T13" t="n">
-        <v>316.00769</v>
+        <v>357.1029522764649</v>
       </c>
       <c r="U13" t="n">
-        <v>551.7847966926828</v>
+        <v>606.7333455731567</v>
       </c>
       <c r="V13" t="n">
-        <v>0.474434027907856</v>
+        <v>0.3705016641033168</v>
       </c>
       <c r="W13" t="n">
-        <v>0.525565972092144</v>
+        <v>0.6294983358966832</v>
       </c>
       <c r="X13" t="n">
-        <v>1049.886838175935</v>
+        <v>963.8362978496216</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.5436503454545455</v>
+        <v>0.6963939090909091</v>
       </c>
       <c r="Z13" t="n">
         <v>1</v>
       </c>
       <c r="AA13" t="n">
-        <v>48.06759061904492</v>
+        <v>44.55727214766546</v>
       </c>
       <c r="AB13" t="n">
         <v>18.38282118782656</v>
       </c>
       <c r="AC13" t="n">
-        <v>50.00977281543064</v>
+        <v>51.23286988151392</v>
       </c>
       <c r="AD13" t="n">
         <v>18.38282118782656</v>
@@ -1694,88 +1694,88 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>38388.80730359554</v>
+        <v>16513.80037270651</v>
       </c>
       <c r="C14" t="n">
-        <v>30432.85924208136</v>
+        <v>15477.982626571</v>
       </c>
       <c r="D14" t="n">
+        <v>130</v>
+      </c>
+      <c r="E14" t="n">
         <v>140</v>
       </c>
-      <c r="E14" t="n">
-        <v>160</v>
-      </c>
       <c r="F14" t="n">
-        <v>139.6573530633309</v>
+        <v>126.3566527715851</v>
       </c>
       <c r="G14" t="n">
-        <v>139.6573530633309</v>
+        <v>126.3566527715851</v>
       </c>
       <c r="H14" t="n">
-        <v>538.2058</v>
+        <v>494.83345</v>
       </c>
       <c r="I14" t="n">
-        <v>98.84903118169768</v>
+        <v>204.9354677848784</v>
       </c>
       <c r="J14" t="n">
-        <v>523.37618094684</v>
+        <v>352.8930298840216</v>
       </c>
       <c r="K14" t="n">
-        <v>212.3622319580755</v>
+        <v>175.081053299742</v>
       </c>
       <c r="L14" t="n">
-        <v>405.9892648968214</v>
+        <v>448.295024694162</v>
       </c>
       <c r="M14" t="n">
-        <v>107.2165360205653</v>
+        <v>77.45212380767674</v>
       </c>
       <c r="N14" t="n">
-        <v>387.6047299043925</v>
+        <v>253.10225825374</v>
       </c>
       <c r="O14" t="n">
-        <v>76.75203891390981</v>
+        <v>55.79572396138168</v>
       </c>
       <c r="P14" t="n">
-        <v>390.4646786498146</v>
+        <v>283.5787300671023</v>
       </c>
       <c r="Q14" t="n">
-        <v>87.91343803717925</v>
+        <v>65.06348830429103</v>
       </c>
       <c r="R14" t="n">
-        <v>402.8586347618499</v>
+        <v>257.6223309888761</v>
       </c>
       <c r="S14" t="n">
-        <v>87.88171388321956</v>
+        <v>66.10094068225931</v>
       </c>
       <c r="T14" t="n">
-        <v>464.3567688183023</v>
+        <v>308.8979822151217</v>
       </c>
       <c r="U14" t="n">
-        <v>478.3781166869938</v>
+        <v>348.6422183713933</v>
       </c>
       <c r="V14" t="n">
-        <v>0.4925634724649145</v>
+        <v>0.4697780940839659</v>
       </c>
       <c r="W14" t="n">
-        <v>0.5074365275350855</v>
+        <v>0.530221905916034</v>
       </c>
       <c r="X14" t="n">
-        <v>942.7348855052961</v>
+        <v>657.540200586515</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.9785559999999999</v>
+        <v>0.8996971818181819</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.9515930562669819</v>
+        <v>0.6416236906982211</v>
       </c>
       <c r="AA14" t="n">
-        <v>49.09542459149156</v>
+        <v>46.95128508327306</v>
       </c>
       <c r="AB14" t="n">
         <v>18.40120400901439</v>
       </c>
       <c r="AC14" t="n">
-        <v>49.35412915093104</v>
+        <v>51.30295941546635</v>
       </c>
       <c r="AD14" t="n">
         <v>18.40120400901439</v>
@@ -1786,88 +1786,88 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>37115.12953782582</v>
+        <v>28713.48182528131</v>
       </c>
       <c r="C15" t="n">
-        <v>28078.02012690582</v>
+        <v>39248.32898243965</v>
       </c>
       <c r="D15" t="n">
         <v>140</v>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F15" t="n">
-        <v>146.6402207164975</v>
+        <v>132.6744854101644</v>
       </c>
       <c r="G15" t="n">
-        <v>146.6402207164975</v>
+        <v>132.6744854101644</v>
       </c>
       <c r="H15" t="n">
-        <v>536.58134</v>
+        <v>289.23733</v>
       </c>
       <c r="I15" t="n">
-        <v>96.25129788401745</v>
+        <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>399.0559614719149</v>
+        <v>550</v>
       </c>
       <c r="K15" t="n">
-        <v>211.346293737602</v>
+        <v>139.9400181232714</v>
       </c>
       <c r="L15" t="n">
-        <v>474.5349387943427</v>
+        <v>370.8672816538979</v>
       </c>
       <c r="M15" t="n">
-        <v>136.8954370846651</v>
+        <v>108.3055132422788</v>
       </c>
       <c r="N15" t="n">
-        <v>386.3750923616626</v>
+        <v>381.6735785158091</v>
       </c>
       <c r="O15" t="n">
-        <v>77.95494975431997</v>
+        <v>71.09546708543115</v>
       </c>
       <c r="P15" t="n">
-        <v>336.2363895734441</v>
+        <v>473.1862609171917</v>
       </c>
       <c r="Q15" t="n">
-        <v>63.83551011894436</v>
+        <v>111.9547742592789</v>
       </c>
       <c r="R15" t="n">
-        <v>348.8928562351055</v>
+        <v>514.3993186458754</v>
       </c>
       <c r="S15" t="n">
-        <v>62.52533719488495</v>
+        <v>104.9180376631156</v>
       </c>
       <c r="T15" t="n">
-        <v>464.3300421159825</v>
+        <v>304.23733</v>
       </c>
       <c r="U15" t="n">
-        <v>400.0718996923885</v>
+        <v>585.1410351764706</v>
       </c>
       <c r="V15" t="n">
-        <v>0.5371691335451901</v>
+        <v>0.43623147514087</v>
       </c>
       <c r="W15" t="n">
-        <v>0.4628308664548098</v>
+        <v>0.5637685248591301</v>
       </c>
       <c r="X15" t="n">
-        <v>864.401941808371</v>
+        <v>1037.910080777711</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.9756024363636363</v>
+        <v>0.5258860545454546</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.7255562935852998</v>
+        <v>1</v>
       </c>
       <c r="AA15" t="n">
-        <v>51.6204565791343</v>
+        <v>47.98738936885736</v>
       </c>
       <c r="AB15" t="n">
         <v>18.4196052130234</v>
       </c>
       <c r="AC15" t="n">
-        <v>50.20633200896671</v>
+        <v>50.86235245192742</v>
       </c>
       <c r="AD15" t="n">
         <v>18.4196052130234</v>
@@ -1878,88 +1878,88 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>33224.40119006937</v>
+        <v>22784.85985374062</v>
       </c>
       <c r="C16" t="n">
-        <v>31570.17431336597</v>
+        <v>17203.66725954727</v>
       </c>
       <c r="D16" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E16" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F16" t="n">
-        <v>139.3082096806726</v>
+        <v>126.0407611396562</v>
       </c>
       <c r="G16" t="n">
-        <v>139.3082096806726</v>
+        <v>126.0407611396562</v>
       </c>
       <c r="H16" t="n">
-        <v>491.16136</v>
+        <v>542.18412</v>
       </c>
       <c r="I16" t="n">
-        <v>82.50804286840025</v>
+        <v>149.4757316292862</v>
       </c>
       <c r="J16" t="n">
-        <v>410.7572961552393</v>
+        <v>436.4688214816807</v>
       </c>
       <c r="K16" t="n">
-        <v>172.4621942926192</v>
+        <v>184.6912978853018</v>
       </c>
       <c r="L16" t="n">
-        <v>441.218681007732</v>
+        <v>463.822811230769</v>
       </c>
       <c r="M16" t="n">
-        <v>124.1939750460987</v>
+        <v>56.36131020211157</v>
       </c>
       <c r="N16" t="n">
-        <v>336.5814568780494</v>
+        <v>370.5165616882077</v>
       </c>
       <c r="O16" t="n">
-        <v>94.0718602535504</v>
+        <v>44.19182668250605</v>
       </c>
       <c r="P16" t="n">
-        <v>341.6206754090986</v>
+        <v>304.4427855260178</v>
       </c>
       <c r="Q16" t="n">
-        <v>108.0207201911235</v>
+        <v>87.27475619363256</v>
       </c>
       <c r="R16" t="n">
-        <v>314.388098251263</v>
+        <v>293.3339471438191</v>
       </c>
       <c r="S16" t="n">
-        <v>107.7154916415781</v>
+        <v>83.07489246113305</v>
       </c>
       <c r="T16" t="n">
-        <v>430.6533171315998</v>
+        <v>414.7083883707138</v>
       </c>
       <c r="U16" t="n">
-        <v>449.641395600222</v>
+        <v>391.7175417196504</v>
       </c>
       <c r="V16" t="n">
-        <v>0.4892149309805028</v>
+        <v>0.5142547788911545</v>
       </c>
       <c r="W16" t="n">
-        <v>0.5107850690194972</v>
+        <v>0.4857452211088455</v>
       </c>
       <c r="X16" t="n">
-        <v>880.2947127318218</v>
+        <v>806.4259300903642</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.8930206545454545</v>
+        <v>0.9857893090909091</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.7468314475549804</v>
+        <v>0.7935796754212376</v>
       </c>
       <c r="AA16" t="n">
-        <v>54.77231988000401</v>
+        <v>49.21058050812418</v>
       </c>
       <c r="AB16" t="n">
         <v>18.43802481823642</v>
       </c>
       <c r="AC16" t="n">
-        <v>50.10921451685141</v>
+        <v>49.62190318939171</v>
       </c>
       <c r="AD16" t="n">
         <v>18.43802481823642</v>
@@ -1970,88 +1970,88 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>31600.28867398621</v>
+        <v>10757.80626807409</v>
       </c>
       <c r="C17" t="n">
-        <v>22754.56797439734</v>
+        <v>9912.28490087208</v>
       </c>
       <c r="D17" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E17" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F17" t="n">
-        <v>146.2736201647062</v>
+        <v>132.342799196639</v>
       </c>
       <c r="G17" t="n">
-        <v>146.2736201647062</v>
+        <v>132.342799196639</v>
       </c>
       <c r="H17" t="n">
-        <v>342.81635</v>
+        <v>479.43376</v>
       </c>
       <c r="I17" t="n">
-        <v>1.197404616386393</v>
+        <v>243.6376011029619</v>
       </c>
       <c r="J17" t="n">
-        <v>367.4820521104208</v>
+        <v>261.0426980812229</v>
       </c>
       <c r="K17" t="n">
-        <v>191.9949343012536</v>
+        <v>192.2078285431573</v>
       </c>
       <c r="L17" t="n">
-        <v>346.881774276726</v>
+        <v>523.671682417233</v>
       </c>
       <c r="M17" t="n">
-        <v>61.44261740118136</v>
+        <v>84.2378068246197</v>
       </c>
       <c r="N17" t="n">
-        <v>289.8060488378497</v>
+        <v>220.4458348052187</v>
       </c>
       <c r="O17" t="n">
-        <v>68.81289654576385</v>
+        <v>36.35032409181945</v>
       </c>
       <c r="P17" t="n">
-        <v>254.0988310735904</v>
+        <v>205.2460778485716</v>
       </c>
       <c r="Q17" t="n">
-        <v>93.85048102819594</v>
+        <v>48.2800895747958</v>
       </c>
       <c r="R17" t="n">
-        <v>251.9063974922246</v>
+        <v>201.1700617877852</v>
       </c>
       <c r="S17" t="n">
-        <v>88.03784891081534</v>
+        <v>44.56393417873937</v>
       </c>
       <c r="T17" t="n">
-        <v>358.6189453836136</v>
+        <v>256.7961588970381</v>
       </c>
       <c r="U17" t="n">
-        <v>347.9493121017864</v>
+        <v>253.5261674233674</v>
       </c>
       <c r="V17" t="n">
-        <v>0.5075503202760617</v>
+        <v>0.503203849121445</v>
       </c>
       <c r="W17" t="n">
-        <v>0.4924496797239383</v>
+        <v>0.496796150878555</v>
       </c>
       <c r="X17" t="n">
-        <v>706.5682574854</v>
+        <v>510.3223263204055</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.6233024545454545</v>
+        <v>0.8716977454545455</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.6681491856553106</v>
+        <v>0.4746230874204052</v>
       </c>
       <c r="AA17" t="n">
-        <v>54.26803263755337</v>
+        <v>46.17617913752036</v>
       </c>
       <c r="AB17" t="n">
         <v>18.45646284305466</v>
       </c>
       <c r="AC17" t="n">
-        <v>47.91034829362857</v>
+        <v>50.20101171605364</v>
       </c>
       <c r="AD17" t="n">
         <v>18.45646284305466</v>
@@ -2062,88 +2062,88 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>37683.20054259532</v>
+        <v>35132.13669510306</v>
       </c>
       <c r="C18" t="n">
-        <v>32650.7259217639</v>
+        <v>23291.29106637952</v>
       </c>
       <c r="D18" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E18" t="n">
         <v>120</v>
       </c>
       <c r="F18" t="n">
-        <v>138.9599391564709</v>
+        <v>125.725659236807</v>
       </c>
       <c r="G18" t="n">
-        <v>138.9599391564709</v>
+        <v>125.725659236807</v>
       </c>
       <c r="H18" t="n">
-        <v>547.6462299999999</v>
+        <v>450.90988</v>
       </c>
       <c r="I18" t="n">
-        <v>93.9470210282206</v>
+        <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>451.9952019673597</v>
+        <v>518.6518057944627</v>
       </c>
       <c r="K18" t="n">
-        <v>181.7967420349935</v>
+        <v>230.082804199417</v>
       </c>
       <c r="L18" t="n">
-        <v>410.2667432170369</v>
+        <v>482.3806104475413</v>
       </c>
       <c r="M18" t="n">
-        <v>118.5768925887393</v>
+        <v>192.1668720477867</v>
       </c>
       <c r="N18" t="n">
-        <v>333.7954258713348</v>
+        <v>425.8442837913082</v>
       </c>
       <c r="O18" t="n">
-        <v>139.9037831004446</v>
+        <v>136.5748143266045</v>
       </c>
       <c r="P18" t="n">
-        <v>341.3466124565545</v>
+        <v>353.4229733655945</v>
       </c>
       <c r="Q18" t="n">
-        <v>120.8467817770652</v>
+        <v>127.3538567726084</v>
       </c>
       <c r="R18" t="n">
-        <v>311.182754123581</v>
+        <v>381.0365079455416</v>
       </c>
       <c r="S18" t="n">
-        <v>132.8073821450322</v>
+        <v>129.8231263920783</v>
       </c>
       <c r="T18" t="n">
-        <v>473.6992089717793</v>
+        <v>470.90988</v>
       </c>
       <c r="U18" t="n">
-        <v>462.1933942336198</v>
+        <v>480.7768301382029</v>
       </c>
       <c r="V18" t="n">
-        <v>0.5061469738615053</v>
+        <v>0.5391308409898555</v>
       </c>
       <c r="W18" t="n">
-        <v>0.4938530261384946</v>
+        <v>0.4608691590101444</v>
       </c>
       <c r="X18" t="n">
-        <v>935.8926032053992</v>
+        <v>1043.195928256116</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.9957204181818181</v>
+        <v>0.8198361454545454</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.8218094581224721</v>
+        <v>0.9430032832626595</v>
       </c>
       <c r="AA18" t="n">
-        <v>51.94374235242586</v>
+        <v>47.4086948480635</v>
       </c>
       <c r="AB18" t="n">
         <v>18.47491930589771</v>
       </c>
       <c r="AC18" t="n">
-        <v>46.57315127577198</v>
+        <v>51.15825554919748</v>
       </c>
       <c r="AD18" t="n">
         <v>18.47491930589771</v>
@@ -2154,88 +2154,88 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>35693.97848181438</v>
+        <v>40615.95660353129</v>
       </c>
       <c r="C19" t="n">
-        <v>26752.26675535211</v>
+        <v>35962.40833447084</v>
       </c>
       <c r="D19" t="n">
         <v>140</v>
       </c>
       <c r="E19" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F19" t="n">
-        <v>145.9079361142945</v>
+        <v>132.0119421986474</v>
       </c>
       <c r="G19" t="n">
-        <v>145.9079361142945</v>
+        <v>132.0119421986474</v>
       </c>
       <c r="H19" t="n">
-        <v>446.07036</v>
+        <v>424.68498</v>
       </c>
       <c r="I19" t="n">
-        <v>41.1369527970748</v>
+        <v>5.87049032480553</v>
       </c>
       <c r="J19" t="n">
-        <v>416.3728236462944</v>
+        <v>550</v>
       </c>
       <c r="K19" t="n">
-        <v>211.4777629823517</v>
+        <v>203.4850018210881</v>
       </c>
       <c r="L19" t="n">
-        <v>411.0961519635019</v>
+        <v>319.6143007251212</v>
       </c>
       <c r="M19" t="n">
-        <v>113.9212274609715</v>
+        <v>90.07068425270036</v>
       </c>
       <c r="N19" t="n">
-        <v>346.1486407262311</v>
+        <v>386.0085935553702</v>
       </c>
       <c r="O19" t="n">
-        <v>73.78476647669416</v>
+        <v>47.80589611982424</v>
       </c>
       <c r="P19" t="n">
-        <v>305.7860438772229</v>
+        <v>488.2327281288533</v>
       </c>
       <c r="Q19" t="n">
-        <v>80.90575882171325</v>
+        <v>88.36507424947567</v>
       </c>
       <c r="R19" t="n">
-        <v>312.8199159754594</v>
+        <v>521.85388522094</v>
       </c>
       <c r="S19" t="n">
-        <v>85.3496497058285</v>
+        <v>95.71364784473111</v>
       </c>
       <c r="T19" t="n">
-        <v>419.9334072029252</v>
+        <v>433.8144896751945</v>
       </c>
       <c r="U19" t="n">
-        <v>386.6918026989362</v>
+        <v>576.597802378329</v>
       </c>
       <c r="V19" t="n">
-        <v>0.5206053592771006</v>
+        <v>0.4293440341996695</v>
       </c>
       <c r="W19" t="n">
-        <v>0.4793946407228994</v>
+        <v>0.5706559658003304</v>
       </c>
       <c r="X19" t="n">
-        <v>806.6252099018614</v>
+        <v>1010.412292053524</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.8110370181818182</v>
+        <v>0.7721545090909091</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.7570414975387171</v>
+        <v>1</v>
       </c>
       <c r="AA19" t="n">
-        <v>51.59370961343632</v>
+        <v>47.34410661367475</v>
       </c>
       <c r="AB19" t="n">
         <v>18.49339422520361</v>
       </c>
       <c r="AC19" t="n">
-        <v>45.81186056259731</v>
+        <v>53.77645563174561</v>
       </c>
       <c r="AD19" t="n">
         <v>18.49339422520361</v>
@@ -2246,88 +2246,88 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>35774.46668026772</v>
+        <v>32916.13828994893</v>
       </c>
       <c r="C20" t="n">
-        <v>35830.12457526714</v>
+        <v>29205.41681930564</v>
       </c>
       <c r="D20" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E20" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F20" t="n">
-        <v>138.6125393085798</v>
+        <v>125.411345088715</v>
       </c>
       <c r="G20" t="n">
-        <v>138.6125393085798</v>
+        <v>125.411345088715</v>
       </c>
       <c r="H20" t="n">
-        <v>485.41782</v>
+        <v>521.53077</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>101.4136127268437</v>
       </c>
       <c r="J20" t="n">
-        <v>457.1105568575338</v>
+        <v>550</v>
       </c>
       <c r="K20" t="n">
-        <v>169.5147495257698</v>
+        <v>195.4493285211004</v>
       </c>
       <c r="L20" t="n">
-        <v>403.6966422221078</v>
+        <v>436.2828652878078</v>
       </c>
       <c r="M20" t="n">
-        <v>100.8581263623944</v>
+        <v>72.11839849223897</v>
       </c>
       <c r="N20" t="n">
-        <v>549.5294884589634</v>
+        <v>377.9448029961819</v>
       </c>
       <c r="O20" t="n">
-        <v>123.2665886172543</v>
+        <v>61.17235427697433</v>
       </c>
       <c r="P20" t="n">
-        <v>356.8223060845501</v>
+        <v>436.3628470933573</v>
       </c>
       <c r="Q20" t="n">
-        <v>142.2512642295655</v>
+        <v>121.6728262066305</v>
       </c>
       <c r="R20" t="n">
-        <v>336.6410857042395</v>
+        <v>473.2481743788741</v>
       </c>
       <c r="S20" t="n">
-        <v>131.947234135646</v>
+        <v>121.7305434144821</v>
       </c>
       <c r="T20" t="n">
-        <v>507.41782</v>
+        <v>439.1171572731562</v>
       </c>
       <c r="U20" t="n">
-        <v>499.0735703141156</v>
+        <v>558.0356732999877</v>
       </c>
       <c r="V20" t="n">
-        <v>0.5741219414415969</v>
+        <v>0.4403709680298057</v>
       </c>
       <c r="W20" t="n">
-        <v>0.4258780585584032</v>
+        <v>0.5596290319701943</v>
       </c>
       <c r="X20" t="n">
-        <v>1171.869647390333</v>
+        <v>997.152830573144</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.8825778545454546</v>
+        <v>0.9482377636363636</v>
       </c>
       <c r="Z20" t="n">
-        <v>0.8311101033773342</v>
+        <v>1</v>
       </c>
       <c r="AA20" t="n">
-        <v>51.74031666108237</v>
+        <v>45.95369306801917</v>
       </c>
       <c r="AB20" t="n">
         <v>18.51188761942881</v>
       </c>
       <c r="AC20" t="n">
-        <v>49.9379466861636</v>
+        <v>54.92027405273547</v>
       </c>
       <c r="AD20" t="n">
         <v>18.51188761942881</v>
@@ -2338,88 +2338,88 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>40432.90249359501</v>
+        <v>36585.1967372293</v>
       </c>
       <c r="C21" t="n">
-        <v>31252.13839167538</v>
+        <v>24868.25867651385</v>
       </c>
       <c r="D21" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E21" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F21" t="n">
-        <v>145.5431662740087</v>
+        <v>119.1407778342793</v>
       </c>
       <c r="G21" t="n">
-        <v>145.5431662740087</v>
+        <v>119.1407778342793</v>
       </c>
       <c r="H21" t="n">
-        <v>415.52137</v>
+        <v>477.33327</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>7.774902461520014</v>
       </c>
       <c r="J21" t="n">
-        <v>494.9464480055041</v>
+        <v>550</v>
       </c>
       <c r="K21" t="n">
-        <v>213.4426044867236</v>
+        <v>204.201708314088</v>
       </c>
       <c r="L21" t="n">
-        <v>348.3216125207679</v>
+        <v>446.9067498999694</v>
       </c>
       <c r="M21" t="n">
-        <v>46.19976123075427</v>
+        <v>107.8401298372872</v>
       </c>
       <c r="N21" t="n">
-        <v>387.189500589682</v>
+        <v>452.5473411997388</v>
       </c>
       <c r="O21" t="n">
-        <v>77.63442665435952</v>
+        <v>41.01102633874122</v>
       </c>
       <c r="P21" t="n">
-        <v>344.6184928395808</v>
+        <v>465.7439515201607</v>
       </c>
       <c r="Q21" t="n">
-        <v>106.4001002049695</v>
+        <v>75.5036686868516</v>
       </c>
       <c r="R21" t="n">
-        <v>348.7655065798838</v>
+        <v>505.5098745056914</v>
       </c>
       <c r="S21" t="n">
-        <v>115.69569095139</v>
+        <v>82.48109105045397</v>
       </c>
       <c r="T21" t="n">
-        <v>436.52137</v>
+        <v>493.55836753848</v>
       </c>
       <c r="U21" t="n">
-        <v>451.0185930445503</v>
+        <v>541.2476202070123</v>
       </c>
       <c r="V21" t="n">
-        <v>0.5075369585347167</v>
+        <v>0.4769573943167686</v>
       </c>
       <c r="W21" t="n">
-        <v>0.4924630414652832</v>
+        <v>0.5230426056832315</v>
       </c>
       <c r="X21" t="n">
-        <v>915.8425202885918</v>
+        <v>1034.805987745492</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.7554934</v>
+        <v>0.8678786727272728</v>
       </c>
       <c r="Z21" t="n">
-        <v>0.8999026327372801</v>
+        <v>1</v>
       </c>
       <c r="AA21" t="n">
-        <v>49.76901502419717</v>
+        <v>47.40138386428681</v>
       </c>
       <c r="AB21" t="n">
         <v>18.53039950704824</v>
       </c>
       <c r="AC21" t="n">
-        <v>48.02929861689351</v>
+        <v>52.75687390981355</v>
       </c>
       <c r="AD21" t="n">
         <v>18.53039950704824</v>
@@ -2430,88 +2430,88 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>51680.86440675028</v>
+        <v>30082.84262899712</v>
       </c>
       <c r="C22" t="n">
-        <v>37729.05508101021</v>
+        <v>28996.02941561121</v>
       </c>
       <c r="D22" t="n">
         <v>140</v>
       </c>
       <c r="E22" t="n">
-        <v>80</v>
+        <v>140</v>
       </c>
       <c r="F22" t="n">
-        <v>138.2660079603083</v>
+        <v>125.0978167259932</v>
       </c>
       <c r="G22" t="n">
-        <v>138.2660079603083</v>
+        <v>125.0978167259932</v>
       </c>
       <c r="H22" t="n">
-        <v>538.88801</v>
+        <v>434.14796</v>
       </c>
       <c r="I22" t="n">
-        <v>0</v>
+        <v>102.369928045262</v>
       </c>
       <c r="J22" t="n">
-        <v>490.9652805062645</v>
+        <v>481.2457502794067</v>
       </c>
       <c r="K22" t="n">
-        <v>190.324831833944</v>
+        <v>164.6030467735823</v>
       </c>
       <c r="L22" t="n">
-        <v>419.2567026716844</v>
+        <v>283.040431885441</v>
       </c>
       <c r="M22" t="n">
-        <v>95.63130843365909</v>
+        <v>138.8824301513268</v>
       </c>
       <c r="N22" t="n">
-        <v>400.6108558681446</v>
+        <v>271.8795505222943</v>
       </c>
       <c r="O22" t="n">
-        <v>167.5047002656671</v>
+        <v>79.89848143244379</v>
       </c>
       <c r="P22" t="n">
-        <v>415.8726297201322</v>
+        <v>426.2689021699277</v>
       </c>
       <c r="Q22" t="n">
-        <v>98.21042343891189</v>
+        <v>94.5755096499847</v>
       </c>
       <c r="R22" t="n">
-        <v>400.3324672107321</v>
+        <v>389.1185933944503</v>
       </c>
       <c r="S22" t="n">
-        <v>104.075417782256</v>
+        <v>96.32886519904451</v>
       </c>
       <c r="T22" t="n">
-        <v>562.88801</v>
+        <v>351.778031954738</v>
       </c>
       <c r="U22" t="n">
-        <v>514.0830531590441</v>
+        <v>520.8444118199125</v>
       </c>
       <c r="V22" t="n">
-        <v>0.5249642267652119</v>
+        <v>0.403127417205857</v>
       </c>
       <c r="W22" t="n">
-        <v>0.4750357732347881</v>
+        <v>0.596872582794143</v>
       </c>
       <c r="X22" t="n">
-        <v>1082.198609292856</v>
+        <v>872.6224437746505</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.9797963818181818</v>
+        <v>0.7893599272727273</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.8926641463750263</v>
+        <v>0.8749922732352849</v>
       </c>
       <c r="AA22" t="n">
-        <v>50.33227032319707</v>
+        <v>43.67483838591729</v>
       </c>
       <c r="AB22" t="n">
         <v>18.54892990655528</v>
       </c>
       <c r="AC22" t="n">
-        <v>46.37516384781094</v>
+        <v>53.25626626305002</v>
       </c>
       <c r="AD22" t="n">
         <v>18.54892990655528</v>
@@ -2522,88 +2522,88 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>39544.14044163503</v>
+        <v>33426.4145969814</v>
       </c>
       <c r="C23" t="n">
-        <v>32779.9705853888</v>
+        <v>23513.1762451373</v>
       </c>
       <c r="D23" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E23" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F23" t="n">
-        <v>145.1793083583237</v>
+        <v>118.8429258896936</v>
       </c>
       <c r="G23" t="n">
-        <v>145.1793083583237</v>
+        <v>118.8429258896936</v>
       </c>
       <c r="H23" t="n">
-        <v>481.4344</v>
+        <v>410.26508</v>
       </c>
       <c r="I23" t="n">
-        <v>42.56160146905921</v>
+        <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>443.1648853825891</v>
+        <v>550</v>
       </c>
       <c r="K23" t="n">
-        <v>195.9931188759207</v>
+        <v>179.4776579892297</v>
       </c>
       <c r="L23" t="n">
-        <v>390.1867025410588</v>
+        <v>392.6454994953268</v>
       </c>
       <c r="M23" t="n">
-        <v>75.24769711249211</v>
+        <v>95.98951298053957</v>
       </c>
       <c r="N23" t="n">
-        <v>392.8632628117987</v>
+        <v>380.7678063256957</v>
       </c>
       <c r="O23" t="n">
-        <v>62.00953571914211</v>
+        <v>75.39712789865129</v>
       </c>
       <c r="P23" t="n">
-        <v>352.30317843099</v>
+        <v>395.8145297226576</v>
       </c>
       <c r="Q23" t="n">
-        <v>85.19341990962238</v>
+        <v>139.310859061695</v>
       </c>
       <c r="R23" t="n">
-        <v>355.1708189668503</v>
+        <v>390.6921137335964</v>
       </c>
       <c r="S23" t="n">
-        <v>78.31889824968276</v>
+        <v>140.0117011811826</v>
       </c>
       <c r="T23" t="n">
-        <v>454.8727985309408</v>
+        <v>434.26508</v>
       </c>
       <c r="U23" t="n">
-        <v>437.4965983406124</v>
+        <v>535.1253887843526</v>
       </c>
       <c r="V23" t="n">
-        <v>0.5097359906397763</v>
+        <v>0.4601728914691964</v>
       </c>
       <c r="W23" t="n">
-        <v>0.4902640093602238</v>
+        <v>0.5398271085308035</v>
       </c>
       <c r="X23" t="n">
-        <v>892.3693968715531</v>
+        <v>991.2903230086996</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.8753352727272727</v>
+        <v>0.7459365090909091</v>
       </c>
       <c r="Z23" t="n">
-        <v>0.8057543370592529</v>
+        <v>1</v>
       </c>
       <c r="AA23" t="n">
-        <v>49.96096695574425</v>
+        <v>45.54468784674192</v>
       </c>
       <c r="AB23" t="n">
         <v>18.56747883646184</v>
       </c>
       <c r="AC23" t="n">
-        <v>45.42639554042096</v>
+        <v>53.65749454513181</v>
       </c>
       <c r="AD23" t="n">
         <v>18.56747883646184</v>
@@ -2614,88 +2614,88 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>45803.0652335039</v>
+        <v>32991.2900210027</v>
       </c>
       <c r="C24" t="n">
-        <v>42638.49338636606</v>
+        <v>20269.82165248213</v>
       </c>
       <c r="D24" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E24" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F24" t="n">
-        <v>137.9203429404075</v>
+        <v>124.7850721841782</v>
       </c>
       <c r="G24" t="n">
-        <v>137.9203429404075</v>
+        <v>124.7850721841782</v>
       </c>
       <c r="H24" t="n">
-        <v>447.57332</v>
+        <v>482.82745</v>
       </c>
       <c r="I24" t="n">
-        <v>0</v>
+        <v>42.90164925298171</v>
       </c>
       <c r="J24" t="n">
-        <v>550</v>
+        <v>513.7300108439707</v>
       </c>
       <c r="K24" t="n">
-        <v>179.0200017853022</v>
+        <v>229.8666476560813</v>
       </c>
       <c r="L24" t="n">
-        <v>346.3003760281439</v>
+        <v>387.7613888851649</v>
       </c>
       <c r="M24" t="n">
-        <v>118.8345429999317</v>
+        <v>76.06606165866009</v>
       </c>
       <c r="N24" t="n">
-        <v>447.5728451764754</v>
+        <v>397.2054314075017</v>
       </c>
       <c r="O24" t="n">
-        <v>85.2298860650511</v>
+        <v>61.72036933951656</v>
       </c>
       <c r="P24" t="n">
-        <v>468.1257032294731</v>
+        <v>339.7021356679776</v>
       </c>
       <c r="Q24" t="n">
-        <v>98.84741386114554</v>
+        <v>123.6388855091415</v>
       </c>
       <c r="R24" t="n">
-        <v>503.9147143069497</v>
+        <v>368.4603687353445</v>
       </c>
       <c r="S24" t="n">
-        <v>102.2268686484356</v>
+        <v>124.7473000978558</v>
       </c>
       <c r="T24" t="n">
-        <v>472.57332</v>
+        <v>458.9258007470183</v>
       </c>
       <c r="U24" t="n">
-        <v>566.9731170906186</v>
+        <v>463.3410211771191</v>
       </c>
       <c r="V24" t="n">
-        <v>0.4844648407669104</v>
+        <v>0.497606321551886</v>
       </c>
       <c r="W24" t="n">
-        <v>0.5155351592330897</v>
+        <v>0.502393678448114</v>
       </c>
       <c r="X24" t="n">
-        <v>1099.775848332145</v>
+        <v>922.2668219241374</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.8137696727272727</v>
+        <v>0.8778680909090909</v>
       </c>
       <c r="Z24" t="n">
-        <v>1</v>
+        <v>0.9340545651708558</v>
       </c>
       <c r="AA24" t="n">
-        <v>45.48349657324549</v>
+        <v>45.55251108886526</v>
       </c>
       <c r="AB24" t="n">
         <v>18.5860463152983</v>
       </c>
       <c r="AC24" t="n">
-        <v>45.41503251596223</v>
+        <v>52.29626804969558</v>
       </c>
       <c r="AD24" t="n">
         <v>18.5860463152983</v>
@@ -2706,88 +2706,88 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>24383.70742697809</v>
+        <v>18034.53774142129</v>
       </c>
       <c r="C25" t="n">
-        <v>23500.92592623192</v>
+        <v>22998.23926493282</v>
       </c>
       <c r="D25" t="n">
         <v>140</v>
       </c>
       <c r="E25" t="n">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="F25" t="n">
-        <v>144.8163600874279</v>
+        <v>131.0243257933872</v>
       </c>
       <c r="G25" t="n">
-        <v>144.8163600874279</v>
+        <v>131.0243257933872</v>
       </c>
       <c r="H25" t="n">
-        <v>518.6442500000001</v>
+        <v>476.64844</v>
       </c>
       <c r="I25" t="n">
-        <v>189.5826010537876</v>
+        <v>199.9286314819689</v>
       </c>
       <c r="J25" t="n">
-        <v>328.6535057280738</v>
+        <v>380.4755425611777</v>
       </c>
       <c r="K25" t="n">
-        <v>174.985511598456</v>
+        <v>209.8611126626874</v>
       </c>
       <c r="L25" t="n">
-        <v>376.8265772375016</v>
+        <v>381.5510226097936</v>
       </c>
       <c r="M25" t="n">
-        <v>117.8176764878082</v>
+        <v>120.9990619622946</v>
       </c>
       <c r="N25" t="n">
-        <v>285.0266072134901</v>
+        <v>234.9464307139382</v>
       </c>
       <c r="O25" t="n">
-        <v>68.03504173272232</v>
+        <v>58.77337780409296</v>
       </c>
       <c r="P25" t="n">
-        <v>257.5258498178787</v>
+        <v>306.2183176923769</v>
       </c>
       <c r="Q25" t="n">
-        <v>75.16214609704129</v>
+        <v>94.26275986219467</v>
       </c>
       <c r="R25" t="n">
-        <v>236.8878416666772</v>
+        <v>312.7337932460518</v>
       </c>
       <c r="S25" t="n">
-        <v>70.78566584669868</v>
+        <v>97.60839697120711</v>
       </c>
       <c r="T25" t="n">
-        <v>353.0616489462125</v>
+        <v>293.7198085180311</v>
       </c>
       <c r="U25" t="n">
-        <v>332.68799591492</v>
+        <v>400.4810775545716</v>
       </c>
       <c r="V25" t="n">
-        <v>0.5148550226631311</v>
+        <v>0.4231049173384555</v>
       </c>
       <c r="W25" t="n">
-        <v>0.4851449773368688</v>
+        <v>0.5768950826615444</v>
       </c>
       <c r="X25" t="n">
-        <v>685.7496448611324</v>
+        <v>694.2008860726028</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.9429895454545456</v>
+        <v>0.8666335272727272</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.5975518285964977</v>
+        <v>0.6917737137475959</v>
       </c>
       <c r="AA25" t="n">
-        <v>47.55814457286296</v>
+        <v>47.59562034471178</v>
       </c>
       <c r="AB25" t="n">
         <v>18.60463236161359</v>
       </c>
       <c r="AC25" t="n">
-        <v>42.8877818711777</v>
+        <v>49.47033852359848</v>
       </c>
       <c r="AD25" t="n">
         <v>18.60463236161359</v>
@@ -2798,88 +2798,88 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>41302.77714535171</v>
+        <v>33168.13248439984</v>
       </c>
       <c r="C26" t="n">
-        <v>27560.35541450699</v>
+        <v>36036.59972537778</v>
       </c>
       <c r="D26" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E26" t="n">
-        <v>80</v>
+        <v>200</v>
       </c>
       <c r="F26" t="n">
-        <v>137.5755420830565</v>
+        <v>124.4731095037178</v>
       </c>
       <c r="G26" t="n">
-        <v>137.5755420830565</v>
+        <v>124.4731095037178</v>
       </c>
       <c r="H26" t="n">
-        <v>474.81596</v>
+        <v>435.83647</v>
       </c>
       <c r="I26" t="n">
-        <v>42.08008476711359</v>
+        <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>466.8991446442613</v>
+        <v>550</v>
       </c>
       <c r="K26" t="n">
-        <v>216.4222774482309</v>
+        <v>164.7430665069646</v>
       </c>
       <c r="L26" t="n">
-        <v>486.9958519540866</v>
+        <v>558.9481592915332</v>
       </c>
       <c r="M26" t="n">
-        <v>158.4027107979167</v>
+        <v>52.8169461168221</v>
       </c>
       <c r="N26" t="n">
-        <v>342.9072496975735</v>
+        <v>527.2932170806928</v>
       </c>
       <c r="O26" t="n">
-        <v>108.828625535313</v>
+        <v>69.45327227857096</v>
       </c>
       <c r="P26" t="n">
-        <v>361.3570208329328</v>
+        <v>455.4934210280269</v>
       </c>
       <c r="Q26" t="n">
-        <v>64.10535796155345</v>
+        <v>139.624625127696</v>
       </c>
       <c r="R26" t="n">
-        <v>374.9239564324091</v>
+        <v>482.2886925812294</v>
       </c>
       <c r="S26" t="n">
-        <v>66.96069981030816</v>
+        <v>139.473748231207</v>
       </c>
       <c r="T26" t="n">
-        <v>451.7358752328864</v>
+        <v>459.83647</v>
       </c>
       <c r="U26" t="n">
-        <v>425.4623787944863</v>
+        <v>595.1180461557228</v>
       </c>
       <c r="V26" t="n">
-        <v>0.5149758029714342</v>
+        <v>0.5006831494498816</v>
       </c>
       <c r="W26" t="n">
-        <v>0.4850241970285658</v>
+        <v>0.4993168505501184</v>
       </c>
       <c r="X26" t="n">
-        <v>877.1982540273727</v>
+        <v>1191.864535514987</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.8633017454545455</v>
+        <v>0.7924299454545455</v>
       </c>
       <c r="Z26" t="n">
-        <v>0.8489075357168387</v>
+        <v>1</v>
       </c>
       <c r="AA26" t="n">
-        <v>46.03064567947159</v>
+        <v>50.50574109963803</v>
       </c>
       <c r="AB26" t="n">
         <v>18.6232369939752</v>
       </c>
       <c r="AC26" t="n">
-        <v>43.47242293188006</v>
+        <v>49.94059549400324</v>
       </c>
       <c r="AD26" t="n">
         <v>18.6232369939752</v>
@@ -2890,13 +2890,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>41058.14572675453</v>
+        <v>12564.75751735416</v>
       </c>
       <c r="C27" t="n">
-        <v>31423.87078506264</v>
+        <v>15051.14444103105</v>
       </c>
       <c r="D27" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E27" t="n">
         <v>160</v>
@@ -2908,70 +2908,70 @@
         <v>130.6967649789037</v>
       </c>
       <c r="H27" t="n">
-        <v>515.68597</v>
+        <v>480.49937</v>
       </c>
       <c r="I27" t="n">
-        <v>0</v>
+        <v>235.8557823769706</v>
       </c>
       <c r="J27" t="n">
-        <v>502.03319493983</v>
+        <v>407.0102586646685</v>
       </c>
       <c r="K27" t="n">
-        <v>229.6572401688507</v>
+        <v>216.547424811198</v>
       </c>
       <c r="L27" t="n">
-        <v>450.0671797718276</v>
+        <v>365.8283168088877</v>
       </c>
       <c r="M27" t="n">
-        <v>91.69887837682478</v>
+        <v>90.6710483518204</v>
       </c>
       <c r="N27" t="n">
-        <v>478.1351452232685</v>
+        <v>226.3949031562336</v>
       </c>
       <c r="O27" t="n">
-        <v>96.99217411556569</v>
+        <v>42.24868446679579</v>
       </c>
       <c r="P27" t="n">
-        <v>370.1412078350306</v>
+        <v>298.0385151043652</v>
       </c>
       <c r="Q27" t="n">
-        <v>118.6570243841796</v>
+        <v>57.16738525606996</v>
       </c>
       <c r="R27" t="n">
-        <v>395.6253339358569</v>
+        <v>315.9902133811004</v>
       </c>
       <c r="S27" t="n">
-        <v>122.830138452204</v>
+        <v>55.76311179053273</v>
       </c>
       <c r="T27" t="n">
-        <v>531.68597</v>
+        <v>268.6435876230294</v>
       </c>
       <c r="U27" t="n">
-        <v>488.7982322192102</v>
+        <v>355.2059003604352</v>
       </c>
       <c r="V27" t="n">
-        <v>0.5405710188054047</v>
+        <v>0.4306224382605408</v>
       </c>
       <c r="W27" t="n">
-        <v>0.4594289811945953</v>
+        <v>0.5693775617394593</v>
       </c>
       <c r="X27" t="n">
-        <v>1063.925551558044</v>
+        <v>623.8494879834645</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.9376108545454546</v>
+        <v>0.8736352181818182</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.9127876271633272</v>
+        <v>0.7400186521175791</v>
       </c>
       <c r="AA27" t="n">
-        <v>44.10469160765701</v>
+        <v>51.14186348489077</v>
       </c>
       <c r="AB27" t="n">
         <v>18.64186023096918</v>
       </c>
       <c r="AC27" t="n">
-        <v>43.32012206609343</v>
+        <v>50.8267278783383</v>
       </c>
       <c r="AD27" t="n">
         <v>18.64186023096918</v>
@@ -2982,88 +2982,88 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>31977.6958561637</v>
+        <v>30854.03988450524</v>
       </c>
       <c r="C28" t="n">
-        <v>31837.29373139142</v>
+        <v>19718.94476899172</v>
       </c>
       <c r="D28" t="n">
+        <v>120</v>
+      </c>
+      <c r="E28" t="n">
         <v>140</v>
       </c>
-      <c r="E28" t="n">
-        <v>200</v>
-      </c>
       <c r="F28" t="n">
-        <v>137.2316032278489</v>
+        <v>124.1619267299585</v>
       </c>
       <c r="G28" t="n">
-        <v>137.2316032278489</v>
+        <v>124.1619267299585</v>
       </c>
       <c r="H28" t="n">
-        <v>474.98114</v>
+        <v>456.0611</v>
       </c>
       <c r="I28" t="n">
-        <v>119.7366893311528</v>
+        <v>28.64038141309146</v>
       </c>
       <c r="J28" t="n">
-        <v>372.0145741775597</v>
+        <v>390.7808298349053</v>
       </c>
       <c r="K28" t="n">
-        <v>177.2588560645775</v>
+        <v>191.2490455843418</v>
       </c>
       <c r="L28" t="n">
-        <v>360.7947511089586</v>
+        <v>567.3802555401577</v>
       </c>
       <c r="M28" t="n">
-        <v>92.18639281912597</v>
+        <v>102.5366252806621</v>
       </c>
       <c r="N28" t="n">
-        <v>315.9100280689236</v>
+        <v>375.6253884940829</v>
       </c>
       <c r="O28" t="n">
-        <v>61.33442259992366</v>
+        <v>73.79533009282561</v>
       </c>
       <c r="P28" t="n">
-        <v>335.4163610621032</v>
+        <v>327.7418391332535</v>
       </c>
       <c r="Q28" t="n">
-        <v>88.99659721972971</v>
+        <v>88.33736992850791</v>
       </c>
       <c r="R28" t="n">
-        <v>317.1854999736415</v>
+        <v>311.6672546789046</v>
       </c>
       <c r="S28" t="n">
-        <v>84.48631437276885</v>
+        <v>95.66099996719868</v>
       </c>
       <c r="T28" t="n">
-        <v>377.2444506688472</v>
+        <v>449.4207185869085</v>
       </c>
       <c r="U28" t="n">
-        <v>424.412958281833</v>
+        <v>416.0792090617614</v>
       </c>
       <c r="V28" t="n">
-        <v>0.470580632645355</v>
+        <v>0.5192614167026721</v>
       </c>
       <c r="W28" t="n">
-        <v>0.5294193673546449</v>
+        <v>0.4807385832973279</v>
       </c>
       <c r="X28" t="n">
-        <v>801.6574089506802</v>
+        <v>865.4999276486699</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.8636020727272727</v>
+        <v>0.829202</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.6763901348682904</v>
+        <v>0.7105105996998278</v>
       </c>
       <c r="AA28" t="n">
-        <v>43.36394042679801</v>
+        <v>50.473863223804</v>
       </c>
       <c r="AB28" t="n">
         <v>18.66050209120014</v>
       </c>
       <c r="AC28" t="n">
-        <v>42.43861450028577</v>
+        <v>54.49724150507136</v>
       </c>
       <c r="AD28" t="n">
         <v>18.66050209120014</v>
@@ -3074,88 +3074,88 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>37030.7224089188</v>
+        <v>18767.29266851334</v>
       </c>
       <c r="C29" t="n">
-        <v>27726.45414861419</v>
+        <v>16692.32029561729</v>
       </c>
       <c r="D29" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E29" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F29" t="n">
-        <v>144.0931833892413</v>
+        <v>130.3700230664564</v>
       </c>
       <c r="G29" t="n">
-        <v>144.0931833892413</v>
+        <v>130.3700230664564</v>
       </c>
       <c r="H29" t="n">
-        <v>518.50339</v>
+        <v>470.58435</v>
       </c>
       <c r="I29" t="n">
-        <v>108.5439138658128</v>
+        <v>153.4830483967635</v>
       </c>
       <c r="J29" t="n">
-        <v>418.2238253975313</v>
+        <v>393.7666635084109</v>
       </c>
       <c r="K29" t="n">
-        <v>206.2824500989175</v>
+        <v>212.2090291695944</v>
       </c>
       <c r="L29" t="n">
-        <v>485.9773790347368</v>
+        <v>371.5078075706774</v>
       </c>
       <c r="M29" t="n">
-        <v>128.2627032333014</v>
+        <v>110.7169241034823</v>
       </c>
       <c r="N29" t="n">
-        <v>328.9118615334429</v>
+        <v>266.3380594960739</v>
       </c>
       <c r="O29" t="n">
-        <v>105.0476146007442</v>
+        <v>67.7632421071626</v>
       </c>
       <c r="P29" t="n">
-        <v>301.6726459536626</v>
+        <v>263.3271715356301</v>
       </c>
       <c r="Q29" t="n">
-        <v>87.52758540952865</v>
+        <v>109.4795083875283</v>
       </c>
       <c r="R29" t="n">
-        <v>302.5585750795016</v>
+        <v>274.2788341420712</v>
       </c>
       <c r="S29" t="n">
-        <v>92.92410638260714</v>
+        <v>110.7368749506816</v>
       </c>
       <c r="T29" t="n">
-        <v>433.9594761341871</v>
+        <v>334.1013016032365</v>
       </c>
       <c r="U29" t="n">
-        <v>389.2002313631913</v>
+        <v>372.8066799231584</v>
       </c>
       <c r="V29" t="n">
-        <v>0.527187460928497</v>
+        <v>0.4726234677416238</v>
       </c>
       <c r="W29" t="n">
-        <v>0.4728125390715031</v>
+        <v>0.5273765322583762</v>
       </c>
       <c r="X29" t="n">
-        <v>823.1597074973783</v>
+        <v>706.9079815263949</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.9427334363636363</v>
+        <v>0.855607909090909</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.7604069552682388</v>
+        <v>0.7159393881971108</v>
       </c>
       <c r="AA29" t="n">
-        <v>45.33531867966335</v>
+        <v>51.76311206081095</v>
       </c>
       <c r="AB29" t="n">
         <v>18.67916259329134</v>
       </c>
       <c r="AC29" t="n">
-        <v>42.24661715777397</v>
+        <v>53.87083175514014</v>
       </c>
       <c r="AD29" t="n">
         <v>18.67916259329134</v>
@@ -3166,88 +3166,88 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>29942.56688168814</v>
+        <v>33256.35232249934</v>
       </c>
       <c r="C30" t="n">
-        <v>27762.66202382493</v>
+        <v>28406.11023557238</v>
       </c>
       <c r="D30" t="n">
         <v>140</v>
       </c>
       <c r="E30" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="F30" t="n">
-        <v>136.8885242197792</v>
+        <v>136.8885242197793</v>
       </c>
       <c r="G30" t="n">
-        <v>136.8885242197792</v>
+        <v>136.8885242197793</v>
       </c>
       <c r="H30" t="n">
-        <v>520.84849</v>
+        <v>471.09996</v>
       </c>
       <c r="I30" t="n">
-        <v>162.7731043728166</v>
+        <v>77.51442848071559</v>
       </c>
       <c r="J30" t="n">
-        <v>387.0810183629328</v>
+        <v>444.3267179201736</v>
       </c>
       <c r="K30" t="n">
-        <v>197.0475718127254</v>
+        <v>206.6215408726475</v>
       </c>
       <c r="L30" t="n">
-        <v>483.1418344872918</v>
+        <v>416.1425849952191</v>
       </c>
       <c r="M30" t="n">
-        <v>122.2505739947209</v>
+        <v>185.4404226772006</v>
       </c>
       <c r="N30" t="n">
-        <v>317.7669112372794</v>
+        <v>318.6102968538856</v>
       </c>
       <c r="O30" t="n">
-        <v>64.30847438990396</v>
+        <v>97.97523466539877</v>
       </c>
       <c r="P30" t="n">
-        <v>339.9307266691621</v>
+        <v>348.5797392474603</v>
       </c>
       <c r="Q30" t="n">
-        <v>56.38516997996278</v>
+        <v>101.3344669696601</v>
       </c>
       <c r="R30" t="n">
-        <v>334.1158523193758</v>
+        <v>363.3083364653543</v>
       </c>
       <c r="S30" t="n">
-        <v>59.24761614247447</v>
+        <v>93.22741062441374</v>
       </c>
       <c r="T30" t="n">
-        <v>382.0753856271834</v>
+        <v>416.5855315192844</v>
       </c>
       <c r="U30" t="n">
-        <v>396.3158966491249</v>
+        <v>449.9142062171205</v>
       </c>
       <c r="V30" t="n">
-        <v>0.4908526011620423</v>
+        <v>0.4807682142034445</v>
       </c>
       <c r="W30" t="n">
-        <v>0.5091473988379578</v>
+        <v>0.5192317857965555</v>
       </c>
       <c r="X30" t="n">
-        <v>778.3912822763082</v>
+        <v>866.4997377364049</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.9469972545454545</v>
+        <v>0.8565453818181819</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.7037836697507869</v>
+        <v>0.807866759854861</v>
       </c>
       <c r="AA30" t="n">
-        <v>44.58578904082432</v>
+        <v>52.87751082220224</v>
       </c>
       <c r="AB30" t="n">
         <v>18.69784175588463</v>
       </c>
       <c r="AC30" t="n">
-        <v>40.84552673447329</v>
+        <v>50.60448657413488</v>
       </c>
       <c r="AD30" t="n">
         <v>18.69784175588463</v>
@@ -3258,88 +3258,88 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>41695.02831058641</v>
+        <v>23664.91164303885</v>
       </c>
       <c r="C31" t="n">
-        <v>28772.95256186561</v>
+        <v>25996.27882436176</v>
       </c>
       <c r="D31" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E31" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F31" t="n">
-        <v>143.7329504307682</v>
+        <v>130.0440980087903</v>
       </c>
       <c r="G31" t="n">
-        <v>143.7329504307682</v>
+        <v>130.0440980087903</v>
       </c>
       <c r="H31" t="n">
-        <v>402.75775</v>
+        <v>514.44807</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>132.6025412245144</v>
       </c>
       <c r="J31" t="n">
-        <v>371.5820501681176</v>
+        <v>406.7979933350492</v>
       </c>
       <c r="K31" t="n">
-        <v>184.9370864610624</v>
+        <v>175.2481005151494</v>
       </c>
       <c r="L31" t="n">
-        <v>450.3400142725828</v>
+        <v>470.337521032725</v>
       </c>
       <c r="M31" t="n">
-        <v>100.1908357809609</v>
+        <v>104.6249787098826</v>
       </c>
       <c r="N31" t="n">
-        <v>342.1615237368266</v>
+        <v>334.843299569991</v>
       </c>
       <c r="O31" t="n">
-        <v>80.81326868864612</v>
+        <v>64.00222920549466</v>
       </c>
       <c r="P31" t="n">
-        <v>316.1900760809001</v>
+        <v>334.3893485224903</v>
       </c>
       <c r="Q31" t="n">
-        <v>67.50245943888054</v>
+        <v>103.782085170057</v>
       </c>
       <c r="R31" t="n">
-        <v>302.0449404584951</v>
+        <v>319.334849685491</v>
       </c>
       <c r="S31" t="n">
-        <v>66.58468152234785</v>
+        <v>94.08468452220573</v>
       </c>
       <c r="T31" t="n">
-        <v>417.75775</v>
+        <v>398.8455287754856</v>
       </c>
       <c r="U31" t="n">
-        <v>383.6925355197806</v>
+        <v>438.1714336925473</v>
       </c>
       <c r="V31" t="n">
-        <v>0.5243484863864215</v>
+        <v>0.4765082987081258</v>
       </c>
       <c r="W31" t="n">
-        <v>0.4756515136135785</v>
+        <v>0.5234917012918741</v>
       </c>
       <c r="X31" t="n">
-        <v>806.6673279452533</v>
+        <v>837.0169624680329</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.7322868181818182</v>
+        <v>0.9353601272727273</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.6756037275783956</v>
+        <v>0.7396327151546348</v>
       </c>
       <c r="AA31" t="n">
-        <v>41.69021375606948</v>
+        <v>54.27137089915654</v>
       </c>
       <c r="AB31" t="n">
         <v>18.71653959764052</v>
       </c>
       <c r="AC31" t="n">
-        <v>42.28497223674159</v>
+        <v>50.00205850798848</v>
       </c>
       <c r="AD31" t="n">
         <v>18.71653959764052</v>

</xml_diff>

<commit_message>
Diverse Optimierungen / Orchestrierung in der sim.py
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -590,10 +590,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="n">
-        <v>5679.821430338987</v>
+        <v>11452.12301555125</v>
       </c>
       <c r="C2" t="n">
-        <v>7038.958685885242</v>
+        <v>6991.196496565582</v>
       </c>
       <c r="D2" t="n">
         <v>120</v>
@@ -602,22 +602,22 @@
         <v>160</v>
       </c>
       <c r="F2" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="G2" t="n">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="H2" t="n">
         <v>482.68944</v>
       </c>
       <c r="I2" t="n">
-        <v>270.8351358168936</v>
+        <v>223.5211883971209</v>
       </c>
       <c r="J2" t="n">
-        <v>550</v>
+        <v>388.4061514001579</v>
       </c>
       <c r="K2" t="n">
-        <v>149.1686104122874</v>
+        <v>44.42080428585865</v>
       </c>
       <c r="L2" t="n">
         <v>375.7246723676083</v>
@@ -626,55 +626,55 @@
         <v>85.96476708572624</v>
       </c>
       <c r="N2" t="n">
-        <v>208.3202128865276</v>
+        <v>253.7765941481692</v>
       </c>
       <c r="O2" t="n">
-        <v>24.53409129657886</v>
+        <v>26.39165745470986</v>
       </c>
       <c r="P2" t="n">
-        <v>355.1036484297632</v>
+        <v>300.8666355631923</v>
       </c>
       <c r="Q2" t="n">
-        <v>45.72774115794944</v>
+        <v>43.1187115511069</v>
       </c>
       <c r="R2" t="n">
-        <v>379.5499168516393</v>
+        <v>321.5790854765853</v>
       </c>
       <c r="S2" t="n">
-        <v>49.66048086110753</v>
+        <v>46.82706592357255</v>
       </c>
       <c r="T2" t="n">
-        <v>232.8543041831064</v>
+        <v>280.1682516028791</v>
       </c>
       <c r="U2" t="n">
-        <v>400.8313895877126</v>
+        <v>343.9853471142992</v>
       </c>
       <c r="V2" t="n">
-        <v>0.3674602511498726</v>
+        <v>0.4488770907973748</v>
       </c>
       <c r="W2" t="n">
-        <v>0.6325397488501274</v>
+        <v>0.5511229092026252</v>
       </c>
       <c r="X2" t="n">
-        <v>633.6856937708189</v>
+        <v>624.1535987171783</v>
       </c>
       <c r="Y2" t="n">
         <v>0.8776171636363637</v>
       </c>
       <c r="Z2" t="n">
-        <v>1</v>
+        <v>0.7061930025457416</v>
       </c>
       <c r="AA2" t="n">
         <v>45</v>
       </c>
       <c r="AB2" t="n">
-        <v>18.18181818181818</v>
+        <v>27.27272727272727</v>
       </c>
       <c r="AC2" t="n">
         <v>45</v>
       </c>
       <c r="AD2" t="n">
-        <v>18.18181818181818</v>
+        <v>27.27272727272727</v>
       </c>
     </row>
     <row r="3">
@@ -682,91 +682,91 @@
         <v>2</v>
       </c>
       <c r="B3" t="n">
-        <v>22319.71931434115</v>
+        <v>28941.49004434307</v>
       </c>
       <c r="C3" t="n">
-        <v>11586.13502190949</v>
+        <v>15403.08896376143</v>
       </c>
       <c r="D3" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E3" t="n">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="F3" t="n">
-        <v>99.75</v>
+        <v>132.25</v>
       </c>
       <c r="G3" t="n">
-        <v>99.75</v>
+        <v>132.25</v>
       </c>
       <c r="H3" t="n">
-        <v>432.0445</v>
+        <v>336.87275</v>
       </c>
       <c r="I3" t="n">
-        <v>47.68288049144132</v>
+        <v>0</v>
       </c>
       <c r="J3" t="n">
-        <v>463.3996279601339</v>
+        <v>292.0140912566667</v>
       </c>
       <c r="K3" t="n">
-        <v>177.3523968049869</v>
+        <v>4.104684053886047</v>
       </c>
       <c r="L3" t="n">
-        <v>599.9608859919654</v>
+        <v>465.0790072752424</v>
       </c>
       <c r="M3" t="n">
-        <v>78.91875469625967</v>
+        <v>71.31492943518526</v>
       </c>
       <c r="N3" t="n">
-        <v>373.0809820866488</v>
+        <v>411.8667074349304</v>
       </c>
       <c r="O3" t="n">
-        <v>35.2806374219099</v>
+        <v>33.53432501625861</v>
       </c>
       <c r="P3" t="n">
-        <v>376.8352245987208</v>
+        <v>279.2748165514733</v>
       </c>
       <c r="Q3" t="n">
-        <v>58.38061696871356</v>
+        <v>53.05539493716601</v>
       </c>
       <c r="R3" t="n">
-        <v>348.8860655823793</v>
+        <v>258.5615292907918</v>
       </c>
       <c r="S3" t="n">
-        <v>63.68217279004205</v>
+        <v>57.8733662517335</v>
       </c>
       <c r="T3" t="n">
-        <v>408.3616195085587</v>
+        <v>360.87275</v>
       </c>
       <c r="U3" t="n">
-        <v>435.2158415674344</v>
+        <v>332.3302114886393</v>
       </c>
       <c r="V3" t="n">
-        <v>0.4840831320785747</v>
+        <v>0.5726927340540905</v>
       </c>
       <c r="W3" t="n">
-        <v>0.5159168679214252</v>
+        <v>0.4273072659459096</v>
       </c>
       <c r="X3" t="n">
-        <v>843.5774610759931</v>
+        <v>777.7312439398283</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.7855354545454546</v>
+        <v>0.6124959090909091</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.8425447781093344</v>
+        <v>0.5309347113757577</v>
       </c>
       <c r="AA3" t="n">
         <v>42.63698965160264</v>
       </c>
       <c r="AB3" t="n">
-        <v>18.2</v>
+        <v>27.3</v>
       </c>
       <c r="AC3" t="n">
         <v>46.31410792301819</v>
       </c>
       <c r="AD3" t="n">
-        <v>18.2</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="4">
@@ -774,91 +774,91 @@
         <v>3</v>
       </c>
       <c r="B4" t="n">
-        <v>25322.70729049107</v>
+        <v>20630.79891825258</v>
       </c>
       <c r="C4" t="n">
-        <v>12842.96661759865</v>
+        <v>15617.41379515517</v>
       </c>
       <c r="D4" t="n">
-        <v>100</v>
+        <v>120</v>
       </c>
       <c r="E4" t="n">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="F4" t="n">
-        <v>104.7375</v>
+        <v>112.4125</v>
       </c>
       <c r="G4" t="n">
-        <v>104.7375</v>
+        <v>112.4125</v>
       </c>
       <c r="H4" t="n">
-        <v>476.8046</v>
+        <v>543.30857</v>
       </c>
       <c r="I4" t="n">
-        <v>46.94010690297796</v>
+        <v>202.2860479705956</v>
       </c>
       <c r="J4" t="n">
-        <v>486.8486512889439</v>
+        <v>542.3939519162641</v>
       </c>
       <c r="K4" t="n">
-        <v>217.390187979185</v>
+        <v>40.24553381847801</v>
       </c>
       <c r="L4" t="n">
-        <v>418.7938689328366</v>
+        <v>423.9717200271172</v>
       </c>
       <c r="M4" t="n">
-        <v>83.69360905449918</v>
+        <v>97.33684613438561</v>
       </c>
       <c r="N4" t="n">
-        <v>410.4880662605666</v>
+        <v>313.3337036312373</v>
       </c>
       <c r="O4" t="n">
-        <v>41.37642683645544</v>
+        <v>49.68881839816719</v>
       </c>
       <c r="P4" t="n">
-        <v>341.1191299112214</v>
+        <v>406.8490891428245</v>
       </c>
       <c r="Q4" t="n">
-        <v>105.6917302035243</v>
+        <v>99.40401300884771</v>
       </c>
       <c r="R4" t="n">
-        <v>356.5442358300962</v>
+        <v>425.2464457925647</v>
       </c>
       <c r="S4" t="n">
-        <v>107.6568122638346</v>
+        <v>101.2521901775854</v>
       </c>
       <c r="T4" t="n">
-        <v>451.864493097022</v>
+        <v>363.0225220294045</v>
       </c>
       <c r="U4" t="n">
-        <v>446.8108601147458</v>
+        <v>506.2531021516722</v>
       </c>
       <c r="V4" t="n">
-        <v>0.5028117122408082</v>
+        <v>0.4176149795657725</v>
       </c>
       <c r="W4" t="n">
-        <v>0.4971882877591919</v>
+        <v>0.5823850204342275</v>
       </c>
       <c r="X4" t="n">
-        <v>898.6753532117677</v>
+        <v>869.2756241810766</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.8669174545454545</v>
+        <v>0.9878337636363637</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.885179365979898</v>
+        <v>0.9861708216659347</v>
       </c>
       <c r="AA4" t="n">
         <v>41.46323631400617</v>
       </c>
       <c r="AB4" t="n">
-        <v>18.21819999999999</v>
+        <v>27.32729999999999</v>
       </c>
       <c r="AC4" t="n">
         <v>48.26981733541643</v>
       </c>
       <c r="AD4" t="n">
-        <v>18.21819999999999</v>
+        <v>27.32729999999999</v>
       </c>
     </row>
     <row r="5">
@@ -866,10 +866,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="n">
-        <v>8916.651908028911</v>
+        <v>22077.11841248934</v>
       </c>
       <c r="C5" t="n">
-        <v>11430.68151926779</v>
+        <v>7169.749557576528</v>
       </c>
       <c r="D5" t="n">
         <v>130</v>
@@ -878,79 +878,79 @@
         <v>180</v>
       </c>
       <c r="F5" t="n">
-        <v>109.974375</v>
+        <v>129.274375</v>
       </c>
       <c r="G5" t="n">
-        <v>109.974375</v>
+        <v>129.274375</v>
       </c>
       <c r="H5" t="n">
-        <v>331.04876</v>
+        <v>236.67561</v>
       </c>
       <c r="I5" t="n">
-        <v>168.4511313251712</v>
+        <v>6.245720480520447</v>
       </c>
       <c r="J5" t="n">
-        <v>343.6436667375286</v>
+        <v>254.6760004753406</v>
       </c>
       <c r="K5" t="n">
-        <v>208.2504509184436</v>
+        <v>25.68334944987578</v>
       </c>
       <c r="L5" t="n">
-        <v>295.2392794800062</v>
+        <v>352.213096848776</v>
       </c>
       <c r="M5" t="n">
-        <v>65.7495863614502</v>
+        <v>69.74855808352319</v>
       </c>
       <c r="N5" t="n">
-        <v>156.3613472699782</v>
+        <v>220.9933612223552</v>
       </c>
       <c r="O5" t="n">
-        <v>23.23628140485065</v>
+        <v>26.43652829712439</v>
       </c>
       <c r="P5" t="n">
-        <v>304.832294121893</v>
+        <v>225.9970780602462</v>
       </c>
       <c r="Q5" t="n">
-        <v>47.95110967637712</v>
+        <v>43.2411067836966</v>
       </c>
       <c r="R5" t="n">
-        <v>315.7847527851116</v>
+        <v>234.1170302542656</v>
       </c>
       <c r="S5" t="n">
-        <v>45.24910193160209</v>
+        <v>40.80450403955298</v>
       </c>
       <c r="T5" t="n">
-        <v>179.5976286748288</v>
+        <v>247.4298895194796</v>
       </c>
       <c r="U5" t="n">
-        <v>352.7834037982701</v>
+        <v>269.2381848439428</v>
       </c>
       <c r="V5" t="n">
-        <v>0.3373479100871307</v>
+        <v>0.4788952555745457</v>
       </c>
       <c r="W5" t="n">
-        <v>0.6626520899128693</v>
+        <v>0.5211047444254542</v>
       </c>
       <c r="X5" t="n">
-        <v>532.3810324730989</v>
+        <v>516.6680743634224</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.6019068363636364</v>
+        <v>0.4303192909090909</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.6248066667955066</v>
+        <v>0.4630472735915283</v>
       </c>
       <c r="AA5" t="n">
         <v>42.57420434696233</v>
       </c>
       <c r="AB5" t="n">
-        <v>18.23641819999999</v>
+        <v>27.35462729999999</v>
       </c>
       <c r="AC5" t="n">
         <v>49.23682159667435</v>
       </c>
       <c r="AD5" t="n">
-        <v>18.23641819999999</v>
+        <v>27.35462729999999</v>
       </c>
     </row>
     <row r="6">
@@ -958,91 +958,91 @@
         <v>5</v>
       </c>
       <c r="B6" t="n">
-        <v>30814.88400066788</v>
+        <v>46074.18461472659</v>
       </c>
       <c r="C6" t="n">
-        <v>37307.80064994509</v>
+        <v>28677.4375998662</v>
       </c>
       <c r="D6" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E6" t="n">
         <v>200</v>
       </c>
       <c r="F6" t="n">
-        <v>115.47309375</v>
+        <v>148.66553125</v>
       </c>
       <c r="G6" t="n">
-        <v>115.47309375</v>
+        <v>148.66553125</v>
       </c>
       <c r="H6" t="n">
-        <v>369.30801</v>
+        <v>501.17653</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>550</v>
+        <v>444.0458791178212</v>
       </c>
       <c r="K6" t="n">
-        <v>120.7063028181639</v>
+        <v>33.71441527875987</v>
       </c>
       <c r="L6" t="n">
-        <v>428.448961551108</v>
+        <v>421.8029240388513</v>
       </c>
       <c r="M6" t="n">
-        <v>86.31017745266422</v>
+        <v>62.61933099667181</v>
       </c>
       <c r="N6" t="n">
-        <v>428.7591868215899</v>
+        <v>545.8371435522724</v>
       </c>
       <c r="O6" t="n">
-        <v>61.54843399851448</v>
+        <v>74.97263276230821</v>
       </c>
       <c r="P6" t="n">
-        <v>500.0425784327534</v>
+        <v>319.4069209950418</v>
       </c>
       <c r="Q6" t="n">
-        <v>137.5015696675262</v>
+        <v>116.6078922938953</v>
       </c>
       <c r="R6" t="n">
-        <v>512.9201567741785</v>
+        <v>327.6325958181712</v>
       </c>
       <c r="S6" t="n">
-        <v>143.9737767651787</v>
+        <v>122.0966327495258</v>
       </c>
       <c r="T6" t="n">
-        <v>392.30801</v>
+        <v>524.17653</v>
       </c>
       <c r="U6" t="n">
-        <v>637.5441481002797</v>
+        <v>436.0148132889371</v>
       </c>
       <c r="V6" t="n">
-        <v>0.4347270043202953</v>
+        <v>0.5874293448712108</v>
       </c>
       <c r="W6" t="n">
-        <v>0.5652729956797048</v>
+        <v>0.4125706551287892</v>
       </c>
       <c r="X6" t="n">
-        <v>1127.851768920384</v>
+        <v>1056.824589603518</v>
       </c>
       <c r="Y6" t="n">
-        <v>0.6714691090909092</v>
+        <v>0.9112300545454546</v>
       </c>
       <c r="Z6" t="n">
-        <v>1</v>
+        <v>0.8073561438505841</v>
       </c>
       <c r="AA6" t="n">
         <v>44.03391412856743</v>
       </c>
       <c r="AB6" t="n">
-        <v>18.25465461819999</v>
+        <v>27.38198192729999</v>
       </c>
       <c r="AC6" t="n">
         <v>47.32713070501108</v>
       </c>
       <c r="AD6" t="n">
-        <v>18.25465461819999</v>
+        <v>27.38198192729999</v>
       </c>
     </row>
     <row r="7">
@@ -1050,91 +1050,91 @@
         <v>6</v>
       </c>
       <c r="B7" t="n">
-        <v>11004.2914012426</v>
+        <v>7710.094182239027</v>
       </c>
       <c r="C7" t="n">
-        <v>5389.751111758396</v>
+        <v>8745.371238840322</v>
       </c>
       <c r="D7" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F7" t="n">
-        <v>121.2467484375</v>
+        <v>126.3657015625</v>
       </c>
       <c r="G7" t="n">
-        <v>121.2467484375</v>
+        <v>126.3657015625</v>
       </c>
       <c r="H7" t="n">
-        <v>532.04476</v>
+        <v>544.76405</v>
       </c>
       <c r="I7" t="n">
-        <v>260.1490288362075</v>
+        <v>315.6504345915594</v>
       </c>
       <c r="J7" t="n">
-        <v>358.6453278208339</v>
+        <v>288.8007998638875</v>
       </c>
       <c r="K7" t="n">
-        <v>194.7765414514787</v>
+        <v>14.77570374713758</v>
       </c>
       <c r="L7" t="n">
-        <v>382.0614233352869</v>
+        <v>432.9052079447526</v>
       </c>
       <c r="M7" t="n">
-        <v>126.9833371793816</v>
+        <v>88.85883950774226</v>
       </c>
       <c r="N7" t="n">
-        <v>230.2846373773471</v>
+        <v>207.6959318539701</v>
       </c>
       <c r="O7" t="n">
-        <v>64.61109378644538</v>
+        <v>44.41768355447051</v>
       </c>
       <c r="P7" t="n">
-        <v>220.9579886862253</v>
+        <v>232.6383174332856</v>
       </c>
       <c r="Q7" t="n">
-        <v>63.61710050129378</v>
+        <v>75.10119396222422</v>
       </c>
       <c r="R7" t="n">
-        <v>213.5780764052037</v>
+        <v>224.8682866411419</v>
       </c>
       <c r="S7" t="n">
-        <v>65.7735542337941</v>
+        <v>77.64692850150543</v>
       </c>
       <c r="T7" t="n">
-        <v>294.8957311637925</v>
+        <v>252.1136154084406</v>
       </c>
       <c r="U7" t="n">
-        <v>284.5750891875191</v>
+        <v>307.7395113955098</v>
       </c>
       <c r="V7" t="n">
-        <v>0.5089052300942577</v>
+        <v>0.4503209919496008</v>
       </c>
       <c r="W7" t="n">
-        <v>0.4910947699057422</v>
+        <v>0.5496790080503993</v>
       </c>
       <c r="X7" t="n">
-        <v>579.4708203513117</v>
+        <v>559.8531268039503</v>
       </c>
       <c r="Y7" t="n">
-        <v>0.9673541090909091</v>
+        <v>0.9904800909090909</v>
       </c>
       <c r="Z7" t="n">
-        <v>0.652082414219698</v>
+        <v>0.5250923633888863</v>
       </c>
       <c r="AA7" t="n">
         <v>44.85129837711415</v>
       </c>
       <c r="AB7" t="n">
-        <v>18.27290927281819</v>
+        <v>27.40936390922728</v>
       </c>
       <c r="AC7" t="n">
         <v>52.06926873704028</v>
       </c>
       <c r="AD7" t="n">
-        <v>18.27290927281819</v>
+        <v>27.40936390922728</v>
       </c>
     </row>
     <row r="8">
@@ -1142,10 +1142,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="n">
-        <v>28193.19606571367</v>
+        <v>26888.67812380631</v>
       </c>
       <c r="C8" t="n">
-        <v>26238.0474522385</v>
+        <v>20810.70579753722</v>
       </c>
       <c r="D8" t="n">
         <v>140</v>
@@ -1154,79 +1154,79 @@
         <v>180</v>
       </c>
       <c r="F8" t="n">
-        <v>127.3090858593751</v>
+        <v>145.3205567968749</v>
       </c>
       <c r="G8" t="n">
-        <v>127.3090858593751</v>
+        <v>145.3205567968749</v>
       </c>
       <c r="H8" t="n">
-        <v>265.78845</v>
+        <v>251.82626</v>
       </c>
       <c r="I8" t="n">
         <v>0</v>
       </c>
       <c r="J8" t="n">
-        <v>477.164018952656</v>
+        <v>377.1957484500535</v>
       </c>
       <c r="K8" t="n">
-        <v>186.1480004148531</v>
+        <v>7.871411140862904</v>
       </c>
       <c r="L8" t="n">
-        <v>382.7784761141201</v>
+        <v>420.4004623718648</v>
       </c>
       <c r="M8" t="n">
-        <v>119.1590043016204</v>
+        <v>123.0762299122076</v>
       </c>
       <c r="N8" t="n">
-        <v>255.767649388604</v>
+        <v>328.1266461942839</v>
       </c>
       <c r="O8" t="n">
-        <v>66.87663830632987</v>
+        <v>73.68053233322486</v>
       </c>
       <c r="P8" t="n">
-        <v>373.9349461488908</v>
+        <v>282.6525714433014</v>
       </c>
       <c r="Q8" t="n">
-        <v>111.8576138403907</v>
+        <v>101.4474696130268</v>
       </c>
       <c r="R8" t="n">
-        <v>371.0599454023582</v>
+        <v>280.4793957016972</v>
       </c>
       <c r="S8" t="n">
-        <v>100.8806150017765</v>
+        <v>91.49205649549397</v>
       </c>
       <c r="T8" t="n">
-        <v>289.78845</v>
+        <v>275.82626</v>
       </c>
       <c r="U8" t="n">
-        <v>485.7925599892816</v>
+        <v>384.1000410563282</v>
       </c>
       <c r="V8" t="n">
-        <v>0.3990964645156332</v>
+        <v>0.5112654121440423</v>
       </c>
       <c r="W8" t="n">
-        <v>0.6009035354843668</v>
+        <v>0.4887345878559577</v>
       </c>
       <c r="X8" t="n">
-        <v>808.4368476842154</v>
+        <v>785.907219583837</v>
       </c>
       <c r="Y8" t="n">
-        <v>0.4832517272727273</v>
+        <v>0.4578659272727272</v>
       </c>
       <c r="Z8" t="n">
-        <v>0.8675709435502835</v>
+        <v>0.6858104517273701</v>
       </c>
       <c r="AA8" t="n">
         <v>46.56781336542775</v>
       </c>
       <c r="AB8" t="n">
-        <v>18.291182182091</v>
+        <v>27.43677327313651</v>
       </c>
       <c r="AC8" t="n">
         <v>52.76029221893338</v>
       </c>
       <c r="AD8" t="n">
-        <v>18.291182182091</v>
+        <v>27.43677327313651</v>
       </c>
     </row>
     <row r="9">
@@ -1234,91 +1234,91 @@
         <v>8</v>
       </c>
       <c r="B9" t="n">
-        <v>29608.0165144758</v>
+        <v>27050.11439414333</v>
       </c>
       <c r="C9" t="n">
-        <v>27576.43845553474</v>
+        <v>25897.988321416</v>
       </c>
       <c r="D9" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E9" t="n">
         <v>180</v>
       </c>
       <c r="F9" t="n">
-        <v>120.9436315664063</v>
+        <v>123.5224732773437</v>
       </c>
       <c r="G9" t="n">
-        <v>120.9436315664063</v>
+        <v>123.5224732773437</v>
       </c>
       <c r="H9" t="n">
-        <v>549.03409</v>
+        <v>482.95391</v>
       </c>
       <c r="I9" t="n">
-        <v>101.9789013657778</v>
+        <v>144.074130716394</v>
       </c>
       <c r="J9" t="n">
-        <v>511.3856329398774</v>
+        <v>550</v>
       </c>
       <c r="K9" t="n">
-        <v>168.9269837990555</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
-        <v>435.0043994573223</v>
+        <v>379.0392056396541</v>
       </c>
       <c r="M9" t="n">
-        <v>89.02968660533621</v>
+        <v>78.91470074627166</v>
       </c>
       <c r="N9" t="n">
-        <v>386.63630407365</v>
+        <v>277.0286442878916</v>
       </c>
       <c r="O9" t="n">
-        <v>85.41888456057215</v>
+        <v>86.85113499571443</v>
       </c>
       <c r="P9" t="n">
-        <v>374.7103287484329</v>
+        <v>456.8452503651537</v>
       </c>
       <c r="Q9" t="n">
-        <v>153.8963208072421</v>
+        <v>151.7776217184527</v>
       </c>
       <c r="R9" t="n">
-        <v>355.5506357812835</v>
+        <v>433.4858336131983</v>
       </c>
       <c r="S9" t="n">
-        <v>141.9829975734469</v>
+        <v>140.0283098589873</v>
       </c>
       <c r="T9" t="n">
-        <v>472.0551886342222</v>
+        <v>363.879779283606</v>
       </c>
       <c r="U9" t="n">
-        <v>528.6066495556749</v>
+        <v>557.8714111408628</v>
       </c>
       <c r="V9" t="n">
-        <v>0.4717429711201194</v>
+        <v>0.3741684187411092</v>
       </c>
       <c r="W9" t="n">
-        <v>0.5282570288798807</v>
+        <v>0.6258315812588908</v>
       </c>
       <c r="X9" t="n">
-        <v>1000.661838189897</v>
+        <v>972.5026513672124</v>
       </c>
       <c r="Y9" t="n">
-        <v>0.9982438</v>
+        <v>0.8780980181818182</v>
       </c>
       <c r="Z9" t="n">
-        <v>0.9297920598906861</v>
+        <v>1</v>
       </c>
       <c r="AA9" t="n">
         <v>48.87610588788633</v>
       </c>
       <c r="AB9" t="n">
-        <v>18.30947336427309</v>
+        <v>27.46421004640964</v>
       </c>
       <c r="AC9" t="n">
         <v>50.73882295981808</v>
       </c>
       <c r="AD9" t="n">
-        <v>18.30947336427309</v>
+        <v>27.46421004640964</v>
       </c>
     </row>
     <row r="10">
@@ -1326,10 +1326,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="n">
-        <v>6694.30867306047</v>
+        <v>2674.787942977335</v>
       </c>
       <c r="C10" t="n">
-        <v>9197.314443436866</v>
+        <v>4513.315682887849</v>
       </c>
       <c r="D10" t="n">
         <v>120</v>
@@ -1338,79 +1338,79 @@
         <v>200</v>
       </c>
       <c r="F10" t="n">
-        <v>114.896449988086</v>
+        <v>104.9941022857421</v>
       </c>
       <c r="G10" t="n">
-        <v>114.896449988086</v>
+        <v>104.9941022857421</v>
       </c>
       <c r="H10" t="n">
-        <v>473.56287</v>
+        <v>450.38433</v>
       </c>
       <c r="I10" t="n">
-        <v>233.5255713919689</v>
+        <v>253.1752952443417</v>
       </c>
       <c r="J10" t="n">
-        <v>376.9243454402647</v>
+        <v>419.3464727748802</v>
       </c>
       <c r="K10" t="n">
-        <v>210.9829944423477</v>
+        <v>32.77177881203096</v>
       </c>
       <c r="L10" t="n">
-        <v>465.3871663633701</v>
+        <v>482.6938962499115</v>
       </c>
       <c r="M10" t="n">
-        <v>93.15460533518568</v>
+        <v>94.76455958902415</v>
       </c>
       <c r="N10" t="n">
-        <v>229.6397867606142</v>
+        <v>188.8198961160242</v>
       </c>
       <c r="O10" t="n">
-        <v>27.39751184741687</v>
+        <v>25.38913863963403</v>
       </c>
       <c r="P10" t="n">
-        <v>273.23340650222</v>
+        <v>321.9353167140761</v>
       </c>
       <c r="Q10" t="n">
-        <v>61.63492829475249</v>
+        <v>64.63937724877319</v>
       </c>
       <c r="R10" t="n">
-        <v>282.9124616535498</v>
+        <v>333.3395945640141</v>
       </c>
       <c r="S10" t="n">
-        <v>62.93886758577036</v>
+        <v>66.00687821086611</v>
       </c>
       <c r="T10" t="n">
-        <v>257.0372986080311</v>
+        <v>214.2090347556583</v>
       </c>
       <c r="U10" t="n">
-        <v>334.8683347969725</v>
+        <v>386.5746939628493</v>
       </c>
       <c r="V10" t="n">
-        <v>0.4342538474070523</v>
+        <v>0.3565493280128833</v>
       </c>
       <c r="W10" t="n">
-        <v>0.5657461525929477</v>
+        <v>0.6434506719871167</v>
       </c>
       <c r="X10" t="n">
-        <v>591.9056334050035</v>
+        <v>600.7837287185075</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.8610234</v>
+        <v>0.8188806</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.6853169917095722</v>
+        <v>0.762448132317964</v>
       </c>
       <c r="AA10" t="n">
         <v>50.01050022591366</v>
       </c>
       <c r="AB10" t="n">
-        <v>18.32778283763736</v>
+        <v>27.49167425645605</v>
       </c>
       <c r="AC10" t="n">
         <v>49.81270675589048</v>
       </c>
       <c r="AD10" t="n">
-        <v>18.32778283763736</v>
+        <v>27.49167425645605</v>
       </c>
     </row>
     <row r="11">
@@ -1418,76 +1418,76 @@
         <v>10</v>
       </c>
       <c r="B11" t="n">
-        <v>23418.21892574612</v>
+        <v>17467.72268465314</v>
       </c>
       <c r="C11" t="n">
-        <v>29096.37476075658</v>
+        <v>9897.277976413454</v>
       </c>
       <c r="D11" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E11" t="n">
         <v>140</v>
       </c>
       <c r="F11" t="n">
-        <v>120.6412724874903</v>
+        <v>89.24498694288081</v>
       </c>
       <c r="G11" t="n">
-        <v>120.6412724874903</v>
+        <v>89.24498694288081</v>
       </c>
       <c r="H11" t="n">
-        <v>295.37939</v>
+        <v>531.27264</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>117.0793367943335</v>
       </c>
       <c r="J11" t="n">
         <v>550</v>
       </c>
       <c r="K11" t="n">
-        <v>209.086061456265</v>
+        <v>0</v>
       </c>
       <c r="L11" t="n">
-        <v>372.8828202609234</v>
+        <v>628.8734929157722</v>
       </c>
       <c r="M11" t="n">
-        <v>138.0221364886003</v>
+        <v>137.5744426499662</v>
       </c>
       <c r="N11" t="n">
-        <v>417.8301914009173</v>
+        <v>341.8692555441909</v>
       </c>
       <c r="O11" t="n">
-        <v>114.3410242193857</v>
+        <v>90.3240476614756</v>
       </c>
       <c r="P11" t="n">
-        <v>409.0168375773614</v>
+        <v>538.656291466473</v>
       </c>
       <c r="Q11" t="n">
-        <v>142.8800954087213</v>
+        <v>175.4942005006191</v>
       </c>
       <c r="R11" t="n">
-        <v>445.7339482600489</v>
+        <v>587.0110310680172</v>
       </c>
       <c r="S11" t="n">
-        <v>129.4899964389384</v>
+        <v>159.047649939436</v>
       </c>
       <c r="T11" t="n">
-        <v>313.37939</v>
+        <v>432.1933032056665</v>
       </c>
       <c r="U11" t="n">
-        <v>551.8969329860827</v>
+        <v>582.771778812031</v>
       </c>
       <c r="V11" t="n">
-        <v>0.4909019938501385</v>
+        <v>0.377018923141232</v>
       </c>
       <c r="W11" t="n">
-        <v>0.5090980061498614</v>
+        <v>0.622981076858768</v>
       </c>
       <c r="X11" t="n">
-        <v>1084.068148606386</v>
+        <v>1146.343795172759</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.5370534363636363</v>
+        <v>0.9659502545454546</v>
       </c>
       <c r="Z11" t="n">
         <v>1</v>
@@ -1496,13 +1496,13 @@
         <v>48.03079820245372</v>
       </c>
       <c r="AB11" t="n">
-        <v>18.346110620475</v>
+        <v>27.5191659307125</v>
       </c>
       <c r="AC11" t="n">
         <v>49.04843736809783</v>
       </c>
       <c r="AD11" t="n">
-        <v>18.346110620475</v>
+        <v>27.5191659307125</v>
       </c>
     </row>
     <row r="12">
@@ -1510,91 +1510,91 @@
         <v>11</v>
       </c>
       <c r="B12" t="n">
-        <v>22585.18164498634</v>
+        <v>26396.6957624931</v>
       </c>
       <c r="C12" t="n">
-        <v>20920.61684259318</v>
+        <v>6422.820829817741</v>
       </c>
       <c r="D12" t="n">
+        <v>100</v>
+      </c>
+      <c r="E12" t="n">
         <v>120</v>
       </c>
-      <c r="E12" t="n">
-        <v>180</v>
-      </c>
       <c r="F12" t="n">
-        <v>114.6092088631158</v>
+        <v>102.6317349843129</v>
       </c>
       <c r="G12" t="n">
-        <v>114.6092088631158</v>
+        <v>102.6317349843129</v>
       </c>
       <c r="H12" t="n">
-        <v>538.49733</v>
+        <v>446.83877</v>
       </c>
       <c r="I12" t="n">
-        <v>163.7976306228127</v>
+        <v>0</v>
       </c>
       <c r="J12" t="n">
-        <v>531.1230447400209</v>
+        <v>512.8908879351565</v>
       </c>
       <c r="K12" t="n">
-        <v>227.5635873602704</v>
+        <v>45.14938816497272</v>
       </c>
       <c r="L12" t="n">
-        <v>410.9122157706648</v>
+        <v>439.9893618625421</v>
       </c>
       <c r="M12" t="n">
-        <v>102.585112339714</v>
+        <v>98.9287421082152</v>
       </c>
       <c r="N12" t="n">
-        <v>356.327550424595</v>
+        <v>433.5191440681202</v>
       </c>
       <c r="O12" t="n">
-        <v>43.37214895259229</v>
+        <v>60.93625239647878</v>
       </c>
       <c r="P12" t="n">
-        <v>428.2351122410087</v>
+        <v>390.7366378573326</v>
       </c>
       <c r="Q12" t="n">
-        <v>84.41040659500683</v>
+        <v>77.00486191285117</v>
       </c>
       <c r="R12" t="n">
-        <v>452.2789595740317</v>
+        <v>412.6750819491683</v>
       </c>
       <c r="S12" t="n">
-        <v>87.93014662225424</v>
+        <v>80.21580598598817</v>
       </c>
       <c r="T12" t="n">
-        <v>399.6996993771873</v>
+        <v>471.83877</v>
       </c>
       <c r="U12" t="n">
-        <v>512.6455188360155</v>
+        <v>467.7414997701837</v>
       </c>
       <c r="V12" t="n">
-        <v>0.4381013802647923</v>
+        <v>0.5138817204664402</v>
       </c>
       <c r="W12" t="n">
-        <v>0.5618986197352077</v>
+        <v>0.4861182795335598</v>
       </c>
       <c r="X12" t="n">
-        <v>912.3452182132028</v>
+        <v>962.1968962347827</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.9790860545454546</v>
+        <v>0.8124341272727273</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.9656782631636743</v>
+        <v>0.93252888715483</v>
       </c>
       <c r="AA12" t="n">
         <v>46.5205408149944</v>
       </c>
       <c r="AB12" t="n">
-        <v>18.36445673109547</v>
+        <v>27.54668509664321</v>
       </c>
       <c r="AC12" t="n">
         <v>51.35853620313758</v>
       </c>
       <c r="AD12" t="n">
-        <v>18.36445673109547</v>
+        <v>27.54668509664321</v>
       </c>
     </row>
     <row r="13">
@@ -1602,10 +1602,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="n">
-        <v>32828.40881212088</v>
+        <v>28135.05091442783</v>
       </c>
       <c r="C13" t="n">
-        <v>34383.79959164998</v>
+        <v>26899.49050976741</v>
       </c>
       <c r="D13" t="n">
         <v>140</v>
@@ -1614,64 +1614,64 @@
         <v>140</v>
       </c>
       <c r="F13" t="n">
-        <v>120.3396693062716</v>
+        <v>118.0264952319599</v>
       </c>
       <c r="G13" t="n">
-        <v>120.3396693062716</v>
+        <v>118.0264952319599</v>
       </c>
       <c r="H13" t="n">
-        <v>383.01665</v>
+        <v>442.00462</v>
       </c>
       <c r="I13" t="n">
-        <v>49.91369772353517</v>
+        <v>122.6132094486388</v>
       </c>
       <c r="J13" t="n">
         <v>550</v>
       </c>
       <c r="K13" t="n">
-        <v>170.8302417871137</v>
+        <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>352.1814714682206</v>
+        <v>261.1423724677961</v>
       </c>
       <c r="M13" t="n">
-        <v>170.6328049625219</v>
+        <v>156.8622457922285</v>
       </c>
       <c r="N13" t="n">
-        <v>276.0263727449985</v>
+        <v>263.4210934235148</v>
       </c>
       <c r="O13" t="n">
-        <v>81.07657953146638</v>
+        <v>79.9703171278464</v>
       </c>
       <c r="P13" t="n">
-        <v>505.0413972423634</v>
+        <v>520.6264972277474</v>
       </c>
       <c r="Q13" t="n">
-        <v>101.6919483307933</v>
+        <v>103.2481343998499</v>
       </c>
       <c r="R13" t="n">
-        <v>522.9138812971395</v>
+        <v>539.0505092414231</v>
       </c>
       <c r="S13" t="n">
-        <v>108.5644605299877</v>
+        <v>110.2258162601567</v>
       </c>
       <c r="T13" t="n">
-        <v>357.1029522764649</v>
+        <v>343.3914105513612</v>
       </c>
       <c r="U13" t="n">
-        <v>606.7333455731567</v>
+        <v>595.1493881649727</v>
       </c>
       <c r="V13" t="n">
-        <v>0.3705016641033168</v>
+        <v>0.3550123705137047</v>
       </c>
       <c r="W13" t="n">
-        <v>0.6294983358966832</v>
+        <v>0.6449876294862952</v>
       </c>
       <c r="X13" t="n">
-        <v>963.8362978496216</v>
+        <v>967.2660421789585</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.6963939090909091</v>
+        <v>0.8036447636363636</v>
       </c>
       <c r="Z13" t="n">
         <v>1</v>
@@ -1680,13 +1680,13 @@
         <v>44.55727214766546</v>
       </c>
       <c r="AB13" t="n">
-        <v>18.38282118782656</v>
+        <v>27.57423178173985</v>
       </c>
       <c r="AC13" t="n">
         <v>51.23286988151392</v>
       </c>
       <c r="AD13" t="n">
-        <v>18.38282118782656</v>
+        <v>27.57423178173985</v>
       </c>
     </row>
     <row r="14">
@@ -1694,10 +1694,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="n">
-        <v>16513.80037270651</v>
+        <v>25836.40008673088</v>
       </c>
       <c r="C14" t="n">
-        <v>15477.982626571</v>
+        <v>10279.69767270541</v>
       </c>
       <c r="D14" t="n">
         <v>130</v>
@@ -1706,79 +1706,79 @@
         <v>140</v>
       </c>
       <c r="F14" t="n">
-        <v>126.3566527715851</v>
+        <v>135.7304695167538</v>
       </c>
       <c r="G14" t="n">
-        <v>126.3566527715851</v>
+        <v>135.7304695167538</v>
       </c>
       <c r="H14" t="n">
-        <v>494.83345</v>
+        <v>402.78395</v>
       </c>
       <c r="I14" t="n">
-        <v>204.9354677848784</v>
+        <v>76.39613143827512</v>
       </c>
       <c r="J14" t="n">
-        <v>352.8930298840216</v>
+        <v>301.56865871796</v>
       </c>
       <c r="K14" t="n">
-        <v>175.081053299742</v>
+        <v>0</v>
       </c>
       <c r="L14" t="n">
-        <v>448.295024694162</v>
+        <v>430.0018452445139</v>
       </c>
       <c r="M14" t="n">
-        <v>77.45212380767674</v>
+        <v>76.39531587196829</v>
       </c>
       <c r="N14" t="n">
-        <v>253.10225825374</v>
+        <v>286.9541637648199</v>
       </c>
       <c r="O14" t="n">
-        <v>55.79572396138168</v>
+        <v>58.43365479690497</v>
       </c>
       <c r="P14" t="n">
-        <v>283.5787300671023</v>
+        <v>241.4838838855446</v>
       </c>
       <c r="Q14" t="n">
-        <v>65.06348830429103</v>
+        <v>61.21212611823439</v>
       </c>
       <c r="R14" t="n">
-        <v>257.6223309888761</v>
+        <v>219.3804910830941</v>
       </c>
       <c r="S14" t="n">
-        <v>66.10094068225931</v>
+        <v>62.1881676348659</v>
       </c>
       <c r="T14" t="n">
-        <v>308.8979822151217</v>
+        <v>345.3878185617249</v>
       </c>
       <c r="U14" t="n">
-        <v>348.6422183713933</v>
+        <v>301.56865871796</v>
       </c>
       <c r="V14" t="n">
-        <v>0.4697780940839659</v>
+        <v>0.5329369494162829</v>
       </c>
       <c r="W14" t="n">
-        <v>0.530221905916034</v>
+        <v>0.4670630505837172</v>
       </c>
       <c r="X14" t="n">
-        <v>657.540200586515</v>
+        <v>648.0838285655038</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.8996971818181819</v>
+        <v>0.7323344545454545</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.6416236906982211</v>
+        <v>0.5483066522144728</v>
       </c>
       <c r="AA14" t="n">
         <v>46.95128508327306</v>
       </c>
       <c r="AB14" t="n">
-        <v>18.40120400901439</v>
+        <v>27.60180601352159</v>
       </c>
       <c r="AC14" t="n">
         <v>51.30295941546635</v>
       </c>
       <c r="AD14" t="n">
-        <v>18.40120400901439</v>
+        <v>27.60180601352159</v>
       </c>
     </row>
     <row r="15">
@@ -1786,10 +1786,10 @@
         <v>14</v>
       </c>
       <c r="B15" t="n">
-        <v>28713.48182528131</v>
+        <v>46462.72729779422</v>
       </c>
       <c r="C15" t="n">
-        <v>39248.32898243965</v>
+        <v>26920.35228317486</v>
       </c>
       <c r="D15" t="n">
         <v>140</v>
@@ -1798,79 +1798,79 @@
         <v>180</v>
       </c>
       <c r="F15" t="n">
-        <v>132.6744854101644</v>
+        <v>156.0900399442669</v>
       </c>
       <c r="G15" t="n">
-        <v>132.6744854101644</v>
+        <v>156.0900399442669</v>
       </c>
       <c r="H15" t="n">
-        <v>289.23733</v>
+        <v>482.13747</v>
       </c>
       <c r="I15" t="n">
         <v>0</v>
       </c>
       <c r="J15" t="n">
-        <v>550</v>
+        <v>463.2074266289</v>
       </c>
       <c r="K15" t="n">
-        <v>139.9400181232714</v>
+        <v>41.91105114435618</v>
       </c>
       <c r="L15" t="n">
-        <v>370.8672816538979</v>
+        <v>429.2262858873523</v>
       </c>
       <c r="M15" t="n">
-        <v>108.3055132422788</v>
+        <v>114.3073141517187</v>
       </c>
       <c r="N15" t="n">
-        <v>381.6735785158091</v>
+        <v>498.4473983176462</v>
       </c>
       <c r="O15" t="n">
-        <v>71.09546708543115</v>
+        <v>79.63668463074222</v>
       </c>
       <c r="P15" t="n">
-        <v>473.1862609171917</v>
+        <v>322.7133154014194</v>
       </c>
       <c r="Q15" t="n">
-        <v>111.9547742592789</v>
+        <v>98.58306008312437</v>
       </c>
       <c r="R15" t="n">
-        <v>514.3993186458754</v>
+        <v>350.8206456347059</v>
       </c>
       <c r="S15" t="n">
-        <v>104.9180376631156</v>
+        <v>92.38678099419403</v>
       </c>
       <c r="T15" t="n">
-        <v>304.23733</v>
+        <v>497.13747</v>
       </c>
       <c r="U15" t="n">
-        <v>585.1410351764706</v>
+        <v>421.2963754845438</v>
       </c>
       <c r="V15" t="n">
-        <v>0.43623147514087</v>
+        <v>0.5784424520916158</v>
       </c>
       <c r="W15" t="n">
-        <v>0.5637685248591301</v>
+        <v>0.4215575479083842</v>
       </c>
       <c r="X15" t="n">
-        <v>1037.910080777711</v>
+        <v>999.3804584329322</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.5258860545454546</v>
+        <v>0.8766135818181818</v>
       </c>
       <c r="Z15" t="n">
-        <v>1</v>
+        <v>0.8421953211434544</v>
       </c>
       <c r="AA15" t="n">
         <v>47.98738936885736</v>
       </c>
       <c r="AB15" t="n">
-        <v>18.4196052130234</v>
+        <v>27.6294078195351</v>
       </c>
       <c r="AC15" t="n">
         <v>50.86235245192742</v>
       </c>
       <c r="AD15" t="n">
-        <v>18.4196052130234</v>
+        <v>27.6294078195351</v>
       </c>
     </row>
     <row r="16">
@@ -1878,91 +1878,91 @@
         <v>15</v>
       </c>
       <c r="B16" t="n">
-        <v>22784.85985374062</v>
+        <v>24354.22869206125</v>
       </c>
       <c r="C16" t="n">
-        <v>17203.66725954727</v>
+        <v>19819.82421222327</v>
       </c>
       <c r="D16" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E16" t="n">
         <v>200</v>
       </c>
       <c r="F16" t="n">
-        <v>126.0407611396562</v>
+        <v>132.6765339526268</v>
       </c>
       <c r="G16" t="n">
-        <v>126.0407611396562</v>
+        <v>132.6765339526268</v>
       </c>
       <c r="H16" t="n">
-        <v>542.18412</v>
+        <v>523.24116</v>
       </c>
       <c r="I16" t="n">
-        <v>149.4757316292862</v>
+        <v>157.4100066560187</v>
       </c>
       <c r="J16" t="n">
-        <v>436.4688214816807</v>
+        <v>362.0333854541295</v>
       </c>
       <c r="K16" t="n">
-        <v>184.6912978853018</v>
+        <v>4.440027138975665</v>
       </c>
       <c r="L16" t="n">
-        <v>463.822811230769</v>
+        <v>432.9583475816503</v>
       </c>
       <c r="M16" t="n">
-        <v>56.36131020211157</v>
+        <v>68.28281701331748</v>
       </c>
       <c r="N16" t="n">
-        <v>370.5165616882077</v>
+        <v>341.8124335271164</v>
       </c>
       <c r="O16" t="n">
-        <v>44.19182668250605</v>
+        <v>46.01871981686503</v>
       </c>
       <c r="P16" t="n">
-        <v>304.4427855260178</v>
+        <v>315.0547421257045</v>
       </c>
       <c r="Q16" t="n">
-        <v>87.27475619363256</v>
+        <v>84.44966733380556</v>
       </c>
       <c r="R16" t="n">
-        <v>293.3339471438191</v>
+        <v>303.5586831674585</v>
       </c>
       <c r="S16" t="n">
-        <v>83.07489246113305</v>
+        <v>80.38575343102717</v>
       </c>
       <c r="T16" t="n">
-        <v>414.7083883707138</v>
+        <v>387.8311533439814</v>
       </c>
       <c r="U16" t="n">
-        <v>391.7175417196504</v>
+        <v>399.50440945951</v>
       </c>
       <c r="V16" t="n">
-        <v>0.5142547788911545</v>
+        <v>0.4925868608843456</v>
       </c>
       <c r="W16" t="n">
-        <v>0.4857452211088455</v>
+        <v>0.5074131391156543</v>
       </c>
       <c r="X16" t="n">
-        <v>806.4259300903642</v>
+        <v>787.3355628034915</v>
       </c>
       <c r="Y16" t="n">
-        <v>0.9857893090909091</v>
+        <v>0.9513475636363637</v>
       </c>
       <c r="Z16" t="n">
-        <v>0.7935796754212376</v>
+        <v>0.6582425190075082</v>
       </c>
       <c r="AA16" t="n">
         <v>49.21058050812418</v>
       </c>
       <c r="AB16" t="n">
-        <v>18.43802481823642</v>
+        <v>27.65703722735464</v>
       </c>
       <c r="AC16" t="n">
         <v>49.62190318939171</v>
       </c>
       <c r="AD16" t="n">
-        <v>18.43802481823642</v>
+        <v>27.65703722735464</v>
       </c>
     </row>
     <row r="17">
@@ -1970,10 +1970,10 @@
         <v>16</v>
       </c>
       <c r="B17" t="n">
-        <v>10757.80626807409</v>
+        <v>-116.9350957104143</v>
       </c>
       <c r="C17" t="n">
-        <v>9912.28490087208</v>
+        <v>5403.458485484054</v>
       </c>
       <c r="D17" t="n">
         <v>130</v>
@@ -1982,79 +1982,79 @@
         <v>160</v>
       </c>
       <c r="F17" t="n">
-        <v>132.342799196639</v>
+        <v>112.7750538597328</v>
       </c>
       <c r="G17" t="n">
-        <v>132.342799196639</v>
+        <v>112.7750538597328</v>
       </c>
       <c r="H17" t="n">
-        <v>479.43376</v>
+        <v>525.55707</v>
       </c>
       <c r="I17" t="n">
-        <v>243.6376011029619</v>
+        <v>355.3116423060612</v>
       </c>
       <c r="J17" t="n">
-        <v>261.0426980812229</v>
+        <v>340.5026507177594</v>
       </c>
       <c r="K17" t="n">
-        <v>192.2078285431573</v>
+        <v>10.25755288443469</v>
       </c>
       <c r="L17" t="n">
-        <v>523.671682417233</v>
+        <v>574.5750552876668</v>
       </c>
       <c r="M17" t="n">
-        <v>84.2378068246197</v>
+        <v>87.39202372944604</v>
       </c>
       <c r="N17" t="n">
-        <v>220.4458348052187</v>
+        <v>158.9980516952984</v>
       </c>
       <c r="O17" t="n">
-        <v>36.35032409181945</v>
+        <v>32.2473759986403</v>
       </c>
       <c r="P17" t="n">
-        <v>205.2460778485716</v>
+        <v>280.4775808927423</v>
       </c>
       <c r="Q17" t="n">
-        <v>48.2800895747958</v>
+        <v>54.2075440795581</v>
       </c>
       <c r="R17" t="n">
-        <v>201.1700617877852</v>
+        <v>274.9075298769426</v>
       </c>
       <c r="S17" t="n">
-        <v>44.56393417873937</v>
+        <v>50.0351479797924</v>
       </c>
       <c r="T17" t="n">
-        <v>256.7961588970381</v>
+        <v>191.2454276939388</v>
       </c>
       <c r="U17" t="n">
-        <v>253.5261674233674</v>
+        <v>334.6851249723003</v>
       </c>
       <c r="V17" t="n">
-        <v>0.503203849121445</v>
+        <v>0.3636324733834299</v>
       </c>
       <c r="W17" t="n">
-        <v>0.496796150878555</v>
+        <v>0.6363675266165701</v>
       </c>
       <c r="X17" t="n">
-        <v>510.3223263204055</v>
+        <v>525.9305526662391</v>
       </c>
       <c r="Y17" t="n">
-        <v>0.8716977454545455</v>
+        <v>0.955558309090909</v>
       </c>
       <c r="Z17" t="n">
-        <v>0.4746230874204052</v>
+        <v>0.6190957285777443</v>
       </c>
       <c r="AA17" t="n">
         <v>46.17617913752036</v>
       </c>
       <c r="AB17" t="n">
-        <v>18.45646284305466</v>
+        <v>27.68469426458199</v>
       </c>
       <c r="AC17" t="n">
         <v>50.20101171605364</v>
       </c>
       <c r="AD17" t="n">
-        <v>18.45646284305466</v>
+        <v>27.68469426458199</v>
       </c>
     </row>
     <row r="18">
@@ -2062,91 +2062,91 @@
         <v>17</v>
       </c>
       <c r="B18" t="n">
-        <v>35132.13669510306</v>
+        <v>20088.50277674346</v>
       </c>
       <c r="C18" t="n">
-        <v>23291.29106637952</v>
+        <v>10326.76536716036</v>
       </c>
       <c r="D18" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E18" t="n">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="F18" t="n">
-        <v>125.725659236807</v>
+        <v>95.85879578077288</v>
       </c>
       <c r="G18" t="n">
-        <v>125.725659236807</v>
+        <v>95.85879578077288</v>
       </c>
       <c r="H18" t="n">
-        <v>450.90988</v>
+        <v>343.94474</v>
       </c>
       <c r="I18" t="n">
         <v>0</v>
       </c>
       <c r="J18" t="n">
-        <v>518.6518057944627</v>
+        <v>550</v>
       </c>
       <c r="K18" t="n">
-        <v>230.082804199417</v>
+        <v>0</v>
       </c>
       <c r="L18" t="n">
-        <v>482.3806104475413</v>
+        <v>585.9917045335083</v>
       </c>
       <c r="M18" t="n">
-        <v>192.1668720477867</v>
+        <v>93.26467482074005</v>
       </c>
       <c r="N18" t="n">
-        <v>425.8442837913082</v>
+        <v>383.0300461641487</v>
       </c>
       <c r="O18" t="n">
-        <v>136.5748143266045</v>
+        <v>64.53546141993874</v>
       </c>
       <c r="P18" t="n">
-        <v>353.4229733655945</v>
+        <v>453.6219039487637</v>
       </c>
       <c r="Q18" t="n">
-        <v>127.3538567726084</v>
+        <v>185.5276245525671</v>
       </c>
       <c r="R18" t="n">
-        <v>381.0365079455416</v>
+        <v>489.0641504208206</v>
       </c>
       <c r="S18" t="n">
-        <v>129.8231263920783</v>
+        <v>189.1248279548799</v>
       </c>
       <c r="T18" t="n">
-        <v>470.90988</v>
+        <v>363.94474</v>
       </c>
       <c r="U18" t="n">
-        <v>480.7768301382029</v>
+        <v>560.2575528844347</v>
       </c>
       <c r="V18" t="n">
-        <v>0.5391308409898555</v>
+        <v>0.4118517667670403</v>
       </c>
       <c r="W18" t="n">
-        <v>0.4608691590101444</v>
+        <v>0.5881482332329597</v>
       </c>
       <c r="X18" t="n">
-        <v>1043.195928256116</v>
+        <v>1086.715036085418</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.8198361454545454</v>
+        <v>0.6253540727272727</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.9430032832626595</v>
+        <v>1</v>
       </c>
       <c r="AA18" t="n">
         <v>47.4086948480635</v>
       </c>
       <c r="AB18" t="n">
-        <v>18.47491930589771</v>
+        <v>27.71237895884657</v>
       </c>
       <c r="AC18" t="n">
         <v>51.15825554919748</v>
       </c>
       <c r="AD18" t="n">
-        <v>18.47491930589771</v>
+        <v>27.71237895884657</v>
       </c>
     </row>
     <row r="19">
@@ -2154,76 +2154,76 @@
         <v>18</v>
       </c>
       <c r="B19" t="n">
-        <v>40615.95660353129</v>
+        <v>28183.60794782861</v>
       </c>
       <c r="C19" t="n">
-        <v>35962.40833447084</v>
+        <v>15796.58749808578</v>
       </c>
       <c r="D19" t="n">
-        <v>140</v>
+        <v>120</v>
       </c>
       <c r="E19" t="n">
         <v>200</v>
       </c>
       <c r="F19" t="n">
-        <v>132.0119421986474</v>
+        <v>110.2376151478888</v>
       </c>
       <c r="G19" t="n">
-        <v>132.0119421986474</v>
+        <v>110.2376151478888</v>
       </c>
       <c r="H19" t="n">
-        <v>424.68498</v>
+        <v>363.13101</v>
       </c>
       <c r="I19" t="n">
-        <v>5.87049032480553</v>
+        <v>0</v>
       </c>
       <c r="J19" t="n">
         <v>550</v>
       </c>
       <c r="K19" t="n">
-        <v>203.4850018210881</v>
+        <v>0</v>
       </c>
       <c r="L19" t="n">
-        <v>319.6143007251212</v>
+        <v>271.243282434225</v>
       </c>
       <c r="M19" t="n">
-        <v>90.07068425270036</v>
+        <v>76.88772719081061</v>
       </c>
       <c r="N19" t="n">
-        <v>386.0085935553702</v>
+        <v>389.2342415416834</v>
       </c>
       <c r="O19" t="n">
-        <v>47.80589611982424</v>
+        <v>41.27167737505374</v>
       </c>
       <c r="P19" t="n">
-        <v>488.2327281288533</v>
+        <v>546.4222869686456</v>
       </c>
       <c r="Q19" t="n">
-        <v>88.36507424947567</v>
+        <v>98.31527460481215</v>
       </c>
       <c r="R19" t="n">
-        <v>521.85388522094</v>
+        <v>584.0505500701344</v>
       </c>
       <c r="S19" t="n">
-        <v>95.71364784473111</v>
+        <v>106.4913219527891</v>
       </c>
       <c r="T19" t="n">
-        <v>433.8144896751945</v>
+        <v>378.13101</v>
       </c>
       <c r="U19" t="n">
-        <v>576.597802378329</v>
+        <v>550</v>
       </c>
       <c r="V19" t="n">
-        <v>0.4293440341996695</v>
+        <v>0.4003799388027658</v>
       </c>
       <c r="W19" t="n">
-        <v>0.5706559658003304</v>
+        <v>0.5996200611972341</v>
       </c>
       <c r="X19" t="n">
-        <v>1010.412292053524</v>
+        <v>1075.243480490195</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.7721545090909091</v>
+        <v>0.6602382</v>
       </c>
       <c r="Z19" t="n">
         <v>1</v>
@@ -2232,13 +2232,13 @@
         <v>47.34410661367475</v>
       </c>
       <c r="AB19" t="n">
-        <v>18.49339422520361</v>
+        <v>27.74009133780541</v>
       </c>
       <c r="AC19" t="n">
         <v>53.77645563174561</v>
       </c>
       <c r="AD19" t="n">
-        <v>18.49339422520361</v>
+        <v>27.74009133780541</v>
       </c>
     </row>
     <row r="20">
@@ -2246,76 +2246,76 @@
         <v>19</v>
       </c>
       <c r="B20" t="n">
-        <v>32916.13828994893</v>
+        <v>38522.86096060775</v>
       </c>
       <c r="C20" t="n">
-        <v>29205.41681930564</v>
+        <v>24246.83356600639</v>
       </c>
       <c r="D20" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E20" t="n">
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="F20" t="n">
-        <v>125.411345088715</v>
+        <v>126.7732574200721</v>
       </c>
       <c r="G20" t="n">
-        <v>125.411345088715</v>
+        <v>126.7732574200721</v>
       </c>
       <c r="H20" t="n">
-        <v>521.53077</v>
+        <v>414.91344</v>
       </c>
       <c r="I20" t="n">
-        <v>101.4136127268437</v>
+        <v>22.24095611152296</v>
       </c>
       <c r="J20" t="n">
         <v>550</v>
       </c>
       <c r="K20" t="n">
-        <v>195.4493285211004</v>
+        <v>0</v>
       </c>
       <c r="L20" t="n">
-        <v>436.2828652878078</v>
+        <v>257.2451720373392</v>
       </c>
       <c r="M20" t="n">
-        <v>72.11839849223897</v>
+        <v>138.6682675990833</v>
       </c>
       <c r="N20" t="n">
-        <v>377.9448029961819</v>
+        <v>321.3620066635933</v>
       </c>
       <c r="O20" t="n">
-        <v>61.17235427697433</v>
+        <v>90.3104772248837</v>
       </c>
       <c r="P20" t="n">
-        <v>436.3628470933573</v>
+        <v>477.8094281580175</v>
       </c>
       <c r="Q20" t="n">
-        <v>121.6728262066305</v>
+        <v>104.7938283488745</v>
       </c>
       <c r="R20" t="n">
-        <v>473.2481743788741</v>
+        <v>518.1981946515672</v>
       </c>
       <c r="S20" t="n">
-        <v>121.7305434144821</v>
+        <v>104.8435387678806</v>
       </c>
       <c r="T20" t="n">
-        <v>439.1171572731562</v>
+        <v>411.672483888477</v>
       </c>
       <c r="U20" t="n">
-        <v>558.0356732999877</v>
+        <v>550</v>
       </c>
       <c r="V20" t="n">
-        <v>0.4403709680298057</v>
+        <v>0.4140425710525507</v>
       </c>
       <c r="W20" t="n">
-        <v>0.5596290319701943</v>
+        <v>0.5859574289474493</v>
       </c>
       <c r="X20" t="n">
-        <v>997.152830573144</v>
+        <v>994.275740395369</v>
       </c>
       <c r="Y20" t="n">
-        <v>0.9482377636363636</v>
+        <v>0.7543880727272727</v>
       </c>
       <c r="Z20" t="n">
         <v>1</v>
@@ -2324,13 +2324,13 @@
         <v>45.95369306801917</v>
       </c>
       <c r="AB20" t="n">
-        <v>18.51188761942881</v>
+        <v>27.76783142914321</v>
       </c>
       <c r="AC20" t="n">
         <v>54.92027405273547</v>
       </c>
       <c r="AD20" t="n">
-        <v>18.51188761942881</v>
+        <v>27.76783142914321</v>
       </c>
     </row>
     <row r="21">
@@ -2338,91 +2338,91 @@
         <v>20</v>
       </c>
       <c r="B21" t="n">
-        <v>36585.1967372293</v>
+        <v>41781.77483931413</v>
       </c>
       <c r="C21" t="n">
-        <v>24868.25867651385</v>
+        <v>19200.55005269767</v>
       </c>
       <c r="D21" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E21" t="n">
-        <v>180</v>
+        <v>200</v>
       </c>
       <c r="F21" t="n">
-        <v>119.1407778342793</v>
+        <v>145.7892460330829</v>
       </c>
       <c r="G21" t="n">
-        <v>119.1407778342793</v>
+        <v>145.7892460330829</v>
       </c>
       <c r="H21" t="n">
-        <v>477.33327</v>
+        <v>468.06807</v>
       </c>
       <c r="I21" t="n">
-        <v>7.774902461520014</v>
+        <v>0</v>
       </c>
       <c r="J21" t="n">
-        <v>550</v>
+        <v>457.9053553861876</v>
       </c>
       <c r="K21" t="n">
-        <v>204.201708314088</v>
+        <v>54.88824113560599</v>
       </c>
       <c r="L21" t="n">
-        <v>446.9067498999694</v>
+        <v>413.7604798282769</v>
       </c>
       <c r="M21" t="n">
-        <v>107.8401298372872</v>
+        <v>52.54854943229288</v>
       </c>
       <c r="N21" t="n">
-        <v>452.5473411997388</v>
+        <v>529.6413878156399</v>
       </c>
       <c r="O21" t="n">
-        <v>41.01102633874122</v>
+        <v>42.48448809848143</v>
       </c>
       <c r="P21" t="n">
-        <v>465.7439515201607</v>
+        <v>335.0202940190385</v>
       </c>
       <c r="Q21" t="n">
-        <v>75.5036686868516</v>
+        <v>67.99682023154308</v>
       </c>
       <c r="R21" t="n">
-        <v>505.5098745056914</v>
+        <v>363.6248334168502</v>
       </c>
       <c r="S21" t="n">
-        <v>82.48109105045397</v>
+        <v>74.28052196933744</v>
       </c>
       <c r="T21" t="n">
-        <v>493.55836753848</v>
+        <v>492.06807</v>
       </c>
       <c r="U21" t="n">
-        <v>541.2476202070123</v>
+        <v>403.0171142505816</v>
       </c>
       <c r="V21" t="n">
-        <v>0.4769573943167686</v>
+        <v>0.5867097253270399</v>
       </c>
       <c r="W21" t="n">
-        <v>0.5230426056832315</v>
+        <v>0.41329027467296</v>
       </c>
       <c r="X21" t="n">
-        <v>1034.805987745492</v>
+        <v>975.142990164703</v>
       </c>
       <c r="Y21" t="n">
-        <v>0.8678786727272728</v>
+        <v>0.8510328545454545</v>
       </c>
       <c r="Z21" t="n">
-        <v>1</v>
+        <v>0.8325551916112502</v>
       </c>
       <c r="AA21" t="n">
         <v>47.40138386428681</v>
       </c>
       <c r="AB21" t="n">
-        <v>18.53039950704824</v>
+        <v>27.79559926057235</v>
       </c>
       <c r="AC21" t="n">
         <v>52.75687390981355</v>
       </c>
       <c r="AD21" t="n">
-        <v>18.53039950704824</v>
+        <v>27.79559926057235</v>
       </c>
     </row>
     <row r="22">
@@ -2430,91 +2430,91 @@
         <v>21</v>
       </c>
       <c r="B22" t="n">
-        <v>30082.84262899712</v>
+        <v>21332.91802126991</v>
       </c>
       <c r="C22" t="n">
-        <v>28996.02941561121</v>
+        <v>24629.36388646858</v>
       </c>
       <c r="D22" t="n">
         <v>140</v>
       </c>
       <c r="E22" t="n">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="F22" t="n">
-        <v>125.0978167259932</v>
+        <v>123.9208591281205</v>
       </c>
       <c r="G22" t="n">
-        <v>125.0978167259932</v>
+        <v>123.9208591281205</v>
       </c>
       <c r="H22" t="n">
-        <v>434.14796</v>
+        <v>549.35582</v>
       </c>
       <c r="I22" t="n">
-        <v>102.369928045262</v>
+        <v>242.1399304497677</v>
       </c>
       <c r="J22" t="n">
-        <v>481.2457502794067</v>
+        <v>468.8406416645093</v>
       </c>
       <c r="K22" t="n">
-        <v>164.6030467735823</v>
+        <v>0</v>
       </c>
       <c r="L22" t="n">
-        <v>283.040431885441</v>
+        <v>434.6193848871106</v>
       </c>
       <c r="M22" t="n">
-        <v>138.8824301513268</v>
+        <v>94.73643270662923</v>
       </c>
       <c r="N22" t="n">
-        <v>271.8795505222943</v>
+        <v>266.1707768292266</v>
       </c>
       <c r="O22" t="n">
-        <v>79.89848143244379</v>
+        <v>61.04511272100565</v>
       </c>
       <c r="P22" t="n">
-        <v>426.2689021699277</v>
+        <v>433.3435895500493</v>
       </c>
       <c r="Q22" t="n">
-        <v>94.5755096499847</v>
+        <v>106.1836164772967</v>
       </c>
       <c r="R22" t="n">
-        <v>389.1185933944503</v>
+        <v>395.5767056049464</v>
       </c>
       <c r="S22" t="n">
-        <v>96.32886519904451</v>
+        <v>108.1521771951689</v>
       </c>
       <c r="T22" t="n">
-        <v>351.778031954738</v>
+        <v>327.2158895502322</v>
       </c>
       <c r="U22" t="n">
-        <v>520.8444118199125</v>
+        <v>523.7288828001153</v>
       </c>
       <c r="V22" t="n">
-        <v>0.403127417205857</v>
+        <v>0.37752350289238</v>
       </c>
       <c r="W22" t="n">
-        <v>0.596872582794143</v>
+        <v>0.62247649710762</v>
       </c>
       <c r="X22" t="n">
-        <v>872.6224437746505</v>
+        <v>866.7430955775783</v>
       </c>
       <c r="Y22" t="n">
-        <v>0.7893599272727273</v>
+        <v>0.9988287636363636</v>
       </c>
       <c r="Z22" t="n">
-        <v>0.8749922732352849</v>
+        <v>0.852437530299108</v>
       </c>
       <c r="AA22" t="n">
         <v>43.67483838591729</v>
       </c>
       <c r="AB22" t="n">
-        <v>18.54892990655528</v>
+        <v>27.82339485983292</v>
       </c>
       <c r="AC22" t="n">
         <v>53.25626626305002</v>
       </c>
       <c r="AD22" t="n">
-        <v>18.54892990655528</v>
+        <v>27.82339485983292</v>
       </c>
     </row>
     <row r="23">
@@ -2522,91 +2522,91 @@
         <v>22</v>
       </c>
       <c r="B23" t="n">
-        <v>33426.4145969814</v>
+        <v>29433.45972064057</v>
       </c>
       <c r="C23" t="n">
-        <v>23513.1762451373</v>
+        <v>10217.96657160306</v>
       </c>
       <c r="D23" t="n">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="E23" t="n">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="F23" t="n">
-        <v>118.8429258896936</v>
+        <v>105.3327302589024</v>
       </c>
       <c r="G23" t="n">
-        <v>118.8429258896936</v>
+        <v>105.3327302589024</v>
       </c>
       <c r="H23" t="n">
-        <v>410.26508</v>
+        <v>496.43384</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
       </c>
       <c r="J23" t="n">
-        <v>550</v>
+        <v>527.3627552092553</v>
       </c>
       <c r="K23" t="n">
-        <v>179.4776579892297</v>
+        <v>15.98261840800808</v>
       </c>
       <c r="L23" t="n">
-        <v>392.6454994953268</v>
+        <v>624.8734586496588</v>
       </c>
       <c r="M23" t="n">
-        <v>95.98951298053957</v>
+        <v>89.70031390128581</v>
       </c>
       <c r="N23" t="n">
-        <v>380.7678063256957</v>
+        <v>451.3545939972465</v>
       </c>
       <c r="O23" t="n">
-        <v>75.39712789865129</v>
+        <v>77.98987846692552</v>
       </c>
       <c r="P23" t="n">
-        <v>395.8145297226576</v>
+        <v>366.677952220272</v>
       </c>
       <c r="Q23" t="n">
-        <v>139.310859061695</v>
+        <v>144.7021845809752</v>
       </c>
       <c r="R23" t="n">
-        <v>390.6921137335964</v>
+        <v>361.9326059425459</v>
       </c>
       <c r="S23" t="n">
-        <v>140.0117011811826</v>
+        <v>145.4301492667094</v>
       </c>
       <c r="T23" t="n">
-        <v>434.26508</v>
+        <v>520.4338399999999</v>
       </c>
       <c r="U23" t="n">
-        <v>535.1253887843526</v>
+        <v>511.3801368012472</v>
       </c>
       <c r="V23" t="n">
-        <v>0.4601728914691964</v>
+        <v>0.5086306864962119</v>
       </c>
       <c r="W23" t="n">
-        <v>0.5398271085308035</v>
+        <v>0.4913693135037882</v>
       </c>
       <c r="X23" t="n">
-        <v>991.2903230086996</v>
+        <v>1040.724609265419</v>
       </c>
       <c r="Y23" t="n">
-        <v>0.7459365090909091</v>
+        <v>0.9026069818181818</v>
       </c>
       <c r="Z23" t="n">
-        <v>1</v>
+        <v>0.9588413731077369</v>
       </c>
       <c r="AA23" t="n">
         <v>45.54468784674192</v>
       </c>
       <c r="AB23" t="n">
-        <v>18.56747883646184</v>
+        <v>27.85121825469275</v>
       </c>
       <c r="AC23" t="n">
         <v>53.65749454513181</v>
       </c>
       <c r="AD23" t="n">
-        <v>18.56747883646184</v>
+        <v>27.85121825469275</v>
       </c>
     </row>
     <row r="24">
@@ -2614,91 +2614,91 @@
         <v>23</v>
       </c>
       <c r="B24" t="n">
-        <v>32991.2900210027</v>
+        <v>30034.38935544476</v>
       </c>
       <c r="C24" t="n">
-        <v>20269.82165248213</v>
+        <v>20408.41702552897</v>
       </c>
       <c r="D24" t="n">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E24" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F24" t="n">
-        <v>124.7850721841782</v>
+        <v>121.1326397977378</v>
       </c>
       <c r="G24" t="n">
-        <v>124.7850721841782</v>
+        <v>121.1326397977378</v>
       </c>
       <c r="H24" t="n">
-        <v>482.82745</v>
+        <v>452.77701</v>
       </c>
       <c r="I24" t="n">
-        <v>42.90164925298171</v>
+        <v>80.84463769505288</v>
       </c>
       <c r="J24" t="n">
-        <v>513.7300108439707</v>
+        <v>550</v>
       </c>
       <c r="K24" t="n">
-        <v>229.8666476560813</v>
+        <v>32.92478737623514</v>
       </c>
       <c r="L24" t="n">
-        <v>387.7613888851649</v>
+        <v>336.1225347242867</v>
       </c>
       <c r="M24" t="n">
-        <v>76.06606165866009</v>
+        <v>97.65447048054887</v>
       </c>
       <c r="N24" t="n">
-        <v>397.2054314075017</v>
+        <v>313.5242912326802</v>
       </c>
       <c r="O24" t="n">
-        <v>61.72036933951656</v>
+        <v>77.40808107226694</v>
       </c>
       <c r="P24" t="n">
-        <v>339.7021356679776</v>
+        <v>415.8616340247169</v>
       </c>
       <c r="Q24" t="n">
-        <v>123.6388855091415</v>
+        <v>117.1961970070561</v>
       </c>
       <c r="R24" t="n">
-        <v>368.4603687353445</v>
+        <v>451.067317296452</v>
       </c>
       <c r="S24" t="n">
-        <v>124.7473000978558</v>
+        <v>118.2468533112562</v>
       </c>
       <c r="T24" t="n">
-        <v>458.9258007470183</v>
+        <v>390.9323723049471</v>
       </c>
       <c r="U24" t="n">
-        <v>463.3410211771191</v>
+        <v>533.0578310317729</v>
       </c>
       <c r="V24" t="n">
-        <v>0.497606321551886</v>
+        <v>0.4230914688199175</v>
       </c>
       <c r="W24" t="n">
-        <v>0.502393678448114</v>
+        <v>0.5769085311800826</v>
       </c>
       <c r="X24" t="n">
-        <v>922.2668219241374</v>
+        <v>923.99020333672</v>
       </c>
       <c r="Y24" t="n">
-        <v>0.8778680909090909</v>
+        <v>0.8232309272727273</v>
       </c>
       <c r="Z24" t="n">
-        <v>0.9340545651708558</v>
+        <v>1</v>
       </c>
       <c r="AA24" t="n">
         <v>45.55251108886526</v>
       </c>
       <c r="AB24" t="n">
-        <v>18.5860463152983</v>
+        <v>27.87906947294744</v>
       </c>
       <c r="AC24" t="n">
         <v>52.29626804969558</v>
       </c>
       <c r="AD24" t="n">
-        <v>18.5860463152983</v>
+        <v>27.87906947294744</v>
       </c>
     </row>
     <row r="25">
@@ -2706,10 +2706,10 @@
         <v>24</v>
       </c>
       <c r="B25" t="n">
-        <v>18034.53774142129</v>
+        <v>25834.02666314178</v>
       </c>
       <c r="C25" t="n">
-        <v>22998.23926493282</v>
+        <v>17095.48407329969</v>
       </c>
       <c r="D25" t="n">
         <v>140</v>
@@ -2718,79 +2718,79 @@
         <v>180</v>
       </c>
       <c r="F25" t="n">
-        <v>131.0243257933872</v>
+        <v>139.3025357673984</v>
       </c>
       <c r="G25" t="n">
-        <v>131.0243257933872</v>
+        <v>139.3025357673984</v>
       </c>
       <c r="H25" t="n">
-        <v>476.64844</v>
+        <v>410.78883</v>
       </c>
       <c r="I25" t="n">
-        <v>199.9286314819689</v>
+        <v>102.1454953685202</v>
       </c>
       <c r="J25" t="n">
-        <v>380.4755425611777</v>
+        <v>355.6192879928951</v>
       </c>
       <c r="K25" t="n">
-        <v>209.8611126626874</v>
+        <v>28.93269112231877</v>
       </c>
       <c r="L25" t="n">
-        <v>381.5510226097936</v>
+        <v>356.4248159206321</v>
       </c>
       <c r="M25" t="n">
-        <v>120.9990619622946</v>
+        <v>118.2086505345519</v>
       </c>
       <c r="N25" t="n">
-        <v>234.9464307139382</v>
+        <v>264.1567299111869</v>
       </c>
       <c r="O25" t="n">
-        <v>58.77337780409296</v>
+        <v>61.48660472029289</v>
       </c>
       <c r="P25" t="n">
-        <v>306.2183176923769</v>
+        <v>269.4869356062381</v>
       </c>
       <c r="Q25" t="n">
-        <v>94.26275986219467</v>
+        <v>90.12444864057335</v>
       </c>
       <c r="R25" t="n">
-        <v>312.7337932460518</v>
+        <v>275.2208693376</v>
       </c>
       <c r="S25" t="n">
-        <v>97.60839697120711</v>
+        <v>93.32320603153023</v>
       </c>
       <c r="T25" t="n">
-        <v>293.7198085180311</v>
+        <v>325.6433346314798</v>
       </c>
       <c r="U25" t="n">
-        <v>400.4810775545716</v>
+        <v>359.6113842468115</v>
       </c>
       <c r="V25" t="n">
-        <v>0.4231049173384555</v>
+        <v>0.4752150195543821</v>
       </c>
       <c r="W25" t="n">
-        <v>0.5768950826615444</v>
+        <v>0.5247849804456179</v>
       </c>
       <c r="X25" t="n">
-        <v>694.2008860726028</v>
+        <v>685.2547188782912</v>
       </c>
       <c r="Y25" t="n">
-        <v>0.8666335272727272</v>
+        <v>0.7468887818181819</v>
       </c>
       <c r="Z25" t="n">
-        <v>0.6917737137475959</v>
+        <v>0.6465805236234456</v>
       </c>
       <c r="AA25" t="n">
         <v>47.59562034471178</v>
       </c>
       <c r="AB25" t="n">
-        <v>18.60463236161359</v>
+        <v>27.90694854242038</v>
       </c>
       <c r="AC25" t="n">
         <v>49.47033852359848</v>
       </c>
       <c r="AD25" t="n">
-        <v>18.60463236161359</v>
+        <v>27.90694854242038</v>
       </c>
     </row>
     <row r="26">
@@ -2798,91 +2798,91 @@
         <v>25</v>
       </c>
       <c r="B26" t="n">
-        <v>33168.13248439984</v>
+        <v>44467.40510024398</v>
       </c>
       <c r="C26" t="n">
-        <v>36036.59972537778</v>
+        <v>31975.2450788545</v>
       </c>
       <c r="D26" t="n">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E26" t="n">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="F26" t="n">
-        <v>124.4731095037178</v>
+        <v>160.1979161325082</v>
       </c>
       <c r="G26" t="n">
-        <v>124.4731095037178</v>
+        <v>160.1979161325082</v>
       </c>
       <c r="H26" t="n">
-        <v>435.83647</v>
+        <v>459.33008</v>
       </c>
       <c r="I26" t="n">
         <v>0</v>
       </c>
       <c r="J26" t="n">
-        <v>550</v>
+        <v>445.1123066968156</v>
       </c>
       <c r="K26" t="n">
-        <v>164.7430665069646</v>
+        <v>39.28799887556079</v>
       </c>
       <c r="L26" t="n">
-        <v>558.9481592915332</v>
+        <v>401.3885665221691</v>
       </c>
       <c r="M26" t="n">
-        <v>52.8169461168221</v>
+        <v>136.0870117333069</v>
       </c>
       <c r="N26" t="n">
-        <v>527.2932170806928</v>
+        <v>564.9614632067484</v>
       </c>
       <c r="O26" t="n">
-        <v>69.45327227857096</v>
+        <v>105.1468092804694</v>
       </c>
       <c r="P26" t="n">
-        <v>455.4934210280269</v>
+        <v>329.8049845038497</v>
       </c>
       <c r="Q26" t="n">
-        <v>139.624625127696</v>
+        <v>104.9520144397239</v>
       </c>
       <c r="R26" t="n">
-        <v>482.2886925812294</v>
+        <v>349.2063934186814</v>
       </c>
       <c r="S26" t="n">
-        <v>139.473748231207</v>
+        <v>104.8386044004529</v>
       </c>
       <c r="T26" t="n">
-        <v>459.83647</v>
+        <v>483.33008</v>
       </c>
       <c r="U26" t="n">
-        <v>595.1180461557228</v>
+        <v>434.7569989435736</v>
       </c>
       <c r="V26" t="n">
-        <v>0.5006831494498816</v>
+        <v>0.6065067749115085</v>
       </c>
       <c r="W26" t="n">
-        <v>0.4993168505501184</v>
+        <v>0.3934932250884914</v>
       </c>
       <c r="X26" t="n">
-        <v>1191.864535514987</v>
+        <v>1104.865271430791</v>
       </c>
       <c r="Y26" t="n">
-        <v>0.7924299454545455</v>
+        <v>0.8351456</v>
       </c>
       <c r="Z26" t="n">
-        <v>1</v>
+        <v>0.8092951030851193</v>
       </c>
       <c r="AA26" t="n">
         <v>50.50574109963803</v>
       </c>
       <c r="AB26" t="n">
-        <v>18.6232369939752</v>
+        <v>27.9348554909628</v>
       </c>
       <c r="AC26" t="n">
         <v>49.94059549400324</v>
       </c>
       <c r="AD26" t="n">
-        <v>18.6232369939752</v>
+        <v>27.9348554909628</v>
       </c>
     </row>
     <row r="27">
@@ -2890,91 +2890,91 @@
         <v>26</v>
       </c>
       <c r="B27" t="n">
-        <v>12564.75751735416</v>
+        <v>15815.74470948091</v>
       </c>
       <c r="C27" t="n">
-        <v>15051.14444103105</v>
+        <v>10487.74370433363</v>
       </c>
       <c r="D27" t="n">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="E27" t="n">
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="F27" t="n">
-        <v>130.6967649789037</v>
+        <v>136.1682287126319</v>
       </c>
       <c r="G27" t="n">
-        <v>130.6967649789037</v>
+        <v>136.1682287126319</v>
       </c>
       <c r="H27" t="n">
-        <v>480.49937</v>
+        <v>503.18054</v>
       </c>
       <c r="I27" t="n">
-        <v>235.8557823769706</v>
+        <v>204.4252651938294</v>
       </c>
       <c r="J27" t="n">
-        <v>407.0102586646685</v>
+        <v>293.7810609439776</v>
       </c>
       <c r="K27" t="n">
-        <v>216.547424811198</v>
+        <v>32.96137991888116</v>
       </c>
       <c r="L27" t="n">
-        <v>365.8283168088877</v>
+        <v>432.0114426281202</v>
       </c>
       <c r="M27" t="n">
-        <v>90.6710483518204</v>
+        <v>47.16909417733114</v>
       </c>
       <c r="N27" t="n">
-        <v>226.3949031562336</v>
+        <v>288.6305986681901</v>
       </c>
       <c r="O27" t="n">
-        <v>42.24868446679579</v>
+        <v>34.12467613798056</v>
       </c>
       <c r="P27" t="n">
-        <v>298.0385151043652</v>
+        <v>239.7877788111751</v>
       </c>
       <c r="Q27" t="n">
-        <v>57.16738525606996</v>
+        <v>60.31990108948214</v>
       </c>
       <c r="R27" t="n">
-        <v>315.9902133811004</v>
+        <v>254.2308713563093</v>
       </c>
       <c r="S27" t="n">
-        <v>55.76311179053273</v>
+        <v>58.83818846322912</v>
       </c>
       <c r="T27" t="n">
-        <v>268.6435876230294</v>
+        <v>322.7552748061707</v>
       </c>
       <c r="U27" t="n">
-        <v>355.2059003604352</v>
+        <v>300.1076799006573</v>
       </c>
       <c r="V27" t="n">
-        <v>0.4306224382605408</v>
+        <v>0.5181802391154996</v>
       </c>
       <c r="W27" t="n">
-        <v>0.5693775617394593</v>
+        <v>0.4818197608845005</v>
       </c>
       <c r="X27" t="n">
-        <v>623.8494879834645</v>
+        <v>622.862954706828</v>
       </c>
       <c r="Y27" t="n">
-        <v>0.8736352181818182</v>
+        <v>0.9148737090909091</v>
       </c>
       <c r="Z27" t="n">
-        <v>0.7400186521175791</v>
+        <v>0.5341473835345049</v>
       </c>
       <c r="AA27" t="n">
         <v>51.14186348489077</v>
       </c>
       <c r="AB27" t="n">
-        <v>18.64186023096918</v>
+        <v>27.96279034645376</v>
       </c>
       <c r="AC27" t="n">
         <v>50.8267278783383</v>
       </c>
       <c r="AD27" t="n">
-        <v>18.64186023096918</v>
+        <v>27.96279034645376</v>
       </c>
     </row>
     <row r="28">
@@ -2982,10 +2982,10 @@
         <v>27</v>
       </c>
       <c r="B28" t="n">
-        <v>30854.03988450524</v>
+        <v>21443.53761642078</v>
       </c>
       <c r="C28" t="n">
-        <v>19718.94476899172</v>
+        <v>15015.22467977439</v>
       </c>
       <c r="D28" t="n">
         <v>120</v>
@@ -2994,79 +2994,79 @@
         <v>140</v>
       </c>
       <c r="F28" t="n">
-        <v>124.1619267299585</v>
+        <v>115.7429944057371</v>
       </c>
       <c r="G28" t="n">
-        <v>124.1619267299585</v>
+        <v>115.7429944057371</v>
       </c>
       <c r="H28" t="n">
-        <v>456.0611</v>
+        <v>522.76243</v>
       </c>
       <c r="I28" t="n">
-        <v>28.64038141309146</v>
+        <v>143.7878245345558</v>
       </c>
       <c r="J28" t="n">
-        <v>390.7808298349053</v>
+        <v>451.5319906250826</v>
       </c>
       <c r="K28" t="n">
-        <v>191.2490455843418</v>
+        <v>8.996939787866097</v>
       </c>
       <c r="L28" t="n">
-        <v>567.3802555401577</v>
+        <v>599.9558401437187</v>
       </c>
       <c r="M28" t="n">
-        <v>102.5366252806621</v>
+        <v>105.231852263155</v>
       </c>
       <c r="N28" t="n">
-        <v>375.6253884940829</v>
+        <v>330.7384507309579</v>
       </c>
       <c r="O28" t="n">
-        <v>73.79533009282561</v>
+        <v>70.23615473448631</v>
       </c>
       <c r="P28" t="n">
-        <v>327.7418391332535</v>
+        <v>382.1413166548259</v>
       </c>
       <c r="Q28" t="n">
-        <v>88.33736992850791</v>
+        <v>93.35511410127181</v>
       </c>
       <c r="R28" t="n">
-        <v>311.6672546789046</v>
+        <v>363.3986291654615</v>
       </c>
       <c r="S28" t="n">
-        <v>95.66099996719868</v>
+        <v>101.0947413785023</v>
       </c>
       <c r="T28" t="n">
-        <v>449.4207185869085</v>
+        <v>400.9746054654442</v>
       </c>
       <c r="U28" t="n">
-        <v>416.0792090617614</v>
+        <v>475.4964307560977</v>
       </c>
       <c r="V28" t="n">
-        <v>0.5192614167026721</v>
+        <v>0.4574875710600111</v>
       </c>
       <c r="W28" t="n">
-        <v>0.4807385832973279</v>
+        <v>0.5425124289399889</v>
       </c>
       <c r="X28" t="n">
-        <v>865.4999276486699</v>
+        <v>876.4710362215419</v>
       </c>
       <c r="Y28" t="n">
-        <v>0.829202</v>
+        <v>0.9504771454545454</v>
       </c>
       <c r="Z28" t="n">
-        <v>0.7105105996998278</v>
+        <v>0.8209672556819684</v>
       </c>
       <c r="AA28" t="n">
         <v>50.473863223804</v>
       </c>
       <c r="AB28" t="n">
-        <v>18.66050209120014</v>
+        <v>27.99075313680021</v>
       </c>
       <c r="AC28" t="n">
         <v>54.49724150507136</v>
       </c>
       <c r="AD28" t="n">
-        <v>18.66050209120014</v>
+        <v>27.99075313680021</v>
       </c>
     </row>
     <row r="29">
@@ -3074,10 +3074,10 @@
         <v>28</v>
       </c>
       <c r="B29" t="n">
-        <v>18767.29266851334</v>
+        <v>25523.32908013812</v>
       </c>
       <c r="C29" t="n">
-        <v>16692.32029561729</v>
+        <v>11754.82569784018</v>
       </c>
       <c r="D29" t="n">
         <v>130</v>
@@ -3086,79 +3086,79 @@
         <v>180</v>
       </c>
       <c r="F29" t="n">
-        <v>130.3700230664564</v>
+        <v>133.1044435665977</v>
       </c>
       <c r="G29" t="n">
-        <v>130.3700230664564</v>
+        <v>133.1044435665977</v>
       </c>
       <c r="H29" t="n">
-        <v>470.58435</v>
+        <v>297.98385</v>
       </c>
       <c r="I29" t="n">
-        <v>153.4830483967635</v>
+        <v>0</v>
       </c>
       <c r="J29" t="n">
-        <v>393.7666635084109</v>
+        <v>381.7643943536804</v>
       </c>
       <c r="K29" t="n">
-        <v>212.2090291695944</v>
+        <v>31.68637196234062</v>
       </c>
       <c r="L29" t="n">
-        <v>371.5078075706774</v>
+        <v>320.0776982946185</v>
       </c>
       <c r="M29" t="n">
-        <v>110.7169241034823</v>
+        <v>104.6939741821436</v>
       </c>
       <c r="N29" t="n">
-        <v>266.3380594960739</v>
+        <v>276.0719461024577</v>
       </c>
       <c r="O29" t="n">
-        <v>67.7632421071626</v>
+        <v>68.82747923928027</v>
       </c>
       <c r="P29" t="n">
-        <v>263.3271715356301</v>
+        <v>251.2044749610021</v>
       </c>
       <c r="Q29" t="n">
-        <v>109.4795083875283</v>
+        <v>107.8704872182038</v>
       </c>
       <c r="R29" t="n">
-        <v>274.2788341420712</v>
+        <v>261.6519598861528</v>
       </c>
       <c r="S29" t="n">
-        <v>110.7368749506816</v>
+        <v>109.1093742553936</v>
       </c>
       <c r="T29" t="n">
-        <v>334.1013016032365</v>
+        <v>314.98385</v>
       </c>
       <c r="U29" t="n">
-        <v>372.8066799231584</v>
+        <v>359.0749621792058</v>
       </c>
       <c r="V29" t="n">
-        <v>0.4726234677416238</v>
+        <v>0.4899317808369512</v>
       </c>
       <c r="W29" t="n">
-        <v>0.5273765322583762</v>
+        <v>0.5100682191630489</v>
       </c>
       <c r="X29" t="n">
-        <v>706.9079815263949</v>
+        <v>703.9743875209438</v>
       </c>
       <c r="Y29" t="n">
-        <v>0.855607909090909</v>
+        <v>0.5417888181818182</v>
       </c>
       <c r="Z29" t="n">
-        <v>0.7159393881971108</v>
+        <v>0.6941170806430552</v>
       </c>
       <c r="AA29" t="n">
         <v>51.76311206081095</v>
       </c>
       <c r="AB29" t="n">
-        <v>18.67916259329134</v>
+        <v>28.01874388993701</v>
       </c>
       <c r="AC29" t="n">
         <v>53.87083175514014</v>
       </c>
       <c r="AD29" t="n">
-        <v>18.67916259329134</v>
+        <v>28.01874388993701</v>
       </c>
     </row>
     <row r="30">
@@ -3166,91 +3166,91 @@
         <v>29</v>
       </c>
       <c r="B30" t="n">
-        <v>33256.35232249934</v>
+        <v>36870.84677375412</v>
       </c>
       <c r="C30" t="n">
-        <v>28406.11023557238</v>
+        <v>23096.24143578053</v>
       </c>
       <c r="D30" t="n">
         <v>140</v>
       </c>
       <c r="E30" t="n">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="F30" t="n">
-        <v>136.8885242197793</v>
+        <v>153.0701101015873</v>
       </c>
       <c r="G30" t="n">
-        <v>136.8885242197793</v>
+        <v>153.0701101015873</v>
       </c>
       <c r="H30" t="n">
-        <v>471.09996</v>
+        <v>527.94314</v>
       </c>
       <c r="I30" t="n">
-        <v>77.51442848071559</v>
+        <v>86.93573047456653</v>
       </c>
       <c r="J30" t="n">
-        <v>444.3267179201736</v>
+        <v>363.2679669612684</v>
       </c>
       <c r="K30" t="n">
-        <v>206.6215408726475</v>
+        <v>22.89773509879001</v>
       </c>
       <c r="L30" t="n">
-        <v>416.1425849952191</v>
+        <v>392.8544617706754</v>
       </c>
       <c r="M30" t="n">
-        <v>185.4404226772006</v>
+        <v>112.0886809978207</v>
       </c>
       <c r="N30" t="n">
-        <v>318.6102968538856</v>
+        <v>381.7129273629599</v>
       </c>
       <c r="O30" t="n">
-        <v>97.97523466539877</v>
+        <v>82.29448216247354</v>
       </c>
       <c r="P30" t="n">
-        <v>348.5797392474603</v>
+        <v>267.1715933392072</v>
       </c>
       <c r="Q30" t="n">
-        <v>101.3344669696601</v>
+        <v>104.8850104856118</v>
       </c>
       <c r="R30" t="n">
-        <v>363.3083364653543</v>
+        <v>278.4604387404099</v>
       </c>
       <c r="S30" t="n">
-        <v>93.22741062441374</v>
+        <v>96.49390018319913</v>
       </c>
       <c r="T30" t="n">
-        <v>416.5855315192844</v>
+        <v>464.0074095254334</v>
       </c>
       <c r="U30" t="n">
-        <v>449.9142062171205</v>
+        <v>372.056603824819</v>
       </c>
       <c r="V30" t="n">
-        <v>0.4807682142034445</v>
+        <v>0.5549902903559691</v>
       </c>
       <c r="W30" t="n">
-        <v>0.5192317857965555</v>
+        <v>0.4450097096440309</v>
       </c>
       <c r="X30" t="n">
-        <v>866.4997377364049</v>
+        <v>836.0640133502525</v>
       </c>
       <c r="Y30" t="n">
-        <v>0.8565453818181819</v>
+        <v>0.9598966181818182</v>
       </c>
       <c r="Z30" t="n">
-        <v>0.807866759854861</v>
+        <v>0.6604872126568517</v>
       </c>
       <c r="AA30" t="n">
         <v>52.87751082220224</v>
       </c>
       <c r="AB30" t="n">
-        <v>18.69784175588463</v>
+        <v>28.04676263382694</v>
       </c>
       <c r="AC30" t="n">
         <v>50.60448657413488</v>
       </c>
       <c r="AD30" t="n">
-        <v>18.69784175588463</v>
+        <v>28.04676263382694</v>
       </c>
     </row>
     <row r="31">
@@ -3258,91 +3258,91 @@
         <v>30</v>
       </c>
       <c r="B31" t="n">
-        <v>23664.91164303885</v>
+        <v>22298.95623048671</v>
       </c>
       <c r="C31" t="n">
-        <v>25996.27882436176</v>
+        <v>23674.83952938466</v>
       </c>
       <c r="D31" t="n">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="E31" t="n">
         <v>180</v>
       </c>
       <c r="F31" t="n">
-        <v>130.0440980087903</v>
+        <v>130.1095935863492</v>
       </c>
       <c r="G31" t="n">
-        <v>130.0440980087903</v>
+        <v>130.1095935863492</v>
       </c>
       <c r="H31" t="n">
-        <v>514.44807</v>
+        <v>474.31877</v>
       </c>
       <c r="I31" t="n">
-        <v>132.6025412245144</v>
+        <v>146.0826878761378</v>
       </c>
       <c r="J31" t="n">
-        <v>406.7979933350492</v>
+        <v>451.1032533248942</v>
       </c>
       <c r="K31" t="n">
-        <v>175.2481005151494</v>
+        <v>0</v>
       </c>
       <c r="L31" t="n">
-        <v>470.337521032725</v>
+        <v>449.4363470838739</v>
       </c>
       <c r="M31" t="n">
-        <v>104.6249787098826</v>
+        <v>94.81815360505615</v>
       </c>
       <c r="N31" t="n">
-        <v>334.843299569991</v>
+        <v>281.2094378983559</v>
       </c>
       <c r="O31" t="n">
-        <v>64.00222920549466</v>
+        <v>64.02664422550635</v>
       </c>
       <c r="P31" t="n">
-        <v>334.3893485224903</v>
+        <v>376.9188454576859</v>
       </c>
       <c r="Q31" t="n">
-        <v>103.782085170057</v>
+        <v>103.7453222005001</v>
       </c>
       <c r="R31" t="n">
-        <v>319.334849685491</v>
+        <v>359.9496317382357</v>
       </c>
       <c r="S31" t="n">
-        <v>94.08468452220573</v>
+        <v>94.05135668544854</v>
       </c>
       <c r="T31" t="n">
-        <v>398.8455287754856</v>
+        <v>345.2360821238622</v>
       </c>
       <c r="U31" t="n">
-        <v>438.1714336925473</v>
+        <v>474.0009884236842</v>
       </c>
       <c r="V31" t="n">
-        <v>0.4765082987081258</v>
+        <v>0.4180118388570153</v>
       </c>
       <c r="W31" t="n">
-        <v>0.5234917012918741</v>
+        <v>0.5819881611429848</v>
       </c>
       <c r="X31" t="n">
-        <v>837.0169624680329</v>
+        <v>825.9002497820481</v>
       </c>
       <c r="Y31" t="n">
-        <v>0.9353601272727273</v>
+        <v>0.8623977636363636</v>
       </c>
       <c r="Z31" t="n">
-        <v>0.7396327151546348</v>
+        <v>0.8201877333179896</v>
       </c>
       <c r="AA31" t="n">
         <v>54.27137089915654</v>
       </c>
       <c r="AB31" t="n">
-        <v>18.71653959764052</v>
+        <v>28.07480939646077</v>
       </c>
       <c r="AC31" t="n">
         <v>50.00205850798848</v>
       </c>
       <c r="AD31" t="n">
-        <v>18.71653959764052</v>
+        <v>28.07480939646077</v>
       </c>
     </row>
   </sheetData>

</xml_diff>